<commit_message>
Added 0201 and deprecated 9921
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$M$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$M$82</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="435">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1502,6 +1502,31 @@
   </si>
   <si>
     <t>Personal identifier</t>
+  </si>
+  <si>
+    <t>0201</t>
+  </si>
+  <si>
+    <t>Codice Univoco Unità Organizzativa iPA</t>
+  </si>
+  <si>
+    <t>Agenzia per l’Italia digitale</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>String of 6 alphanumeric characters</t>
+  </si>
+  <si>
+    <t>"Alphanumeric characters"</t>
+  </si>
+  <si>
+    <t>IT:CUUO</t>
+  </si>
+  <si>
+    <t>RegEx: [0-9a-zA-Z]{6}
+No checkdigit</t>
   </si>
 </sst>
 </file>
@@ -1923,31 +1948,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AML81"/>
+  <dimension ref="A1:AML82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.90625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="67.81640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="34.1796875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="23.7265625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="54.26953125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="29.08984375" style="1" customWidth="1"/>
-    <col min="14" max="1026" width="14.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="67.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="34.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="54.28515625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" style="1" customWidth="1"/>
+    <col min="14" max="1026" width="14.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1026" s="4" customFormat="1">
@@ -1991,7 +2016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1026" ht="87">
+    <row r="2" spans="1:1026" ht="105">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -2030,7 +2055,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1026" ht="43.5">
+    <row r="3" spans="1:1026" ht="45">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -2066,7 +2091,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:1026" ht="29">
+    <row r="4" spans="1:1026" ht="30">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -2102,7 +2127,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:1026" ht="116">
+    <row r="5" spans="1:1026" ht="135">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -2141,7 +2166,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:1026" ht="72.5">
+    <row r="6" spans="1:1026" ht="90">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -2180,7 +2205,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="7" spans="1:1026" ht="29">
+    <row r="7" spans="1:1026" ht="30">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -2219,7 +2244,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="8" spans="1:1026" ht="145">
+    <row r="8" spans="1:1026" ht="180">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2252,7 +2277,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="1:1026" ht="174">
+    <row r="9" spans="1:1026" ht="180">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -2288,7 +2313,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:1026" ht="159.5">
+    <row r="10" spans="1:1026" ht="195">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -2324,7 +2349,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="11" spans="1:1026" s="14" customFormat="1" ht="43.5">
+    <row r="11" spans="1:1026" s="14" customFormat="1" ht="45">
       <c r="A11" s="11" t="s">
         <v>62</v>
       </c>
@@ -3373,7 +3398,7 @@
       <c r="AMK11" s="11"/>
       <c r="AML11" s="11"/>
     </row>
-    <row r="12" spans="1:1026" s="14" customFormat="1" ht="29">
+    <row r="12" spans="1:1026" s="14" customFormat="1" ht="30">
       <c r="A12" s="11" t="s">
         <v>68</v>
       </c>
@@ -5471,7 +5496,7 @@
       <c r="AMK13" s="11"/>
       <c r="AML13" s="11"/>
     </row>
-    <row r="14" spans="1:1026" ht="232">
+    <row r="14" spans="1:1026" ht="165">
       <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
@@ -5510,7 +5535,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="15" spans="1:1026" ht="145">
+    <row r="15" spans="1:1026" ht="150">
       <c r="A15" s="1" t="s">
         <v>345</v>
       </c>
@@ -6595,7 +6620,7 @@
       <c r="AMK16" s="11"/>
       <c r="AML16" s="11"/>
     </row>
-    <row r="17" spans="1:1026" ht="116">
+    <row r="17" spans="1:1026" ht="135">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -6634,7 +6659,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="18" spans="1:1026" ht="159.5">
+    <row r="18" spans="1:1026" ht="165">
       <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
@@ -6673,7 +6698,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="19" spans="1:1026" ht="58">
+    <row r="19" spans="1:1026" ht="60">
       <c r="A19" s="1" t="s">
         <v>98</v>
       </c>
@@ -6709,7 +6734,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="20" spans="1:1026" s="14" customFormat="1" ht="43.5">
+    <row r="20" spans="1:1026" s="14" customFormat="1" ht="45">
       <c r="A20" s="11" t="s">
         <v>104</v>
       </c>
@@ -7758,7 +7783,7 @@
       <c r="AMK20" s="11"/>
       <c r="AML20" s="11"/>
     </row>
-    <row r="21" spans="1:1026" ht="72.5">
+    <row r="21" spans="1:1026" ht="75">
       <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
@@ -7794,7 +7819,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="22" spans="1:1026" ht="87">
+    <row r="22" spans="1:1026" ht="90">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -7827,7 +7852,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="1:1026" ht="29">
+    <row r="23" spans="1:1026" ht="30">
       <c r="A23" s="1" t="s">
         <v>351</v>
       </c>
@@ -7893,7 +7918,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:1026" ht="72.5">
+    <row r="25" spans="1:1026" ht="75">
       <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
@@ -7912,1114 +7937,1124 @@
       <c r="F25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="2" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1026" ht="30">
+      <c r="A26" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G26" s="2" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" s="10"/>
+      <c r="L26" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1026" s="14" customFormat="1" ht="30">
+      <c r="A27" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="12">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J25" s="3" t="s">
+      <c r="H27" s="11"/>
+      <c r="I27" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J27" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>425</v>
-      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="11"/>
+      <c r="AC27" s="11"/>
+      <c r="AD27" s="11"/>
+      <c r="AE27" s="11"/>
+      <c r="AF27" s="11"/>
+      <c r="AG27" s="11"/>
+      <c r="AH27" s="11"/>
+      <c r="AI27" s="11"/>
+      <c r="AJ27" s="11"/>
+      <c r="AK27" s="11"/>
+      <c r="AL27" s="11"/>
+      <c r="AM27" s="11"/>
+      <c r="AN27" s="11"/>
+      <c r="AO27" s="11"/>
+      <c r="AP27" s="11"/>
+      <c r="AQ27" s="11"/>
+      <c r="AR27" s="11"/>
+      <c r="AS27" s="11"/>
+      <c r="AT27" s="11"/>
+      <c r="AU27" s="11"/>
+      <c r="AV27" s="11"/>
+      <c r="AW27" s="11"/>
+      <c r="AX27" s="11"/>
+      <c r="AY27" s="11"/>
+      <c r="AZ27" s="11"/>
+      <c r="BA27" s="11"/>
+      <c r="BB27" s="11"/>
+      <c r="BC27" s="11"/>
+      <c r="BD27" s="11"/>
+      <c r="BE27" s="11"/>
+      <c r="BF27" s="11"/>
+      <c r="BG27" s="11"/>
+      <c r="BH27" s="11"/>
+      <c r="BI27" s="11"/>
+      <c r="BJ27" s="11"/>
+      <c r="BK27" s="11"/>
+      <c r="BL27" s="11"/>
+      <c r="BM27" s="11"/>
+      <c r="BN27" s="11"/>
+      <c r="BO27" s="11"/>
+      <c r="BP27" s="11"/>
+      <c r="BQ27" s="11"/>
+      <c r="BR27" s="11"/>
+      <c r="BS27" s="11"/>
+      <c r="BT27" s="11"/>
+      <c r="BU27" s="11"/>
+      <c r="BV27" s="11"/>
+      <c r="BW27" s="11"/>
+      <c r="BX27" s="11"/>
+      <c r="BY27" s="11"/>
+      <c r="BZ27" s="11"/>
+      <c r="CA27" s="11"/>
+      <c r="CB27" s="11"/>
+      <c r="CC27" s="11"/>
+      <c r="CD27" s="11"/>
+      <c r="CE27" s="11"/>
+      <c r="CF27" s="11"/>
+      <c r="CG27" s="11"/>
+      <c r="CH27" s="11"/>
+      <c r="CI27" s="11"/>
+      <c r="CJ27" s="11"/>
+      <c r="CK27" s="11"/>
+      <c r="CL27" s="11"/>
+      <c r="CM27" s="11"/>
+      <c r="CN27" s="11"/>
+      <c r="CO27" s="11"/>
+      <c r="CP27" s="11"/>
+      <c r="CQ27" s="11"/>
+      <c r="CR27" s="11"/>
+      <c r="CS27" s="11"/>
+      <c r="CT27" s="11"/>
+      <c r="CU27" s="11"/>
+      <c r="CV27" s="11"/>
+      <c r="CW27" s="11"/>
+      <c r="CX27" s="11"/>
+      <c r="CY27" s="11"/>
+      <c r="CZ27" s="11"/>
+      <c r="DA27" s="11"/>
+      <c r="DB27" s="11"/>
+      <c r="DC27" s="11"/>
+      <c r="DD27" s="11"/>
+      <c r="DE27" s="11"/>
+      <c r="DF27" s="11"/>
+      <c r="DG27" s="11"/>
+      <c r="DH27" s="11"/>
+      <c r="DI27" s="11"/>
+      <c r="DJ27" s="11"/>
+      <c r="DK27" s="11"/>
+      <c r="DL27" s="11"/>
+      <c r="DM27" s="11"/>
+      <c r="DN27" s="11"/>
+      <c r="DO27" s="11"/>
+      <c r="DP27" s="11"/>
+      <c r="DQ27" s="11"/>
+      <c r="DR27" s="11"/>
+      <c r="DS27" s="11"/>
+      <c r="DT27" s="11"/>
+      <c r="DU27" s="11"/>
+      <c r="DV27" s="11"/>
+      <c r="DW27" s="11"/>
+      <c r="DX27" s="11"/>
+      <c r="DY27" s="11"/>
+      <c r="DZ27" s="11"/>
+      <c r="EA27" s="11"/>
+      <c r="EB27" s="11"/>
+      <c r="EC27" s="11"/>
+      <c r="ED27" s="11"/>
+      <c r="EE27" s="11"/>
+      <c r="EF27" s="11"/>
+      <c r="EG27" s="11"/>
+      <c r="EH27" s="11"/>
+      <c r="EI27" s="11"/>
+      <c r="EJ27" s="11"/>
+      <c r="EK27" s="11"/>
+      <c r="EL27" s="11"/>
+      <c r="EM27" s="11"/>
+      <c r="EN27" s="11"/>
+      <c r="EO27" s="11"/>
+      <c r="EP27" s="11"/>
+      <c r="EQ27" s="11"/>
+      <c r="ER27" s="11"/>
+      <c r="ES27" s="11"/>
+      <c r="ET27" s="11"/>
+      <c r="EU27" s="11"/>
+      <c r="EV27" s="11"/>
+      <c r="EW27" s="11"/>
+      <c r="EX27" s="11"/>
+      <c r="EY27" s="11"/>
+      <c r="EZ27" s="11"/>
+      <c r="FA27" s="11"/>
+      <c r="FB27" s="11"/>
+      <c r="FC27" s="11"/>
+      <c r="FD27" s="11"/>
+      <c r="FE27" s="11"/>
+      <c r="FF27" s="11"/>
+      <c r="FG27" s="11"/>
+      <c r="FH27" s="11"/>
+      <c r="FI27" s="11"/>
+      <c r="FJ27" s="11"/>
+      <c r="FK27" s="11"/>
+      <c r="FL27" s="11"/>
+      <c r="FM27" s="11"/>
+      <c r="FN27" s="11"/>
+      <c r="FO27" s="11"/>
+      <c r="FP27" s="11"/>
+      <c r="FQ27" s="11"/>
+      <c r="FR27" s="11"/>
+      <c r="FS27" s="11"/>
+      <c r="FT27" s="11"/>
+      <c r="FU27" s="11"/>
+      <c r="FV27" s="11"/>
+      <c r="FW27" s="11"/>
+      <c r="FX27" s="11"/>
+      <c r="FY27" s="11"/>
+      <c r="FZ27" s="11"/>
+      <c r="GA27" s="11"/>
+      <c r="GB27" s="11"/>
+      <c r="GC27" s="11"/>
+      <c r="GD27" s="11"/>
+      <c r="GE27" s="11"/>
+      <c r="GF27" s="11"/>
+      <c r="GG27" s="11"/>
+      <c r="GH27" s="11"/>
+      <c r="GI27" s="11"/>
+      <c r="GJ27" s="11"/>
+      <c r="GK27" s="11"/>
+      <c r="GL27" s="11"/>
+      <c r="GM27" s="11"/>
+      <c r="GN27" s="11"/>
+      <c r="GO27" s="11"/>
+      <c r="GP27" s="11"/>
+      <c r="GQ27" s="11"/>
+      <c r="GR27" s="11"/>
+      <c r="GS27" s="11"/>
+      <c r="GT27" s="11"/>
+      <c r="GU27" s="11"/>
+      <c r="GV27" s="11"/>
+      <c r="GW27" s="11"/>
+      <c r="GX27" s="11"/>
+      <c r="GY27" s="11"/>
+      <c r="GZ27" s="11"/>
+      <c r="HA27" s="11"/>
+      <c r="HB27" s="11"/>
+      <c r="HC27" s="11"/>
+      <c r="HD27" s="11"/>
+      <c r="HE27" s="11"/>
+      <c r="HF27" s="11"/>
+      <c r="HG27" s="11"/>
+      <c r="HH27" s="11"/>
+      <c r="HI27" s="11"/>
+      <c r="HJ27" s="11"/>
+      <c r="HK27" s="11"/>
+      <c r="HL27" s="11"/>
+      <c r="HM27" s="11"/>
+      <c r="HN27" s="11"/>
+      <c r="HO27" s="11"/>
+      <c r="HP27" s="11"/>
+      <c r="HQ27" s="11"/>
+      <c r="HR27" s="11"/>
+      <c r="HS27" s="11"/>
+      <c r="HT27" s="11"/>
+      <c r="HU27" s="11"/>
+      <c r="HV27" s="11"/>
+      <c r="HW27" s="11"/>
+      <c r="HX27" s="11"/>
+      <c r="HY27" s="11"/>
+      <c r="HZ27" s="11"/>
+      <c r="IA27" s="11"/>
+      <c r="IB27" s="11"/>
+      <c r="IC27" s="11"/>
+      <c r="ID27" s="11"/>
+      <c r="IE27" s="11"/>
+      <c r="IF27" s="11"/>
+      <c r="IG27" s="11"/>
+      <c r="IH27" s="11"/>
+      <c r="II27" s="11"/>
+      <c r="IJ27" s="11"/>
+      <c r="IK27" s="11"/>
+      <c r="IL27" s="11"/>
+      <c r="IM27" s="11"/>
+      <c r="IN27" s="11"/>
+      <c r="IO27" s="11"/>
+      <c r="IP27" s="11"/>
+      <c r="IQ27" s="11"/>
+      <c r="IR27" s="11"/>
+      <c r="IS27" s="11"/>
+      <c r="IT27" s="11"/>
+      <c r="IU27" s="11"/>
+      <c r="IV27" s="11"/>
+      <c r="IW27" s="11"/>
+      <c r="IX27" s="11"/>
+      <c r="IY27" s="11"/>
+      <c r="IZ27" s="11"/>
+      <c r="JA27" s="11"/>
+      <c r="JB27" s="11"/>
+      <c r="JC27" s="11"/>
+      <c r="JD27" s="11"/>
+      <c r="JE27" s="11"/>
+      <c r="JF27" s="11"/>
+      <c r="JG27" s="11"/>
+      <c r="JH27" s="11"/>
+      <c r="JI27" s="11"/>
+      <c r="JJ27" s="11"/>
+      <c r="JK27" s="11"/>
+      <c r="JL27" s="11"/>
+      <c r="JM27" s="11"/>
+      <c r="JN27" s="11"/>
+      <c r="JO27" s="11"/>
+      <c r="JP27" s="11"/>
+      <c r="JQ27" s="11"/>
+      <c r="JR27" s="11"/>
+      <c r="JS27" s="11"/>
+      <c r="JT27" s="11"/>
+      <c r="JU27" s="11"/>
+      <c r="JV27" s="11"/>
+      <c r="JW27" s="11"/>
+      <c r="JX27" s="11"/>
+      <c r="JY27" s="11"/>
+      <c r="JZ27" s="11"/>
+      <c r="KA27" s="11"/>
+      <c r="KB27" s="11"/>
+      <c r="KC27" s="11"/>
+      <c r="KD27" s="11"/>
+      <c r="KE27" s="11"/>
+      <c r="KF27" s="11"/>
+      <c r="KG27" s="11"/>
+      <c r="KH27" s="11"/>
+      <c r="KI27" s="11"/>
+      <c r="KJ27" s="11"/>
+      <c r="KK27" s="11"/>
+      <c r="KL27" s="11"/>
+      <c r="KM27" s="11"/>
+      <c r="KN27" s="11"/>
+      <c r="KO27" s="11"/>
+      <c r="KP27" s="11"/>
+      <c r="KQ27" s="11"/>
+      <c r="KR27" s="11"/>
+      <c r="KS27" s="11"/>
+      <c r="KT27" s="11"/>
+      <c r="KU27" s="11"/>
+      <c r="KV27" s="11"/>
+      <c r="KW27" s="11"/>
+      <c r="KX27" s="11"/>
+      <c r="KY27" s="11"/>
+      <c r="KZ27" s="11"/>
+      <c r="LA27" s="11"/>
+      <c r="LB27" s="11"/>
+      <c r="LC27" s="11"/>
+      <c r="LD27" s="11"/>
+      <c r="LE27" s="11"/>
+      <c r="LF27" s="11"/>
+      <c r="LG27" s="11"/>
+      <c r="LH27" s="11"/>
+      <c r="LI27" s="11"/>
+      <c r="LJ27" s="11"/>
+      <c r="LK27" s="11"/>
+      <c r="LL27" s="11"/>
+      <c r="LM27" s="11"/>
+      <c r="LN27" s="11"/>
+      <c r="LO27" s="11"/>
+      <c r="LP27" s="11"/>
+      <c r="LQ27" s="11"/>
+      <c r="LR27" s="11"/>
+      <c r="LS27" s="11"/>
+      <c r="LT27" s="11"/>
+      <c r="LU27" s="11"/>
+      <c r="LV27" s="11"/>
+      <c r="LW27" s="11"/>
+      <c r="LX27" s="11"/>
+      <c r="LY27" s="11"/>
+      <c r="LZ27" s="11"/>
+      <c r="MA27" s="11"/>
+      <c r="MB27" s="11"/>
+      <c r="MC27" s="11"/>
+      <c r="MD27" s="11"/>
+      <c r="ME27" s="11"/>
+      <c r="MF27" s="11"/>
+      <c r="MG27" s="11"/>
+      <c r="MH27" s="11"/>
+      <c r="MI27" s="11"/>
+      <c r="MJ27" s="11"/>
+      <c r="MK27" s="11"/>
+      <c r="ML27" s="11"/>
+      <c r="MM27" s="11"/>
+      <c r="MN27" s="11"/>
+      <c r="MO27" s="11"/>
+      <c r="MP27" s="11"/>
+      <c r="MQ27" s="11"/>
+      <c r="MR27" s="11"/>
+      <c r="MS27" s="11"/>
+      <c r="MT27" s="11"/>
+      <c r="MU27" s="11"/>
+      <c r="MV27" s="11"/>
+      <c r="MW27" s="11"/>
+      <c r="MX27" s="11"/>
+      <c r="MY27" s="11"/>
+      <c r="MZ27" s="11"/>
+      <c r="NA27" s="11"/>
+      <c r="NB27" s="11"/>
+      <c r="NC27" s="11"/>
+      <c r="ND27" s="11"/>
+      <c r="NE27" s="11"/>
+      <c r="NF27" s="11"/>
+      <c r="NG27" s="11"/>
+      <c r="NH27" s="11"/>
+      <c r="NI27" s="11"/>
+      <c r="NJ27" s="11"/>
+      <c r="NK27" s="11"/>
+      <c r="NL27" s="11"/>
+      <c r="NM27" s="11"/>
+      <c r="NN27" s="11"/>
+      <c r="NO27" s="11"/>
+      <c r="NP27" s="11"/>
+      <c r="NQ27" s="11"/>
+      <c r="NR27" s="11"/>
+      <c r="NS27" s="11"/>
+      <c r="NT27" s="11"/>
+      <c r="NU27" s="11"/>
+      <c r="NV27" s="11"/>
+      <c r="NW27" s="11"/>
+      <c r="NX27" s="11"/>
+      <c r="NY27" s="11"/>
+      <c r="NZ27" s="11"/>
+      <c r="OA27" s="11"/>
+      <c r="OB27" s="11"/>
+      <c r="OC27" s="11"/>
+      <c r="OD27" s="11"/>
+      <c r="OE27" s="11"/>
+      <c r="OF27" s="11"/>
+      <c r="OG27" s="11"/>
+      <c r="OH27" s="11"/>
+      <c r="OI27" s="11"/>
+      <c r="OJ27" s="11"/>
+      <c r="OK27" s="11"/>
+      <c r="OL27" s="11"/>
+      <c r="OM27" s="11"/>
+      <c r="ON27" s="11"/>
+      <c r="OO27" s="11"/>
+      <c r="OP27" s="11"/>
+      <c r="OQ27" s="11"/>
+      <c r="OR27" s="11"/>
+      <c r="OS27" s="11"/>
+      <c r="OT27" s="11"/>
+      <c r="OU27" s="11"/>
+      <c r="OV27" s="11"/>
+      <c r="OW27" s="11"/>
+      <c r="OX27" s="11"/>
+      <c r="OY27" s="11"/>
+      <c r="OZ27" s="11"/>
+      <c r="PA27" s="11"/>
+      <c r="PB27" s="11"/>
+      <c r="PC27" s="11"/>
+      <c r="PD27" s="11"/>
+      <c r="PE27" s="11"/>
+      <c r="PF27" s="11"/>
+      <c r="PG27" s="11"/>
+      <c r="PH27" s="11"/>
+      <c r="PI27" s="11"/>
+      <c r="PJ27" s="11"/>
+      <c r="PK27" s="11"/>
+      <c r="PL27" s="11"/>
+      <c r="PM27" s="11"/>
+      <c r="PN27" s="11"/>
+      <c r="PO27" s="11"/>
+      <c r="PP27" s="11"/>
+      <c r="PQ27" s="11"/>
+      <c r="PR27" s="11"/>
+      <c r="PS27" s="11"/>
+      <c r="PT27" s="11"/>
+      <c r="PU27" s="11"/>
+      <c r="PV27" s="11"/>
+      <c r="PW27" s="11"/>
+      <c r="PX27" s="11"/>
+      <c r="PY27" s="11"/>
+      <c r="PZ27" s="11"/>
+      <c r="QA27" s="11"/>
+      <c r="QB27" s="11"/>
+      <c r="QC27" s="11"/>
+      <c r="QD27" s="11"/>
+      <c r="QE27" s="11"/>
+      <c r="QF27" s="11"/>
+      <c r="QG27" s="11"/>
+      <c r="QH27" s="11"/>
+      <c r="QI27" s="11"/>
+      <c r="QJ27" s="11"/>
+      <c r="QK27" s="11"/>
+      <c r="QL27" s="11"/>
+      <c r="QM27" s="11"/>
+      <c r="QN27" s="11"/>
+      <c r="QO27" s="11"/>
+      <c r="QP27" s="11"/>
+      <c r="QQ27" s="11"/>
+      <c r="QR27" s="11"/>
+      <c r="QS27" s="11"/>
+      <c r="QT27" s="11"/>
+      <c r="QU27" s="11"/>
+      <c r="QV27" s="11"/>
+      <c r="QW27" s="11"/>
+      <c r="QX27" s="11"/>
+      <c r="QY27" s="11"/>
+      <c r="QZ27" s="11"/>
+      <c r="RA27" s="11"/>
+      <c r="RB27" s="11"/>
+      <c r="RC27" s="11"/>
+      <c r="RD27" s="11"/>
+      <c r="RE27" s="11"/>
+      <c r="RF27" s="11"/>
+      <c r="RG27" s="11"/>
+      <c r="RH27" s="11"/>
+      <c r="RI27" s="11"/>
+      <c r="RJ27" s="11"/>
+      <c r="RK27" s="11"/>
+      <c r="RL27" s="11"/>
+      <c r="RM27" s="11"/>
+      <c r="RN27" s="11"/>
+      <c r="RO27" s="11"/>
+      <c r="RP27" s="11"/>
+      <c r="RQ27" s="11"/>
+      <c r="RR27" s="11"/>
+      <c r="RS27" s="11"/>
+      <c r="RT27" s="11"/>
+      <c r="RU27" s="11"/>
+      <c r="RV27" s="11"/>
+      <c r="RW27" s="11"/>
+      <c r="RX27" s="11"/>
+      <c r="RY27" s="11"/>
+      <c r="RZ27" s="11"/>
+      <c r="SA27" s="11"/>
+      <c r="SB27" s="11"/>
+      <c r="SC27" s="11"/>
+      <c r="SD27" s="11"/>
+      <c r="SE27" s="11"/>
+      <c r="SF27" s="11"/>
+      <c r="SG27" s="11"/>
+      <c r="SH27" s="11"/>
+      <c r="SI27" s="11"/>
+      <c r="SJ27" s="11"/>
+      <c r="SK27" s="11"/>
+      <c r="SL27" s="11"/>
+      <c r="SM27" s="11"/>
+      <c r="SN27" s="11"/>
+      <c r="SO27" s="11"/>
+      <c r="SP27" s="11"/>
+      <c r="SQ27" s="11"/>
+      <c r="SR27" s="11"/>
+      <c r="SS27" s="11"/>
+      <c r="ST27" s="11"/>
+      <c r="SU27" s="11"/>
+      <c r="SV27" s="11"/>
+      <c r="SW27" s="11"/>
+      <c r="SX27" s="11"/>
+      <c r="SY27" s="11"/>
+      <c r="SZ27" s="11"/>
+      <c r="TA27" s="11"/>
+      <c r="TB27" s="11"/>
+      <c r="TC27" s="11"/>
+      <c r="TD27" s="11"/>
+      <c r="TE27" s="11"/>
+      <c r="TF27" s="11"/>
+      <c r="TG27" s="11"/>
+      <c r="TH27" s="11"/>
+      <c r="TI27" s="11"/>
+      <c r="TJ27" s="11"/>
+      <c r="TK27" s="11"/>
+      <c r="TL27" s="11"/>
+      <c r="TM27" s="11"/>
+      <c r="TN27" s="11"/>
+      <c r="TO27" s="11"/>
+      <c r="TP27" s="11"/>
+      <c r="TQ27" s="11"/>
+      <c r="TR27" s="11"/>
+      <c r="TS27" s="11"/>
+      <c r="TT27" s="11"/>
+      <c r="TU27" s="11"/>
+      <c r="TV27" s="11"/>
+      <c r="TW27" s="11"/>
+      <c r="TX27" s="11"/>
+      <c r="TY27" s="11"/>
+      <c r="TZ27" s="11"/>
+      <c r="UA27" s="11"/>
+      <c r="UB27" s="11"/>
+      <c r="UC27" s="11"/>
+      <c r="UD27" s="11"/>
+      <c r="UE27" s="11"/>
+      <c r="UF27" s="11"/>
+      <c r="UG27" s="11"/>
+      <c r="UH27" s="11"/>
+      <c r="UI27" s="11"/>
+      <c r="UJ27" s="11"/>
+      <c r="UK27" s="11"/>
+      <c r="UL27" s="11"/>
+      <c r="UM27" s="11"/>
+      <c r="UN27" s="11"/>
+      <c r="UO27" s="11"/>
+      <c r="UP27" s="11"/>
+      <c r="UQ27" s="11"/>
+      <c r="UR27" s="11"/>
+      <c r="US27" s="11"/>
+      <c r="UT27" s="11"/>
+      <c r="UU27" s="11"/>
+      <c r="UV27" s="11"/>
+      <c r="UW27" s="11"/>
+      <c r="UX27" s="11"/>
+      <c r="UY27" s="11"/>
+      <c r="UZ27" s="11"/>
+      <c r="VA27" s="11"/>
+      <c r="VB27" s="11"/>
+      <c r="VC27" s="11"/>
+      <c r="VD27" s="11"/>
+      <c r="VE27" s="11"/>
+      <c r="VF27" s="11"/>
+      <c r="VG27" s="11"/>
+      <c r="VH27" s="11"/>
+      <c r="VI27" s="11"/>
+      <c r="VJ27" s="11"/>
+      <c r="VK27" s="11"/>
+      <c r="VL27" s="11"/>
+      <c r="VM27" s="11"/>
+      <c r="VN27" s="11"/>
+      <c r="VO27" s="11"/>
+      <c r="VP27" s="11"/>
+      <c r="VQ27" s="11"/>
+      <c r="VR27" s="11"/>
+      <c r="VS27" s="11"/>
+      <c r="VT27" s="11"/>
+      <c r="VU27" s="11"/>
+      <c r="VV27" s="11"/>
+      <c r="VW27" s="11"/>
+      <c r="VX27" s="11"/>
+      <c r="VY27" s="11"/>
+      <c r="VZ27" s="11"/>
+      <c r="WA27" s="11"/>
+      <c r="WB27" s="11"/>
+      <c r="WC27" s="11"/>
+      <c r="WD27" s="11"/>
+      <c r="WE27" s="11"/>
+      <c r="WF27" s="11"/>
+      <c r="WG27" s="11"/>
+      <c r="WH27" s="11"/>
+      <c r="WI27" s="11"/>
+      <c r="WJ27" s="11"/>
+      <c r="WK27" s="11"/>
+      <c r="WL27" s="11"/>
+      <c r="WM27" s="11"/>
+      <c r="WN27" s="11"/>
+      <c r="WO27" s="11"/>
+      <c r="WP27" s="11"/>
+      <c r="WQ27" s="11"/>
+      <c r="WR27" s="11"/>
+      <c r="WS27" s="11"/>
+      <c r="WT27" s="11"/>
+      <c r="WU27" s="11"/>
+      <c r="WV27" s="11"/>
+      <c r="WW27" s="11"/>
+      <c r="WX27" s="11"/>
+      <c r="WY27" s="11"/>
+      <c r="WZ27" s="11"/>
+      <c r="XA27" s="11"/>
+      <c r="XB27" s="11"/>
+      <c r="XC27" s="11"/>
+      <c r="XD27" s="11"/>
+      <c r="XE27" s="11"/>
+      <c r="XF27" s="11"/>
+      <c r="XG27" s="11"/>
+      <c r="XH27" s="11"/>
+      <c r="XI27" s="11"/>
+      <c r="XJ27" s="11"/>
+      <c r="XK27" s="11"/>
+      <c r="XL27" s="11"/>
+      <c r="XM27" s="11"/>
+      <c r="XN27" s="11"/>
+      <c r="XO27" s="11"/>
+      <c r="XP27" s="11"/>
+      <c r="XQ27" s="11"/>
+      <c r="XR27" s="11"/>
+      <c r="XS27" s="11"/>
+      <c r="XT27" s="11"/>
+      <c r="XU27" s="11"/>
+      <c r="XV27" s="11"/>
+      <c r="XW27" s="11"/>
+      <c r="XX27" s="11"/>
+      <c r="XY27" s="11"/>
+      <c r="XZ27" s="11"/>
+      <c r="YA27" s="11"/>
+      <c r="YB27" s="11"/>
+      <c r="YC27" s="11"/>
+      <c r="YD27" s="11"/>
+      <c r="YE27" s="11"/>
+      <c r="YF27" s="11"/>
+      <c r="YG27" s="11"/>
+      <c r="YH27" s="11"/>
+      <c r="YI27" s="11"/>
+      <c r="YJ27" s="11"/>
+      <c r="YK27" s="11"/>
+      <c r="YL27" s="11"/>
+      <c r="YM27" s="11"/>
+      <c r="YN27" s="11"/>
+      <c r="YO27" s="11"/>
+      <c r="YP27" s="11"/>
+      <c r="YQ27" s="11"/>
+      <c r="YR27" s="11"/>
+      <c r="YS27" s="11"/>
+      <c r="YT27" s="11"/>
+      <c r="YU27" s="11"/>
+      <c r="YV27" s="11"/>
+      <c r="YW27" s="11"/>
+      <c r="YX27" s="11"/>
+      <c r="YY27" s="11"/>
+      <c r="YZ27" s="11"/>
+      <c r="ZA27" s="11"/>
+      <c r="ZB27" s="11"/>
+      <c r="ZC27" s="11"/>
+      <c r="ZD27" s="11"/>
+      <c r="ZE27" s="11"/>
+      <c r="ZF27" s="11"/>
+      <c r="ZG27" s="11"/>
+      <c r="ZH27" s="11"/>
+      <c r="ZI27" s="11"/>
+      <c r="ZJ27" s="11"/>
+      <c r="ZK27" s="11"/>
+      <c r="ZL27" s="11"/>
+      <c r="ZM27" s="11"/>
+      <c r="ZN27" s="11"/>
+      <c r="ZO27" s="11"/>
+      <c r="ZP27" s="11"/>
+      <c r="ZQ27" s="11"/>
+      <c r="ZR27" s="11"/>
+      <c r="ZS27" s="11"/>
+      <c r="ZT27" s="11"/>
+      <c r="ZU27" s="11"/>
+      <c r="ZV27" s="11"/>
+      <c r="ZW27" s="11"/>
+      <c r="ZX27" s="11"/>
+      <c r="ZY27" s="11"/>
+      <c r="ZZ27" s="11"/>
+      <c r="AAA27" s="11"/>
+      <c r="AAB27" s="11"/>
+      <c r="AAC27" s="11"/>
+      <c r="AAD27" s="11"/>
+      <c r="AAE27" s="11"/>
+      <c r="AAF27" s="11"/>
+      <c r="AAG27" s="11"/>
+      <c r="AAH27" s="11"/>
+      <c r="AAI27" s="11"/>
+      <c r="AAJ27" s="11"/>
+      <c r="AAK27" s="11"/>
+      <c r="AAL27" s="11"/>
+      <c r="AAM27" s="11"/>
+      <c r="AAN27" s="11"/>
+      <c r="AAO27" s="11"/>
+      <c r="AAP27" s="11"/>
+      <c r="AAQ27" s="11"/>
+      <c r="AAR27" s="11"/>
+      <c r="AAS27" s="11"/>
+      <c r="AAT27" s="11"/>
+      <c r="AAU27" s="11"/>
+      <c r="AAV27" s="11"/>
+      <c r="AAW27" s="11"/>
+      <c r="AAX27" s="11"/>
+      <c r="AAY27" s="11"/>
+      <c r="AAZ27" s="11"/>
+      <c r="ABA27" s="11"/>
+      <c r="ABB27" s="11"/>
+      <c r="ABC27" s="11"/>
+      <c r="ABD27" s="11"/>
+      <c r="ABE27" s="11"/>
+      <c r="ABF27" s="11"/>
+      <c r="ABG27" s="11"/>
+      <c r="ABH27" s="11"/>
+      <c r="ABI27" s="11"/>
+      <c r="ABJ27" s="11"/>
+      <c r="ABK27" s="11"/>
+      <c r="ABL27" s="11"/>
+      <c r="ABM27" s="11"/>
+      <c r="ABN27" s="11"/>
+      <c r="ABO27" s="11"/>
+      <c r="ABP27" s="11"/>
+      <c r="ABQ27" s="11"/>
+      <c r="ABR27" s="11"/>
+      <c r="ABS27" s="11"/>
+      <c r="ABT27" s="11"/>
+      <c r="ABU27" s="11"/>
+      <c r="ABV27" s="11"/>
+      <c r="ABW27" s="11"/>
+      <c r="ABX27" s="11"/>
+      <c r="ABY27" s="11"/>
+      <c r="ABZ27" s="11"/>
+      <c r="ACA27" s="11"/>
+      <c r="ACB27" s="11"/>
+      <c r="ACC27" s="11"/>
+      <c r="ACD27" s="11"/>
+      <c r="ACE27" s="11"/>
+      <c r="ACF27" s="11"/>
+      <c r="ACG27" s="11"/>
+      <c r="ACH27" s="11"/>
+      <c r="ACI27" s="11"/>
+      <c r="ACJ27" s="11"/>
+      <c r="ACK27" s="11"/>
+      <c r="ACL27" s="11"/>
+      <c r="ACM27" s="11"/>
+      <c r="ACN27" s="11"/>
+      <c r="ACO27" s="11"/>
+      <c r="ACP27" s="11"/>
+      <c r="ACQ27" s="11"/>
+      <c r="ACR27" s="11"/>
+      <c r="ACS27" s="11"/>
+      <c r="ACT27" s="11"/>
+      <c r="ACU27" s="11"/>
+      <c r="ACV27" s="11"/>
+      <c r="ACW27" s="11"/>
+      <c r="ACX27" s="11"/>
+      <c r="ACY27" s="11"/>
+      <c r="ACZ27" s="11"/>
+      <c r="ADA27" s="11"/>
+      <c r="ADB27" s="11"/>
+      <c r="ADC27" s="11"/>
+      <c r="ADD27" s="11"/>
+      <c r="ADE27" s="11"/>
+      <c r="ADF27" s="11"/>
+      <c r="ADG27" s="11"/>
+      <c r="ADH27" s="11"/>
+      <c r="ADI27" s="11"/>
+      <c r="ADJ27" s="11"/>
+      <c r="ADK27" s="11"/>
+      <c r="ADL27" s="11"/>
+      <c r="ADM27" s="11"/>
+      <c r="ADN27" s="11"/>
+      <c r="ADO27" s="11"/>
+      <c r="ADP27" s="11"/>
+      <c r="ADQ27" s="11"/>
+      <c r="ADR27" s="11"/>
+      <c r="ADS27" s="11"/>
+      <c r="ADT27" s="11"/>
+      <c r="ADU27" s="11"/>
+      <c r="ADV27" s="11"/>
+      <c r="ADW27" s="11"/>
+      <c r="ADX27" s="11"/>
+      <c r="ADY27" s="11"/>
+      <c r="ADZ27" s="11"/>
+      <c r="AEA27" s="11"/>
+      <c r="AEB27" s="11"/>
+      <c r="AEC27" s="11"/>
+      <c r="AED27" s="11"/>
+      <c r="AEE27" s="11"/>
+      <c r="AEF27" s="11"/>
+      <c r="AEG27" s="11"/>
+      <c r="AEH27" s="11"/>
+      <c r="AEI27" s="11"/>
+      <c r="AEJ27" s="11"/>
+      <c r="AEK27" s="11"/>
+      <c r="AEL27" s="11"/>
+      <c r="AEM27" s="11"/>
+      <c r="AEN27" s="11"/>
+      <c r="AEO27" s="11"/>
+      <c r="AEP27" s="11"/>
+      <c r="AEQ27" s="11"/>
+      <c r="AER27" s="11"/>
+      <c r="AES27" s="11"/>
+      <c r="AET27" s="11"/>
+      <c r="AEU27" s="11"/>
+      <c r="AEV27" s="11"/>
+      <c r="AEW27" s="11"/>
+      <c r="AEX27" s="11"/>
+      <c r="AEY27" s="11"/>
+      <c r="AEZ27" s="11"/>
+      <c r="AFA27" s="11"/>
+      <c r="AFB27" s="11"/>
+      <c r="AFC27" s="11"/>
+      <c r="AFD27" s="11"/>
+      <c r="AFE27" s="11"/>
+      <c r="AFF27" s="11"/>
+      <c r="AFG27" s="11"/>
+      <c r="AFH27" s="11"/>
+      <c r="AFI27" s="11"/>
+      <c r="AFJ27" s="11"/>
+      <c r="AFK27" s="11"/>
+      <c r="AFL27" s="11"/>
+      <c r="AFM27" s="11"/>
+      <c r="AFN27" s="11"/>
+      <c r="AFO27" s="11"/>
+      <c r="AFP27" s="11"/>
+      <c r="AFQ27" s="11"/>
+      <c r="AFR27" s="11"/>
+      <c r="AFS27" s="11"/>
+      <c r="AFT27" s="11"/>
+      <c r="AFU27" s="11"/>
+      <c r="AFV27" s="11"/>
+      <c r="AFW27" s="11"/>
+      <c r="AFX27" s="11"/>
+      <c r="AFY27" s="11"/>
+      <c r="AFZ27" s="11"/>
+      <c r="AGA27" s="11"/>
+      <c r="AGB27" s="11"/>
+      <c r="AGC27" s="11"/>
+      <c r="AGD27" s="11"/>
+      <c r="AGE27" s="11"/>
+      <c r="AGF27" s="11"/>
+      <c r="AGG27" s="11"/>
+      <c r="AGH27" s="11"/>
+      <c r="AGI27" s="11"/>
+      <c r="AGJ27" s="11"/>
+      <c r="AGK27" s="11"/>
+      <c r="AGL27" s="11"/>
+      <c r="AGM27" s="11"/>
+      <c r="AGN27" s="11"/>
+      <c r="AGO27" s="11"/>
+      <c r="AGP27" s="11"/>
+      <c r="AGQ27" s="11"/>
+      <c r="AGR27" s="11"/>
+      <c r="AGS27" s="11"/>
+      <c r="AGT27" s="11"/>
+      <c r="AGU27" s="11"/>
+      <c r="AGV27" s="11"/>
+      <c r="AGW27" s="11"/>
+      <c r="AGX27" s="11"/>
+      <c r="AGY27" s="11"/>
+      <c r="AGZ27" s="11"/>
+      <c r="AHA27" s="11"/>
+      <c r="AHB27" s="11"/>
+      <c r="AHC27" s="11"/>
+      <c r="AHD27" s="11"/>
+      <c r="AHE27" s="11"/>
+      <c r="AHF27" s="11"/>
+      <c r="AHG27" s="11"/>
+      <c r="AHH27" s="11"/>
+      <c r="AHI27" s="11"/>
+      <c r="AHJ27" s="11"/>
+      <c r="AHK27" s="11"/>
+      <c r="AHL27" s="11"/>
+      <c r="AHM27" s="11"/>
+      <c r="AHN27" s="11"/>
+      <c r="AHO27" s="11"/>
+      <c r="AHP27" s="11"/>
+      <c r="AHQ27" s="11"/>
+      <c r="AHR27" s="11"/>
+      <c r="AHS27" s="11"/>
+      <c r="AHT27" s="11"/>
+      <c r="AHU27" s="11"/>
+      <c r="AHV27" s="11"/>
+      <c r="AHW27" s="11"/>
+      <c r="AHX27" s="11"/>
+      <c r="AHY27" s="11"/>
+      <c r="AHZ27" s="11"/>
+      <c r="AIA27" s="11"/>
+      <c r="AIB27" s="11"/>
+      <c r="AIC27" s="11"/>
+      <c r="AID27" s="11"/>
+      <c r="AIE27" s="11"/>
+      <c r="AIF27" s="11"/>
+      <c r="AIG27" s="11"/>
+      <c r="AIH27" s="11"/>
+      <c r="AII27" s="11"/>
+      <c r="AIJ27" s="11"/>
+      <c r="AIK27" s="11"/>
+      <c r="AIL27" s="11"/>
+      <c r="AIM27" s="11"/>
+      <c r="AIN27" s="11"/>
+      <c r="AIO27" s="11"/>
+      <c r="AIP27" s="11"/>
+      <c r="AIQ27" s="11"/>
+      <c r="AIR27" s="11"/>
+      <c r="AIS27" s="11"/>
+      <c r="AIT27" s="11"/>
+      <c r="AIU27" s="11"/>
+      <c r="AIV27" s="11"/>
+      <c r="AIW27" s="11"/>
+      <c r="AIX27" s="11"/>
+      <c r="AIY27" s="11"/>
+      <c r="AIZ27" s="11"/>
+      <c r="AJA27" s="11"/>
+      <c r="AJB27" s="11"/>
+      <c r="AJC27" s="11"/>
+      <c r="AJD27" s="11"/>
+      <c r="AJE27" s="11"/>
+      <c r="AJF27" s="11"/>
+      <c r="AJG27" s="11"/>
+      <c r="AJH27" s="11"/>
+      <c r="AJI27" s="11"/>
+      <c r="AJJ27" s="11"/>
+      <c r="AJK27" s="11"/>
+      <c r="AJL27" s="11"/>
+      <c r="AJM27" s="11"/>
+      <c r="AJN27" s="11"/>
+      <c r="AJO27" s="11"/>
+      <c r="AJP27" s="11"/>
+      <c r="AJQ27" s="11"/>
+      <c r="AJR27" s="11"/>
+      <c r="AJS27" s="11"/>
+      <c r="AJT27" s="11"/>
+      <c r="AJU27" s="11"/>
+      <c r="AJV27" s="11"/>
+      <c r="AJW27" s="11"/>
+      <c r="AJX27" s="11"/>
+      <c r="AJY27" s="11"/>
+      <c r="AJZ27" s="11"/>
+      <c r="AKA27" s="11"/>
+      <c r="AKB27" s="11"/>
+      <c r="AKC27" s="11"/>
+      <c r="AKD27" s="11"/>
+      <c r="AKE27" s="11"/>
+      <c r="AKF27" s="11"/>
+      <c r="AKG27" s="11"/>
+      <c r="AKH27" s="11"/>
+      <c r="AKI27" s="11"/>
+      <c r="AKJ27" s="11"/>
+      <c r="AKK27" s="11"/>
+      <c r="AKL27" s="11"/>
+      <c r="AKM27" s="11"/>
+      <c r="AKN27" s="11"/>
+      <c r="AKO27" s="11"/>
+      <c r="AKP27" s="11"/>
+      <c r="AKQ27" s="11"/>
+      <c r="AKR27" s="11"/>
+      <c r="AKS27" s="11"/>
+      <c r="AKT27" s="11"/>
+      <c r="AKU27" s="11"/>
+      <c r="AKV27" s="11"/>
+      <c r="AKW27" s="11"/>
+      <c r="AKX27" s="11"/>
+      <c r="AKY27" s="11"/>
+      <c r="AKZ27" s="11"/>
+      <c r="ALA27" s="11"/>
+      <c r="ALB27" s="11"/>
+      <c r="ALC27" s="11"/>
+      <c r="ALD27" s="11"/>
+      <c r="ALE27" s="11"/>
+      <c r="ALF27" s="11"/>
+      <c r="ALG27" s="11"/>
+      <c r="ALH27" s="11"/>
+      <c r="ALI27" s="11"/>
+      <c r="ALJ27" s="11"/>
+      <c r="ALK27" s="11"/>
+      <c r="ALL27" s="11"/>
+      <c r="ALM27" s="11"/>
+      <c r="ALN27" s="11"/>
+      <c r="ALO27" s="11"/>
+      <c r="ALP27" s="11"/>
+      <c r="ALQ27" s="11"/>
+      <c r="ALR27" s="11"/>
+      <c r="ALS27" s="11"/>
+      <c r="ALT27" s="11"/>
+      <c r="ALU27" s="11"/>
+      <c r="ALV27" s="11"/>
+      <c r="ALW27" s="11"/>
+      <c r="ALX27" s="11"/>
+      <c r="ALY27" s="11"/>
+      <c r="ALZ27" s="11"/>
+      <c r="AMA27" s="11"/>
+      <c r="AMB27" s="11"/>
+      <c r="AMC27" s="11"/>
+      <c r="AMD27" s="11"/>
+      <c r="AME27" s="11"/>
+      <c r="AMF27" s="11"/>
+      <c r="AMG27" s="11"/>
+      <c r="AMH27" s="11"/>
+      <c r="AMI27" s="11"/>
+      <c r="AMJ27" s="11"/>
+      <c r="AMK27" s="11"/>
+      <c r="AML27" s="11"/>
     </row>
-    <row r="26" spans="1:1026" s="14" customFormat="1" ht="29">
-      <c r="A26" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="12">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K26" s="11"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
-      <c r="Z26" s="11"/>
-      <c r="AA26" s="11"/>
-      <c r="AB26" s="11"/>
-      <c r="AC26" s="11"/>
-      <c r="AD26" s="11"/>
-      <c r="AE26" s="11"/>
-      <c r="AF26" s="11"/>
-      <c r="AG26" s="11"/>
-      <c r="AH26" s="11"/>
-      <c r="AI26" s="11"/>
-      <c r="AJ26" s="11"/>
-      <c r="AK26" s="11"/>
-      <c r="AL26" s="11"/>
-      <c r="AM26" s="11"/>
-      <c r="AN26" s="11"/>
-      <c r="AO26" s="11"/>
-      <c r="AP26" s="11"/>
-      <c r="AQ26" s="11"/>
-      <c r="AR26" s="11"/>
-      <c r="AS26" s="11"/>
-      <c r="AT26" s="11"/>
-      <c r="AU26" s="11"/>
-      <c r="AV26" s="11"/>
-      <c r="AW26" s="11"/>
-      <c r="AX26" s="11"/>
-      <c r="AY26" s="11"/>
-      <c r="AZ26" s="11"/>
-      <c r="BA26" s="11"/>
-      <c r="BB26" s="11"/>
-      <c r="BC26" s="11"/>
-      <c r="BD26" s="11"/>
-      <c r="BE26" s="11"/>
-      <c r="BF26" s="11"/>
-      <c r="BG26" s="11"/>
-      <c r="BH26" s="11"/>
-      <c r="BI26" s="11"/>
-      <c r="BJ26" s="11"/>
-      <c r="BK26" s="11"/>
-      <c r="BL26" s="11"/>
-      <c r="BM26" s="11"/>
-      <c r="BN26" s="11"/>
-      <c r="BO26" s="11"/>
-      <c r="BP26" s="11"/>
-      <c r="BQ26" s="11"/>
-      <c r="BR26" s="11"/>
-      <c r="BS26" s="11"/>
-      <c r="BT26" s="11"/>
-      <c r="BU26" s="11"/>
-      <c r="BV26" s="11"/>
-      <c r="BW26" s="11"/>
-      <c r="BX26" s="11"/>
-      <c r="BY26" s="11"/>
-      <c r="BZ26" s="11"/>
-      <c r="CA26" s="11"/>
-      <c r="CB26" s="11"/>
-      <c r="CC26" s="11"/>
-      <c r="CD26" s="11"/>
-      <c r="CE26" s="11"/>
-      <c r="CF26" s="11"/>
-      <c r="CG26" s="11"/>
-      <c r="CH26" s="11"/>
-      <c r="CI26" s="11"/>
-      <c r="CJ26" s="11"/>
-      <c r="CK26" s="11"/>
-      <c r="CL26" s="11"/>
-      <c r="CM26" s="11"/>
-      <c r="CN26" s="11"/>
-      <c r="CO26" s="11"/>
-      <c r="CP26" s="11"/>
-      <c r="CQ26" s="11"/>
-      <c r="CR26" s="11"/>
-      <c r="CS26" s="11"/>
-      <c r="CT26" s="11"/>
-      <c r="CU26" s="11"/>
-      <c r="CV26" s="11"/>
-      <c r="CW26" s="11"/>
-      <c r="CX26" s="11"/>
-      <c r="CY26" s="11"/>
-      <c r="CZ26" s="11"/>
-      <c r="DA26" s="11"/>
-      <c r="DB26" s="11"/>
-      <c r="DC26" s="11"/>
-      <c r="DD26" s="11"/>
-      <c r="DE26" s="11"/>
-      <c r="DF26" s="11"/>
-      <c r="DG26" s="11"/>
-      <c r="DH26" s="11"/>
-      <c r="DI26" s="11"/>
-      <c r="DJ26" s="11"/>
-      <c r="DK26" s="11"/>
-      <c r="DL26" s="11"/>
-      <c r="DM26" s="11"/>
-      <c r="DN26" s="11"/>
-      <c r="DO26" s="11"/>
-      <c r="DP26" s="11"/>
-      <c r="DQ26" s="11"/>
-      <c r="DR26" s="11"/>
-      <c r="DS26" s="11"/>
-      <c r="DT26" s="11"/>
-      <c r="DU26" s="11"/>
-      <c r="DV26" s="11"/>
-      <c r="DW26" s="11"/>
-      <c r="DX26" s="11"/>
-      <c r="DY26" s="11"/>
-      <c r="DZ26" s="11"/>
-      <c r="EA26" s="11"/>
-      <c r="EB26" s="11"/>
-      <c r="EC26" s="11"/>
-      <c r="ED26" s="11"/>
-      <c r="EE26" s="11"/>
-      <c r="EF26" s="11"/>
-      <c r="EG26" s="11"/>
-      <c r="EH26" s="11"/>
-      <c r="EI26" s="11"/>
-      <c r="EJ26" s="11"/>
-      <c r="EK26" s="11"/>
-      <c r="EL26" s="11"/>
-      <c r="EM26" s="11"/>
-      <c r="EN26" s="11"/>
-      <c r="EO26" s="11"/>
-      <c r="EP26" s="11"/>
-      <c r="EQ26" s="11"/>
-      <c r="ER26" s="11"/>
-      <c r="ES26" s="11"/>
-      <c r="ET26" s="11"/>
-      <c r="EU26" s="11"/>
-      <c r="EV26" s="11"/>
-      <c r="EW26" s="11"/>
-      <c r="EX26" s="11"/>
-      <c r="EY26" s="11"/>
-      <c r="EZ26" s="11"/>
-      <c r="FA26" s="11"/>
-      <c r="FB26" s="11"/>
-      <c r="FC26" s="11"/>
-      <c r="FD26" s="11"/>
-      <c r="FE26" s="11"/>
-      <c r="FF26" s="11"/>
-      <c r="FG26" s="11"/>
-      <c r="FH26" s="11"/>
-      <c r="FI26" s="11"/>
-      <c r="FJ26" s="11"/>
-      <c r="FK26" s="11"/>
-      <c r="FL26" s="11"/>
-      <c r="FM26" s="11"/>
-      <c r="FN26" s="11"/>
-      <c r="FO26" s="11"/>
-      <c r="FP26" s="11"/>
-      <c r="FQ26" s="11"/>
-      <c r="FR26" s="11"/>
-      <c r="FS26" s="11"/>
-      <c r="FT26" s="11"/>
-      <c r="FU26" s="11"/>
-      <c r="FV26" s="11"/>
-      <c r="FW26" s="11"/>
-      <c r="FX26" s="11"/>
-      <c r="FY26" s="11"/>
-      <c r="FZ26" s="11"/>
-      <c r="GA26" s="11"/>
-      <c r="GB26" s="11"/>
-      <c r="GC26" s="11"/>
-      <c r="GD26" s="11"/>
-      <c r="GE26" s="11"/>
-      <c r="GF26" s="11"/>
-      <c r="GG26" s="11"/>
-      <c r="GH26" s="11"/>
-      <c r="GI26" s="11"/>
-      <c r="GJ26" s="11"/>
-      <c r="GK26" s="11"/>
-      <c r="GL26" s="11"/>
-      <c r="GM26" s="11"/>
-      <c r="GN26" s="11"/>
-      <c r="GO26" s="11"/>
-      <c r="GP26" s="11"/>
-      <c r="GQ26" s="11"/>
-      <c r="GR26" s="11"/>
-      <c r="GS26" s="11"/>
-      <c r="GT26" s="11"/>
-      <c r="GU26" s="11"/>
-      <c r="GV26" s="11"/>
-      <c r="GW26" s="11"/>
-      <c r="GX26" s="11"/>
-      <c r="GY26" s="11"/>
-      <c r="GZ26" s="11"/>
-      <c r="HA26" s="11"/>
-      <c r="HB26" s="11"/>
-      <c r="HC26" s="11"/>
-      <c r="HD26" s="11"/>
-      <c r="HE26" s="11"/>
-      <c r="HF26" s="11"/>
-      <c r="HG26" s="11"/>
-      <c r="HH26" s="11"/>
-      <c r="HI26" s="11"/>
-      <c r="HJ26" s="11"/>
-      <c r="HK26" s="11"/>
-      <c r="HL26" s="11"/>
-      <c r="HM26" s="11"/>
-      <c r="HN26" s="11"/>
-      <c r="HO26" s="11"/>
-      <c r="HP26" s="11"/>
-      <c r="HQ26" s="11"/>
-      <c r="HR26" s="11"/>
-      <c r="HS26" s="11"/>
-      <c r="HT26" s="11"/>
-      <c r="HU26" s="11"/>
-      <c r="HV26" s="11"/>
-      <c r="HW26" s="11"/>
-      <c r="HX26" s="11"/>
-      <c r="HY26" s="11"/>
-      <c r="HZ26" s="11"/>
-      <c r="IA26" s="11"/>
-      <c r="IB26" s="11"/>
-      <c r="IC26" s="11"/>
-      <c r="ID26" s="11"/>
-      <c r="IE26" s="11"/>
-      <c r="IF26" s="11"/>
-      <c r="IG26" s="11"/>
-      <c r="IH26" s="11"/>
-      <c r="II26" s="11"/>
-      <c r="IJ26" s="11"/>
-      <c r="IK26" s="11"/>
-      <c r="IL26" s="11"/>
-      <c r="IM26" s="11"/>
-      <c r="IN26" s="11"/>
-      <c r="IO26" s="11"/>
-      <c r="IP26" s="11"/>
-      <c r="IQ26" s="11"/>
-      <c r="IR26" s="11"/>
-      <c r="IS26" s="11"/>
-      <c r="IT26" s="11"/>
-      <c r="IU26" s="11"/>
-      <c r="IV26" s="11"/>
-      <c r="IW26" s="11"/>
-      <c r="IX26" s="11"/>
-      <c r="IY26" s="11"/>
-      <c r="IZ26" s="11"/>
-      <c r="JA26" s="11"/>
-      <c r="JB26" s="11"/>
-      <c r="JC26" s="11"/>
-      <c r="JD26" s="11"/>
-      <c r="JE26" s="11"/>
-      <c r="JF26" s="11"/>
-      <c r="JG26" s="11"/>
-      <c r="JH26" s="11"/>
-      <c r="JI26" s="11"/>
-      <c r="JJ26" s="11"/>
-      <c r="JK26" s="11"/>
-      <c r="JL26" s="11"/>
-      <c r="JM26" s="11"/>
-      <c r="JN26" s="11"/>
-      <c r="JO26" s="11"/>
-      <c r="JP26" s="11"/>
-      <c r="JQ26" s="11"/>
-      <c r="JR26" s="11"/>
-      <c r="JS26" s="11"/>
-      <c r="JT26" s="11"/>
-      <c r="JU26" s="11"/>
-      <c r="JV26" s="11"/>
-      <c r="JW26" s="11"/>
-      <c r="JX26" s="11"/>
-      <c r="JY26" s="11"/>
-      <c r="JZ26" s="11"/>
-      <c r="KA26" s="11"/>
-      <c r="KB26" s="11"/>
-      <c r="KC26" s="11"/>
-      <c r="KD26" s="11"/>
-      <c r="KE26" s="11"/>
-      <c r="KF26" s="11"/>
-      <c r="KG26" s="11"/>
-      <c r="KH26" s="11"/>
-      <c r="KI26" s="11"/>
-      <c r="KJ26" s="11"/>
-      <c r="KK26" s="11"/>
-      <c r="KL26" s="11"/>
-      <c r="KM26" s="11"/>
-      <c r="KN26" s="11"/>
-      <c r="KO26" s="11"/>
-      <c r="KP26" s="11"/>
-      <c r="KQ26" s="11"/>
-      <c r="KR26" s="11"/>
-      <c r="KS26" s="11"/>
-      <c r="KT26" s="11"/>
-      <c r="KU26" s="11"/>
-      <c r="KV26" s="11"/>
-      <c r="KW26" s="11"/>
-      <c r="KX26" s="11"/>
-      <c r="KY26" s="11"/>
-      <c r="KZ26" s="11"/>
-      <c r="LA26" s="11"/>
-      <c r="LB26" s="11"/>
-      <c r="LC26" s="11"/>
-      <c r="LD26" s="11"/>
-      <c r="LE26" s="11"/>
-      <c r="LF26" s="11"/>
-      <c r="LG26" s="11"/>
-      <c r="LH26" s="11"/>
-      <c r="LI26" s="11"/>
-      <c r="LJ26" s="11"/>
-      <c r="LK26" s="11"/>
-      <c r="LL26" s="11"/>
-      <c r="LM26" s="11"/>
-      <c r="LN26" s="11"/>
-      <c r="LO26" s="11"/>
-      <c r="LP26" s="11"/>
-      <c r="LQ26" s="11"/>
-      <c r="LR26" s="11"/>
-      <c r="LS26" s="11"/>
-      <c r="LT26" s="11"/>
-      <c r="LU26" s="11"/>
-      <c r="LV26" s="11"/>
-      <c r="LW26" s="11"/>
-      <c r="LX26" s="11"/>
-      <c r="LY26" s="11"/>
-      <c r="LZ26" s="11"/>
-      <c r="MA26" s="11"/>
-      <c r="MB26" s="11"/>
-      <c r="MC26" s="11"/>
-      <c r="MD26" s="11"/>
-      <c r="ME26" s="11"/>
-      <c r="MF26" s="11"/>
-      <c r="MG26" s="11"/>
-      <c r="MH26" s="11"/>
-      <c r="MI26" s="11"/>
-      <c r="MJ26" s="11"/>
-      <c r="MK26" s="11"/>
-      <c r="ML26" s="11"/>
-      <c r="MM26" s="11"/>
-      <c r="MN26" s="11"/>
-      <c r="MO26" s="11"/>
-      <c r="MP26" s="11"/>
-      <c r="MQ26" s="11"/>
-      <c r="MR26" s="11"/>
-      <c r="MS26" s="11"/>
-      <c r="MT26" s="11"/>
-      <c r="MU26" s="11"/>
-      <c r="MV26" s="11"/>
-      <c r="MW26" s="11"/>
-      <c r="MX26" s="11"/>
-      <c r="MY26" s="11"/>
-      <c r="MZ26" s="11"/>
-      <c r="NA26" s="11"/>
-      <c r="NB26" s="11"/>
-      <c r="NC26" s="11"/>
-      <c r="ND26" s="11"/>
-      <c r="NE26" s="11"/>
-      <c r="NF26" s="11"/>
-      <c r="NG26" s="11"/>
-      <c r="NH26" s="11"/>
-      <c r="NI26" s="11"/>
-      <c r="NJ26" s="11"/>
-      <c r="NK26" s="11"/>
-      <c r="NL26" s="11"/>
-      <c r="NM26" s="11"/>
-      <c r="NN26" s="11"/>
-      <c r="NO26" s="11"/>
-      <c r="NP26" s="11"/>
-      <c r="NQ26" s="11"/>
-      <c r="NR26" s="11"/>
-      <c r="NS26" s="11"/>
-      <c r="NT26" s="11"/>
-      <c r="NU26" s="11"/>
-      <c r="NV26" s="11"/>
-      <c r="NW26" s="11"/>
-      <c r="NX26" s="11"/>
-      <c r="NY26" s="11"/>
-      <c r="NZ26" s="11"/>
-      <c r="OA26" s="11"/>
-      <c r="OB26" s="11"/>
-      <c r="OC26" s="11"/>
-      <c r="OD26" s="11"/>
-      <c r="OE26" s="11"/>
-      <c r="OF26" s="11"/>
-      <c r="OG26" s="11"/>
-      <c r="OH26" s="11"/>
-      <c r="OI26" s="11"/>
-      <c r="OJ26" s="11"/>
-      <c r="OK26" s="11"/>
-      <c r="OL26" s="11"/>
-      <c r="OM26" s="11"/>
-      <c r="ON26" s="11"/>
-      <c r="OO26" s="11"/>
-      <c r="OP26" s="11"/>
-      <c r="OQ26" s="11"/>
-      <c r="OR26" s="11"/>
-      <c r="OS26" s="11"/>
-      <c r="OT26" s="11"/>
-      <c r="OU26" s="11"/>
-      <c r="OV26" s="11"/>
-      <c r="OW26" s="11"/>
-      <c r="OX26" s="11"/>
-      <c r="OY26" s="11"/>
-      <c r="OZ26" s="11"/>
-      <c r="PA26" s="11"/>
-      <c r="PB26" s="11"/>
-      <c r="PC26" s="11"/>
-      <c r="PD26" s="11"/>
-      <c r="PE26" s="11"/>
-      <c r="PF26" s="11"/>
-      <c r="PG26" s="11"/>
-      <c r="PH26" s="11"/>
-      <c r="PI26" s="11"/>
-      <c r="PJ26" s="11"/>
-      <c r="PK26" s="11"/>
-      <c r="PL26" s="11"/>
-      <c r="PM26" s="11"/>
-      <c r="PN26" s="11"/>
-      <c r="PO26" s="11"/>
-      <c r="PP26" s="11"/>
-      <c r="PQ26" s="11"/>
-      <c r="PR26" s="11"/>
-      <c r="PS26" s="11"/>
-      <c r="PT26" s="11"/>
-      <c r="PU26" s="11"/>
-      <c r="PV26" s="11"/>
-      <c r="PW26" s="11"/>
-      <c r="PX26" s="11"/>
-      <c r="PY26" s="11"/>
-      <c r="PZ26" s="11"/>
-      <c r="QA26" s="11"/>
-      <c r="QB26" s="11"/>
-      <c r="QC26" s="11"/>
-      <c r="QD26" s="11"/>
-      <c r="QE26" s="11"/>
-      <c r="QF26" s="11"/>
-      <c r="QG26" s="11"/>
-      <c r="QH26" s="11"/>
-      <c r="QI26" s="11"/>
-      <c r="QJ26" s="11"/>
-      <c r="QK26" s="11"/>
-      <c r="QL26" s="11"/>
-      <c r="QM26" s="11"/>
-      <c r="QN26" s="11"/>
-      <c r="QO26" s="11"/>
-      <c r="QP26" s="11"/>
-      <c r="QQ26" s="11"/>
-      <c r="QR26" s="11"/>
-      <c r="QS26" s="11"/>
-      <c r="QT26" s="11"/>
-      <c r="QU26" s="11"/>
-      <c r="QV26" s="11"/>
-      <c r="QW26" s="11"/>
-      <c r="QX26" s="11"/>
-      <c r="QY26" s="11"/>
-      <c r="QZ26" s="11"/>
-      <c r="RA26" s="11"/>
-      <c r="RB26" s="11"/>
-      <c r="RC26" s="11"/>
-      <c r="RD26" s="11"/>
-      <c r="RE26" s="11"/>
-      <c r="RF26" s="11"/>
-      <c r="RG26" s="11"/>
-      <c r="RH26" s="11"/>
-      <c r="RI26" s="11"/>
-      <c r="RJ26" s="11"/>
-      <c r="RK26" s="11"/>
-      <c r="RL26" s="11"/>
-      <c r="RM26" s="11"/>
-      <c r="RN26" s="11"/>
-      <c r="RO26" s="11"/>
-      <c r="RP26" s="11"/>
-      <c r="RQ26" s="11"/>
-      <c r="RR26" s="11"/>
-      <c r="RS26" s="11"/>
-      <c r="RT26" s="11"/>
-      <c r="RU26" s="11"/>
-      <c r="RV26" s="11"/>
-      <c r="RW26" s="11"/>
-      <c r="RX26" s="11"/>
-      <c r="RY26" s="11"/>
-      <c r="RZ26" s="11"/>
-      <c r="SA26" s="11"/>
-      <c r="SB26" s="11"/>
-      <c r="SC26" s="11"/>
-      <c r="SD26" s="11"/>
-      <c r="SE26" s="11"/>
-      <c r="SF26" s="11"/>
-      <c r="SG26" s="11"/>
-      <c r="SH26" s="11"/>
-      <c r="SI26" s="11"/>
-      <c r="SJ26" s="11"/>
-      <c r="SK26" s="11"/>
-      <c r="SL26" s="11"/>
-      <c r="SM26" s="11"/>
-      <c r="SN26" s="11"/>
-      <c r="SO26" s="11"/>
-      <c r="SP26" s="11"/>
-      <c r="SQ26" s="11"/>
-      <c r="SR26" s="11"/>
-      <c r="SS26" s="11"/>
-      <c r="ST26" s="11"/>
-      <c r="SU26" s="11"/>
-      <c r="SV26" s="11"/>
-      <c r="SW26" s="11"/>
-      <c r="SX26" s="11"/>
-      <c r="SY26" s="11"/>
-      <c r="SZ26" s="11"/>
-      <c r="TA26" s="11"/>
-      <c r="TB26" s="11"/>
-      <c r="TC26" s="11"/>
-      <c r="TD26" s="11"/>
-      <c r="TE26" s="11"/>
-      <c r="TF26" s="11"/>
-      <c r="TG26" s="11"/>
-      <c r="TH26" s="11"/>
-      <c r="TI26" s="11"/>
-      <c r="TJ26" s="11"/>
-      <c r="TK26" s="11"/>
-      <c r="TL26" s="11"/>
-      <c r="TM26" s="11"/>
-      <c r="TN26" s="11"/>
-      <c r="TO26" s="11"/>
-      <c r="TP26" s="11"/>
-      <c r="TQ26" s="11"/>
-      <c r="TR26" s="11"/>
-      <c r="TS26" s="11"/>
-      <c r="TT26" s="11"/>
-      <c r="TU26" s="11"/>
-      <c r="TV26" s="11"/>
-      <c r="TW26" s="11"/>
-      <c r="TX26" s="11"/>
-      <c r="TY26" s="11"/>
-      <c r="TZ26" s="11"/>
-      <c r="UA26" s="11"/>
-      <c r="UB26" s="11"/>
-      <c r="UC26" s="11"/>
-      <c r="UD26" s="11"/>
-      <c r="UE26" s="11"/>
-      <c r="UF26" s="11"/>
-      <c r="UG26" s="11"/>
-      <c r="UH26" s="11"/>
-      <c r="UI26" s="11"/>
-      <c r="UJ26" s="11"/>
-      <c r="UK26" s="11"/>
-      <c r="UL26" s="11"/>
-      <c r="UM26" s="11"/>
-      <c r="UN26" s="11"/>
-      <c r="UO26" s="11"/>
-      <c r="UP26" s="11"/>
-      <c r="UQ26" s="11"/>
-      <c r="UR26" s="11"/>
-      <c r="US26" s="11"/>
-      <c r="UT26" s="11"/>
-      <c r="UU26" s="11"/>
-      <c r="UV26" s="11"/>
-      <c r="UW26" s="11"/>
-      <c r="UX26" s="11"/>
-      <c r="UY26" s="11"/>
-      <c r="UZ26" s="11"/>
-      <c r="VA26" s="11"/>
-      <c r="VB26" s="11"/>
-      <c r="VC26" s="11"/>
-      <c r="VD26" s="11"/>
-      <c r="VE26" s="11"/>
-      <c r="VF26" s="11"/>
-      <c r="VG26" s="11"/>
-      <c r="VH26" s="11"/>
-      <c r="VI26" s="11"/>
-      <c r="VJ26" s="11"/>
-      <c r="VK26" s="11"/>
-      <c r="VL26" s="11"/>
-      <c r="VM26" s="11"/>
-      <c r="VN26" s="11"/>
-      <c r="VO26" s="11"/>
-      <c r="VP26" s="11"/>
-      <c r="VQ26" s="11"/>
-      <c r="VR26" s="11"/>
-      <c r="VS26" s="11"/>
-      <c r="VT26" s="11"/>
-      <c r="VU26" s="11"/>
-      <c r="VV26" s="11"/>
-      <c r="VW26" s="11"/>
-      <c r="VX26" s="11"/>
-      <c r="VY26" s="11"/>
-      <c r="VZ26" s="11"/>
-      <c r="WA26" s="11"/>
-      <c r="WB26" s="11"/>
-      <c r="WC26" s="11"/>
-      <c r="WD26" s="11"/>
-      <c r="WE26" s="11"/>
-      <c r="WF26" s="11"/>
-      <c r="WG26" s="11"/>
-      <c r="WH26" s="11"/>
-      <c r="WI26" s="11"/>
-      <c r="WJ26" s="11"/>
-      <c r="WK26" s="11"/>
-      <c r="WL26" s="11"/>
-      <c r="WM26" s="11"/>
-      <c r="WN26" s="11"/>
-      <c r="WO26" s="11"/>
-      <c r="WP26" s="11"/>
-      <c r="WQ26" s="11"/>
-      <c r="WR26" s="11"/>
-      <c r="WS26" s="11"/>
-      <c r="WT26" s="11"/>
-      <c r="WU26" s="11"/>
-      <c r="WV26" s="11"/>
-      <c r="WW26" s="11"/>
-      <c r="WX26" s="11"/>
-      <c r="WY26" s="11"/>
-      <c r="WZ26" s="11"/>
-      <c r="XA26" s="11"/>
-      <c r="XB26" s="11"/>
-      <c r="XC26" s="11"/>
-      <c r="XD26" s="11"/>
-      <c r="XE26" s="11"/>
-      <c r="XF26" s="11"/>
-      <c r="XG26" s="11"/>
-      <c r="XH26" s="11"/>
-      <c r="XI26" s="11"/>
-      <c r="XJ26" s="11"/>
-      <c r="XK26" s="11"/>
-      <c r="XL26" s="11"/>
-      <c r="XM26" s="11"/>
-      <c r="XN26" s="11"/>
-      <c r="XO26" s="11"/>
-      <c r="XP26" s="11"/>
-      <c r="XQ26" s="11"/>
-      <c r="XR26" s="11"/>
-      <c r="XS26" s="11"/>
-      <c r="XT26" s="11"/>
-      <c r="XU26" s="11"/>
-      <c r="XV26" s="11"/>
-      <c r="XW26" s="11"/>
-      <c r="XX26" s="11"/>
-      <c r="XY26" s="11"/>
-      <c r="XZ26" s="11"/>
-      <c r="YA26" s="11"/>
-      <c r="YB26" s="11"/>
-      <c r="YC26" s="11"/>
-      <c r="YD26" s="11"/>
-      <c r="YE26" s="11"/>
-      <c r="YF26" s="11"/>
-      <c r="YG26" s="11"/>
-      <c r="YH26" s="11"/>
-      <c r="YI26" s="11"/>
-      <c r="YJ26" s="11"/>
-      <c r="YK26" s="11"/>
-      <c r="YL26" s="11"/>
-      <c r="YM26" s="11"/>
-      <c r="YN26" s="11"/>
-      <c r="YO26" s="11"/>
-      <c r="YP26" s="11"/>
-      <c r="YQ26" s="11"/>
-      <c r="YR26" s="11"/>
-      <c r="YS26" s="11"/>
-      <c r="YT26" s="11"/>
-      <c r="YU26" s="11"/>
-      <c r="YV26" s="11"/>
-      <c r="YW26" s="11"/>
-      <c r="YX26" s="11"/>
-      <c r="YY26" s="11"/>
-      <c r="YZ26" s="11"/>
-      <c r="ZA26" s="11"/>
-      <c r="ZB26" s="11"/>
-      <c r="ZC26" s="11"/>
-      <c r="ZD26" s="11"/>
-      <c r="ZE26" s="11"/>
-      <c r="ZF26" s="11"/>
-      <c r="ZG26" s="11"/>
-      <c r="ZH26" s="11"/>
-      <c r="ZI26" s="11"/>
-      <c r="ZJ26" s="11"/>
-      <c r="ZK26" s="11"/>
-      <c r="ZL26" s="11"/>
-      <c r="ZM26" s="11"/>
-      <c r="ZN26" s="11"/>
-      <c r="ZO26" s="11"/>
-      <c r="ZP26" s="11"/>
-      <c r="ZQ26" s="11"/>
-      <c r="ZR26" s="11"/>
-      <c r="ZS26" s="11"/>
-      <c r="ZT26" s="11"/>
-      <c r="ZU26" s="11"/>
-      <c r="ZV26" s="11"/>
-      <c r="ZW26" s="11"/>
-      <c r="ZX26" s="11"/>
-      <c r="ZY26" s="11"/>
-      <c r="ZZ26" s="11"/>
-      <c r="AAA26" s="11"/>
-      <c r="AAB26" s="11"/>
-      <c r="AAC26" s="11"/>
-      <c r="AAD26" s="11"/>
-      <c r="AAE26" s="11"/>
-      <c r="AAF26" s="11"/>
-      <c r="AAG26" s="11"/>
-      <c r="AAH26" s="11"/>
-      <c r="AAI26" s="11"/>
-      <c r="AAJ26" s="11"/>
-      <c r="AAK26" s="11"/>
-      <c r="AAL26" s="11"/>
-      <c r="AAM26" s="11"/>
-      <c r="AAN26" s="11"/>
-      <c r="AAO26" s="11"/>
-      <c r="AAP26" s="11"/>
-      <c r="AAQ26" s="11"/>
-      <c r="AAR26" s="11"/>
-      <c r="AAS26" s="11"/>
-      <c r="AAT26" s="11"/>
-      <c r="AAU26" s="11"/>
-      <c r="AAV26" s="11"/>
-      <c r="AAW26" s="11"/>
-      <c r="AAX26" s="11"/>
-      <c r="AAY26" s="11"/>
-      <c r="AAZ26" s="11"/>
-      <c r="ABA26" s="11"/>
-      <c r="ABB26" s="11"/>
-      <c r="ABC26" s="11"/>
-      <c r="ABD26" s="11"/>
-      <c r="ABE26" s="11"/>
-      <c r="ABF26" s="11"/>
-      <c r="ABG26" s="11"/>
-      <c r="ABH26" s="11"/>
-      <c r="ABI26" s="11"/>
-      <c r="ABJ26" s="11"/>
-      <c r="ABK26" s="11"/>
-      <c r="ABL26" s="11"/>
-      <c r="ABM26" s="11"/>
-      <c r="ABN26" s="11"/>
-      <c r="ABO26" s="11"/>
-      <c r="ABP26" s="11"/>
-      <c r="ABQ26" s="11"/>
-      <c r="ABR26" s="11"/>
-      <c r="ABS26" s="11"/>
-      <c r="ABT26" s="11"/>
-      <c r="ABU26" s="11"/>
-      <c r="ABV26" s="11"/>
-      <c r="ABW26" s="11"/>
-      <c r="ABX26" s="11"/>
-      <c r="ABY26" s="11"/>
-      <c r="ABZ26" s="11"/>
-      <c r="ACA26" s="11"/>
-      <c r="ACB26" s="11"/>
-      <c r="ACC26" s="11"/>
-      <c r="ACD26" s="11"/>
-      <c r="ACE26" s="11"/>
-      <c r="ACF26" s="11"/>
-      <c r="ACG26" s="11"/>
-      <c r="ACH26" s="11"/>
-      <c r="ACI26" s="11"/>
-      <c r="ACJ26" s="11"/>
-      <c r="ACK26" s="11"/>
-      <c r="ACL26" s="11"/>
-      <c r="ACM26" s="11"/>
-      <c r="ACN26" s="11"/>
-      <c r="ACO26" s="11"/>
-      <c r="ACP26" s="11"/>
-      <c r="ACQ26" s="11"/>
-      <c r="ACR26" s="11"/>
-      <c r="ACS26" s="11"/>
-      <c r="ACT26" s="11"/>
-      <c r="ACU26" s="11"/>
-      <c r="ACV26" s="11"/>
-      <c r="ACW26" s="11"/>
-      <c r="ACX26" s="11"/>
-      <c r="ACY26" s="11"/>
-      <c r="ACZ26" s="11"/>
-      <c r="ADA26" s="11"/>
-      <c r="ADB26" s="11"/>
-      <c r="ADC26" s="11"/>
-      <c r="ADD26" s="11"/>
-      <c r="ADE26" s="11"/>
-      <c r="ADF26" s="11"/>
-      <c r="ADG26" s="11"/>
-      <c r="ADH26" s="11"/>
-      <c r="ADI26" s="11"/>
-      <c r="ADJ26" s="11"/>
-      <c r="ADK26" s="11"/>
-      <c r="ADL26" s="11"/>
-      <c r="ADM26" s="11"/>
-      <c r="ADN26" s="11"/>
-      <c r="ADO26" s="11"/>
-      <c r="ADP26" s="11"/>
-      <c r="ADQ26" s="11"/>
-      <c r="ADR26" s="11"/>
-      <c r="ADS26" s="11"/>
-      <c r="ADT26" s="11"/>
-      <c r="ADU26" s="11"/>
-      <c r="ADV26" s="11"/>
-      <c r="ADW26" s="11"/>
-      <c r="ADX26" s="11"/>
-      <c r="ADY26" s="11"/>
-      <c r="ADZ26" s="11"/>
-      <c r="AEA26" s="11"/>
-      <c r="AEB26" s="11"/>
-      <c r="AEC26" s="11"/>
-      <c r="AED26" s="11"/>
-      <c r="AEE26" s="11"/>
-      <c r="AEF26" s="11"/>
-      <c r="AEG26" s="11"/>
-      <c r="AEH26" s="11"/>
-      <c r="AEI26" s="11"/>
-      <c r="AEJ26" s="11"/>
-      <c r="AEK26" s="11"/>
-      <c r="AEL26" s="11"/>
-      <c r="AEM26" s="11"/>
-      <c r="AEN26" s="11"/>
-      <c r="AEO26" s="11"/>
-      <c r="AEP26" s="11"/>
-      <c r="AEQ26" s="11"/>
-      <c r="AER26" s="11"/>
-      <c r="AES26" s="11"/>
-      <c r="AET26" s="11"/>
-      <c r="AEU26" s="11"/>
-      <c r="AEV26" s="11"/>
-      <c r="AEW26" s="11"/>
-      <c r="AEX26" s="11"/>
-      <c r="AEY26" s="11"/>
-      <c r="AEZ26" s="11"/>
-      <c r="AFA26" s="11"/>
-      <c r="AFB26" s="11"/>
-      <c r="AFC26" s="11"/>
-      <c r="AFD26" s="11"/>
-      <c r="AFE26" s="11"/>
-      <c r="AFF26" s="11"/>
-      <c r="AFG26" s="11"/>
-      <c r="AFH26" s="11"/>
-      <c r="AFI26" s="11"/>
-      <c r="AFJ26" s="11"/>
-      <c r="AFK26" s="11"/>
-      <c r="AFL26" s="11"/>
-      <c r="AFM26" s="11"/>
-      <c r="AFN26" s="11"/>
-      <c r="AFO26" s="11"/>
-      <c r="AFP26" s="11"/>
-      <c r="AFQ26" s="11"/>
-      <c r="AFR26" s="11"/>
-      <c r="AFS26" s="11"/>
-      <c r="AFT26" s="11"/>
-      <c r="AFU26" s="11"/>
-      <c r="AFV26" s="11"/>
-      <c r="AFW26" s="11"/>
-      <c r="AFX26" s="11"/>
-      <c r="AFY26" s="11"/>
-      <c r="AFZ26" s="11"/>
-      <c r="AGA26" s="11"/>
-      <c r="AGB26" s="11"/>
-      <c r="AGC26" s="11"/>
-      <c r="AGD26" s="11"/>
-      <c r="AGE26" s="11"/>
-      <c r="AGF26" s="11"/>
-      <c r="AGG26" s="11"/>
-      <c r="AGH26" s="11"/>
-      <c r="AGI26" s="11"/>
-      <c r="AGJ26" s="11"/>
-      <c r="AGK26" s="11"/>
-      <c r="AGL26" s="11"/>
-      <c r="AGM26" s="11"/>
-      <c r="AGN26" s="11"/>
-      <c r="AGO26" s="11"/>
-      <c r="AGP26" s="11"/>
-      <c r="AGQ26" s="11"/>
-      <c r="AGR26" s="11"/>
-      <c r="AGS26" s="11"/>
-      <c r="AGT26" s="11"/>
-      <c r="AGU26" s="11"/>
-      <c r="AGV26" s="11"/>
-      <c r="AGW26" s="11"/>
-      <c r="AGX26" s="11"/>
-      <c r="AGY26" s="11"/>
-      <c r="AGZ26" s="11"/>
-      <c r="AHA26" s="11"/>
-      <c r="AHB26" s="11"/>
-      <c r="AHC26" s="11"/>
-      <c r="AHD26" s="11"/>
-      <c r="AHE26" s="11"/>
-      <c r="AHF26" s="11"/>
-      <c r="AHG26" s="11"/>
-      <c r="AHH26" s="11"/>
-      <c r="AHI26" s="11"/>
-      <c r="AHJ26" s="11"/>
-      <c r="AHK26" s="11"/>
-      <c r="AHL26" s="11"/>
-      <c r="AHM26" s="11"/>
-      <c r="AHN26" s="11"/>
-      <c r="AHO26" s="11"/>
-      <c r="AHP26" s="11"/>
-      <c r="AHQ26" s="11"/>
-      <c r="AHR26" s="11"/>
-      <c r="AHS26" s="11"/>
-      <c r="AHT26" s="11"/>
-      <c r="AHU26" s="11"/>
-      <c r="AHV26" s="11"/>
-      <c r="AHW26" s="11"/>
-      <c r="AHX26" s="11"/>
-      <c r="AHY26" s="11"/>
-      <c r="AHZ26" s="11"/>
-      <c r="AIA26" s="11"/>
-      <c r="AIB26" s="11"/>
-      <c r="AIC26" s="11"/>
-      <c r="AID26" s="11"/>
-      <c r="AIE26" s="11"/>
-      <c r="AIF26" s="11"/>
-      <c r="AIG26" s="11"/>
-      <c r="AIH26" s="11"/>
-      <c r="AII26" s="11"/>
-      <c r="AIJ26" s="11"/>
-      <c r="AIK26" s="11"/>
-      <c r="AIL26" s="11"/>
-      <c r="AIM26" s="11"/>
-      <c r="AIN26" s="11"/>
-      <c r="AIO26" s="11"/>
-      <c r="AIP26" s="11"/>
-      <c r="AIQ26" s="11"/>
-      <c r="AIR26" s="11"/>
-      <c r="AIS26" s="11"/>
-      <c r="AIT26" s="11"/>
-      <c r="AIU26" s="11"/>
-      <c r="AIV26" s="11"/>
-      <c r="AIW26" s="11"/>
-      <c r="AIX26" s="11"/>
-      <c r="AIY26" s="11"/>
-      <c r="AIZ26" s="11"/>
-      <c r="AJA26" s="11"/>
-      <c r="AJB26" s="11"/>
-      <c r="AJC26" s="11"/>
-      <c r="AJD26" s="11"/>
-      <c r="AJE26" s="11"/>
-      <c r="AJF26" s="11"/>
-      <c r="AJG26" s="11"/>
-      <c r="AJH26" s="11"/>
-      <c r="AJI26" s="11"/>
-      <c r="AJJ26" s="11"/>
-      <c r="AJK26" s="11"/>
-      <c r="AJL26" s="11"/>
-      <c r="AJM26" s="11"/>
-      <c r="AJN26" s="11"/>
-      <c r="AJO26" s="11"/>
-      <c r="AJP26" s="11"/>
-      <c r="AJQ26" s="11"/>
-      <c r="AJR26" s="11"/>
-      <c r="AJS26" s="11"/>
-      <c r="AJT26" s="11"/>
-      <c r="AJU26" s="11"/>
-      <c r="AJV26" s="11"/>
-      <c r="AJW26" s="11"/>
-      <c r="AJX26" s="11"/>
-      <c r="AJY26" s="11"/>
-      <c r="AJZ26" s="11"/>
-      <c r="AKA26" s="11"/>
-      <c r="AKB26" s="11"/>
-      <c r="AKC26" s="11"/>
-      <c r="AKD26" s="11"/>
-      <c r="AKE26" s="11"/>
-      <c r="AKF26" s="11"/>
-      <c r="AKG26" s="11"/>
-      <c r="AKH26" s="11"/>
-      <c r="AKI26" s="11"/>
-      <c r="AKJ26" s="11"/>
-      <c r="AKK26" s="11"/>
-      <c r="AKL26" s="11"/>
-      <c r="AKM26" s="11"/>
-      <c r="AKN26" s="11"/>
-      <c r="AKO26" s="11"/>
-      <c r="AKP26" s="11"/>
-      <c r="AKQ26" s="11"/>
-      <c r="AKR26" s="11"/>
-      <c r="AKS26" s="11"/>
-      <c r="AKT26" s="11"/>
-      <c r="AKU26" s="11"/>
-      <c r="AKV26" s="11"/>
-      <c r="AKW26" s="11"/>
-      <c r="AKX26" s="11"/>
-      <c r="AKY26" s="11"/>
-      <c r="AKZ26" s="11"/>
-      <c r="ALA26" s="11"/>
-      <c r="ALB26" s="11"/>
-      <c r="ALC26" s="11"/>
-      <c r="ALD26" s="11"/>
-      <c r="ALE26" s="11"/>
-      <c r="ALF26" s="11"/>
-      <c r="ALG26" s="11"/>
-      <c r="ALH26" s="11"/>
-      <c r="ALI26" s="11"/>
-      <c r="ALJ26" s="11"/>
-      <c r="ALK26" s="11"/>
-      <c r="ALL26" s="11"/>
-      <c r="ALM26" s="11"/>
-      <c r="ALN26" s="11"/>
-      <c r="ALO26" s="11"/>
-      <c r="ALP26" s="11"/>
-      <c r="ALQ26" s="11"/>
-      <c r="ALR26" s="11"/>
-      <c r="ALS26" s="11"/>
-      <c r="ALT26" s="11"/>
-      <c r="ALU26" s="11"/>
-      <c r="ALV26" s="11"/>
-      <c r="ALW26" s="11"/>
-      <c r="ALX26" s="11"/>
-      <c r="ALY26" s="11"/>
-      <c r="ALZ26" s="11"/>
-      <c r="AMA26" s="11"/>
-      <c r="AMB26" s="11"/>
-      <c r="AMC26" s="11"/>
-      <c r="AMD26" s="11"/>
-      <c r="AME26" s="11"/>
-      <c r="AMF26" s="11"/>
-      <c r="AMG26" s="11"/>
-      <c r="AMH26" s="11"/>
-      <c r="AMI26" s="11"/>
-      <c r="AMJ26" s="11"/>
-      <c r="AMK26" s="11"/>
-      <c r="AML26" s="11"/>
-    </row>
-    <row r="27" spans="1:1026" ht="29">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:1026" ht="30">
+      <c r="A28" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1026" ht="29">
-      <c r="A28" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>16</v>
@@ -9029,24 +9064,24 @@
         <v>0</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:1026">
+    <row r="29" spans="1:1026" ht="30">
       <c r="A29" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>16</v>
@@ -9061,16 +9096,19 @@
     </row>
     <row r="30" spans="1:1026">
       <c r="A30" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>16</v>
@@ -9080,24 +9118,21 @@
         <v>0</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:1026" ht="72.5">
+    <row r="31" spans="1:1026">
       <c r="A31" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>16</v>
@@ -9107,27 +9142,24 @@
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>361</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:1026" ht="29">
+    <row r="32" spans="1:1026" ht="75">
       <c r="A32" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>16</v>
@@ -9136,125 +9168,134 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="K32" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>361</v>
+      </c>
     </row>
-    <row r="33" spans="1:13" ht="29">
+    <row r="33" spans="1:13" ht="30">
       <c r="A33" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>348</v>
+        <v>150</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="30">
+      <c r="A34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K34" s="1">
         <v>990399123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E35"/>
+        <v>157</v>
+      </c>
       <c r="F35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G35" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="30">
+      <c r="A36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36"/>
+      <c r="F36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I36" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:13" ht="30">
+      <c r="A37" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="29">
-      <c r="A37" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>16</v>
@@ -9263,24 +9304,20 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>171</v>
-      </c>
     </row>
-    <row r="38" spans="1:13" ht="29">
+    <row r="38" spans="1:13" ht="30">
       <c r="A38" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>168</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E38"/>
+        <v>169</v>
+      </c>
       <c r="F38" s="1" t="s">
         <v>16</v>
       </c>
@@ -9288,43 +9325,44 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="K38" s="1" t="s">
+        <v>171</v>
+      </c>
     </row>
-    <row r="39" spans="1:13" ht="29">
+    <row r="39" spans="1:13" ht="30">
       <c r="A39" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>168</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>177</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="E39"/>
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>179</v>
+        <f>0</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" ht="30">
       <c r="A40" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>117</v>
+        <v>168</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>119</v>
+        <v>177</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -9334,77 +9372,74 @@
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="43.5">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:13" ht="45">
+      <c r="A42" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="G41" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E42"/>
-      <c r="F42" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="G42" s="2">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I42" s="3" t="s">
-        <v>190</v>
-      </c>
     </row>
-    <row r="43" spans="1:13" ht="29">
+    <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>178</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="E43"/>
       <c r="F43" s="1" t="s">
         <v>179</v>
       </c>
@@ -9412,65 +9447,73 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="I43" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" ht="30">
       <c r="A44" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="G44" s="2">
         <f>0</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="8" t="s">
-        <v>196</v>
+    <row r="45" spans="1:13" ht="30">
+      <c r="A45" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>198</v>
+        <v>54</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E45"/>
+        <v>182</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="F45" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G45" s="2">
-        <f>0</f>
-        <v>0</v>
+      <c r="G45" s="2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E46"/>
       <c r="F46" s="1" t="s">
@@ -9483,16 +9526,16 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E47"/>
       <c r="F47" s="1" t="s">
@@ -9505,16 +9548,16 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E48"/>
       <c r="F48" s="1" t="s">
@@ -9527,16 +9570,16 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>213</v>
+        <v>106</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E49"/>
       <c r="F49" s="1" t="s">
@@ -9549,16 +9592,16 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E50"/>
       <c r="F50" s="1" t="s">
@@ -9571,17 +9614,18 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="E51"/>
       <c r="F51" s="1" t="s">
         <v>153</v>
       </c>
@@ -9592,18 +9636,17 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="8" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E52"/>
+        <v>222</v>
+      </c>
       <c r="F52" s="1" t="s">
         <v>153</v>
       </c>
@@ -9614,16 +9657,16 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="8" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E53"/>
       <c r="F53" s="1" t="s">
@@ -9636,16 +9679,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="8" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>95</v>
+        <v>229</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E54"/>
       <c r="F54" s="1" t="s">
@@ -9657,17 +9700,17 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="9" t="s">
-        <v>234</v>
+      <c r="A55" s="8" t="s">
+        <v>231</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>236</v>
+        <v>95</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E55"/>
       <c r="F55" s="1" t="s">
@@ -9680,16 +9723,16 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="9" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E56"/>
       <c r="F56" s="1" t="s">
@@ -9702,16 +9745,16 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E57"/>
       <c r="F57" s="1" t="s">
@@ -9724,16 +9767,16 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E58"/>
       <c r="F58" s="1" t="s">
@@ -9746,16 +9789,16 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="9" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E59"/>
       <c r="F59" s="1" t="s">
@@ -9768,16 +9811,16 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="9" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>122</v>
+        <v>252</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E60"/>
       <c r="F60" s="1" t="s">
@@ -9790,16 +9833,16 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>259</v>
+        <v>122</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E61"/>
       <c r="F61" s="1" t="s">
@@ -9812,16 +9855,16 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E62"/>
       <c r="F62" s="1" t="s">
@@ -9834,16 +9877,16 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E63"/>
       <c r="F63" s="1" t="s">
@@ -9856,16 +9899,16 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E64"/>
       <c r="F64" s="1" t="s">
@@ -9876,18 +9919,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="29">
+    <row r="65" spans="1:13">
       <c r="A65" s="9" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E65"/>
       <c r="F65" s="1" t="s">
@@ -9898,18 +9941,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" ht="30">
       <c r="A66" s="9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E66"/>
       <c r="F66" s="1" t="s">
@@ -9922,16 +9965,16 @@
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="9" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>58</v>
+        <v>279</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E67"/>
       <c r="F67" s="1" t="s">
@@ -9944,16 +9987,16 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>286</v>
+        <v>58</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="1" t="s">
@@ -9966,16 +10009,16 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E69"/>
       <c r="F69" s="1" t="s">
@@ -9988,16 +10031,16 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="9" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E70"/>
       <c r="F70" s="1" t="s">
@@ -10010,16 +10053,16 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E71"/>
       <c r="F71" s="1" t="s">
@@ -10032,16 +10075,16 @@
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E72"/>
       <c r="F72" s="1" t="s">
@@ -10054,16 +10097,16 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="9" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E73"/>
       <c r="F73" s="1" t="s">
@@ -10076,17 +10119,18 @@
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="9" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>311</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="E74"/>
       <c r="F74" s="1" t="s">
         <v>153</v>
       </c>
@@ -10097,18 +10141,17 @@
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="9" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E75"/>
+        <v>311</v>
+      </c>
       <c r="F75" s="1" t="s">
         <v>153</v>
       </c>
@@ -10119,16 +10162,16 @@
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="9" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E76"/>
       <c r="F76" s="1" t="s">
@@ -10139,93 +10182,91 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
-      <c r="A77" s="1" t="s">
-        <v>320</v>
+    <row r="77" spans="1:13" ht="30">
+      <c r="A77" s="9" t="s">
+        <v>316</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>58</v>
+        <v>318</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>322</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="E77"/>
       <c r="F77" s="1" t="s">
-        <v>323</v>
+        <v>153</v>
       </c>
       <c r="G77" s="2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M77" s="1" t="s">
-        <v>324</v>
+        <f>0</f>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G78" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="A79" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F79" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="G78" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="29">
-      <c r="A79" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="G79" s="2">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I79" s="3" t="s">
-        <v>333</v>
-      </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" ht="30">
       <c r="A80" s="1" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>87</v>
@@ -10234,33 +10275,57 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="I80" s="3" t="s">
+        <v>333</v>
+      </c>
     </row>
-    <row r="81" spans="1:13" ht="29">
+    <row r="81" spans="1:13">
       <c r="A81" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>229</v>
+        <v>13</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G81" s="2">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="M81" s="1" t="s">
+    </row>
+    <row r="82" spans="1:13" ht="30">
+      <c r="A82" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G82" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="M82" s="1" t="s">
         <v>340</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M81">
+  <autoFilter ref="A1:M82">
     <filterColumn colId="11"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Resolved TICC-96 - added 0204
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$M$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$M$83</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="443">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1527,6 +1527,31 @@
   <si>
     <t>RegEx: [0-9a-zA-Z]{6}
 No checkdigit</t>
+  </si>
+  <si>
+    <t>DE:LWID</t>
+  </si>
+  <si>
+    <t>0204</t>
+  </si>
+  <si>
+    <t>Leitweg-ID</t>
+  </si>
+  <si>
+    <t>Koordinierungsstelle für IT-Standards (KoSIT)</t>
+  </si>
+  <si>
+    <t>Up to 44 alphanumeric characters
+Format: “Up to 12 numeric characters – up to 30 alphanumeric characters – 2 numeric characters”</t>
+  </si>
+  <si>
+    <t>Whole string</t>
+  </si>
+  <si>
+    <t>RegEx: [0-9]{0,12}(\-[0-9a-zA-Z]{0,30}(\-[0-9]{2}))</t>
+  </si>
+  <si>
+    <t>Each part is somehow optional</t>
   </si>
 </sst>
 </file>
@@ -1948,13 +1973,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AML82"/>
+  <dimension ref="A1:AML83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L26" sqref="L26"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -7991,1097 +8016,1107 @@
         <v>432</v>
       </c>
     </row>
-    <row r="27" spans="1:1026" s="14" customFormat="1" ht="30">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:1026" ht="45">
+      <c r="A27" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G27" s="2" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="K27" s="10"/>
+      <c r="L27" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1026" s="14" customFormat="1" ht="30">
+      <c r="A28" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C28" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D28" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G28" s="12">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="13" t="s">
+      <c r="H28" s="11"/>
+      <c r="I28" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="11" t="s">
+      <c r="K28" s="11"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
-      <c r="AD27" s="11"/>
-      <c r="AE27" s="11"/>
-      <c r="AF27" s="11"/>
-      <c r="AG27" s="11"/>
-      <c r="AH27" s="11"/>
-      <c r="AI27" s="11"/>
-      <c r="AJ27" s="11"/>
-      <c r="AK27" s="11"/>
-      <c r="AL27" s="11"/>
-      <c r="AM27" s="11"/>
-      <c r="AN27" s="11"/>
-      <c r="AO27" s="11"/>
-      <c r="AP27" s="11"/>
-      <c r="AQ27" s="11"/>
-      <c r="AR27" s="11"/>
-      <c r="AS27" s="11"/>
-      <c r="AT27" s="11"/>
-      <c r="AU27" s="11"/>
-      <c r="AV27" s="11"/>
-      <c r="AW27" s="11"/>
-      <c r="AX27" s="11"/>
-      <c r="AY27" s="11"/>
-      <c r="AZ27" s="11"/>
-      <c r="BA27" s="11"/>
-      <c r="BB27" s="11"/>
-      <c r="BC27" s="11"/>
-      <c r="BD27" s="11"/>
-      <c r="BE27" s="11"/>
-      <c r="BF27" s="11"/>
-      <c r="BG27" s="11"/>
-      <c r="BH27" s="11"/>
-      <c r="BI27" s="11"/>
-      <c r="BJ27" s="11"/>
-      <c r="BK27" s="11"/>
-      <c r="BL27" s="11"/>
-      <c r="BM27" s="11"/>
-      <c r="BN27" s="11"/>
-      <c r="BO27" s="11"/>
-      <c r="BP27" s="11"/>
-      <c r="BQ27" s="11"/>
-      <c r="BR27" s="11"/>
-      <c r="BS27" s="11"/>
-      <c r="BT27" s="11"/>
-      <c r="BU27" s="11"/>
-      <c r="BV27" s="11"/>
-      <c r="BW27" s="11"/>
-      <c r="BX27" s="11"/>
-      <c r="BY27" s="11"/>
-      <c r="BZ27" s="11"/>
-      <c r="CA27" s="11"/>
-      <c r="CB27" s="11"/>
-      <c r="CC27" s="11"/>
-      <c r="CD27" s="11"/>
-      <c r="CE27" s="11"/>
-      <c r="CF27" s="11"/>
-      <c r="CG27" s="11"/>
-      <c r="CH27" s="11"/>
-      <c r="CI27" s="11"/>
-      <c r="CJ27" s="11"/>
-      <c r="CK27" s="11"/>
-      <c r="CL27" s="11"/>
-      <c r="CM27" s="11"/>
-      <c r="CN27" s="11"/>
-      <c r="CO27" s="11"/>
-      <c r="CP27" s="11"/>
-      <c r="CQ27" s="11"/>
-      <c r="CR27" s="11"/>
-      <c r="CS27" s="11"/>
-      <c r="CT27" s="11"/>
-      <c r="CU27" s="11"/>
-      <c r="CV27" s="11"/>
-      <c r="CW27" s="11"/>
-      <c r="CX27" s="11"/>
-      <c r="CY27" s="11"/>
-      <c r="CZ27" s="11"/>
-      <c r="DA27" s="11"/>
-      <c r="DB27" s="11"/>
-      <c r="DC27" s="11"/>
-      <c r="DD27" s="11"/>
-      <c r="DE27" s="11"/>
-      <c r="DF27" s="11"/>
-      <c r="DG27" s="11"/>
-      <c r="DH27" s="11"/>
-      <c r="DI27" s="11"/>
-      <c r="DJ27" s="11"/>
-      <c r="DK27" s="11"/>
-      <c r="DL27" s="11"/>
-      <c r="DM27" s="11"/>
-      <c r="DN27" s="11"/>
-      <c r="DO27" s="11"/>
-      <c r="DP27" s="11"/>
-      <c r="DQ27" s="11"/>
-      <c r="DR27" s="11"/>
-      <c r="DS27" s="11"/>
-      <c r="DT27" s="11"/>
-      <c r="DU27" s="11"/>
-      <c r="DV27" s="11"/>
-      <c r="DW27" s="11"/>
-      <c r="DX27" s="11"/>
-      <c r="DY27" s="11"/>
-      <c r="DZ27" s="11"/>
-      <c r="EA27" s="11"/>
-      <c r="EB27" s="11"/>
-      <c r="EC27" s="11"/>
-      <c r="ED27" s="11"/>
-      <c r="EE27" s="11"/>
-      <c r="EF27" s="11"/>
-      <c r="EG27" s="11"/>
-      <c r="EH27" s="11"/>
-      <c r="EI27" s="11"/>
-      <c r="EJ27" s="11"/>
-      <c r="EK27" s="11"/>
-      <c r="EL27" s="11"/>
-      <c r="EM27" s="11"/>
-      <c r="EN27" s="11"/>
-      <c r="EO27" s="11"/>
-      <c r="EP27" s="11"/>
-      <c r="EQ27" s="11"/>
-      <c r="ER27" s="11"/>
-      <c r="ES27" s="11"/>
-      <c r="ET27" s="11"/>
-      <c r="EU27" s="11"/>
-      <c r="EV27" s="11"/>
-      <c r="EW27" s="11"/>
-      <c r="EX27" s="11"/>
-      <c r="EY27" s="11"/>
-      <c r="EZ27" s="11"/>
-      <c r="FA27" s="11"/>
-      <c r="FB27" s="11"/>
-      <c r="FC27" s="11"/>
-      <c r="FD27" s="11"/>
-      <c r="FE27" s="11"/>
-      <c r="FF27" s="11"/>
-      <c r="FG27" s="11"/>
-      <c r="FH27" s="11"/>
-      <c r="FI27" s="11"/>
-      <c r="FJ27" s="11"/>
-      <c r="FK27" s="11"/>
-      <c r="FL27" s="11"/>
-      <c r="FM27" s="11"/>
-      <c r="FN27" s="11"/>
-      <c r="FO27" s="11"/>
-      <c r="FP27" s="11"/>
-      <c r="FQ27" s="11"/>
-      <c r="FR27" s="11"/>
-      <c r="FS27" s="11"/>
-      <c r="FT27" s="11"/>
-      <c r="FU27" s="11"/>
-      <c r="FV27" s="11"/>
-      <c r="FW27" s="11"/>
-      <c r="FX27" s="11"/>
-      <c r="FY27" s="11"/>
-      <c r="FZ27" s="11"/>
-      <c r="GA27" s="11"/>
-      <c r="GB27" s="11"/>
-      <c r="GC27" s="11"/>
-      <c r="GD27" s="11"/>
-      <c r="GE27" s="11"/>
-      <c r="GF27" s="11"/>
-      <c r="GG27" s="11"/>
-      <c r="GH27" s="11"/>
-      <c r="GI27" s="11"/>
-      <c r="GJ27" s="11"/>
-      <c r="GK27" s="11"/>
-      <c r="GL27" s="11"/>
-      <c r="GM27" s="11"/>
-      <c r="GN27" s="11"/>
-      <c r="GO27" s="11"/>
-      <c r="GP27" s="11"/>
-      <c r="GQ27" s="11"/>
-      <c r="GR27" s="11"/>
-      <c r="GS27" s="11"/>
-      <c r="GT27" s="11"/>
-      <c r="GU27" s="11"/>
-      <c r="GV27" s="11"/>
-      <c r="GW27" s="11"/>
-      <c r="GX27" s="11"/>
-      <c r="GY27" s="11"/>
-      <c r="GZ27" s="11"/>
-      <c r="HA27" s="11"/>
-      <c r="HB27" s="11"/>
-      <c r="HC27" s="11"/>
-      <c r="HD27" s="11"/>
-      <c r="HE27" s="11"/>
-      <c r="HF27" s="11"/>
-      <c r="HG27" s="11"/>
-      <c r="HH27" s="11"/>
-      <c r="HI27" s="11"/>
-      <c r="HJ27" s="11"/>
-      <c r="HK27" s="11"/>
-      <c r="HL27" s="11"/>
-      <c r="HM27" s="11"/>
-      <c r="HN27" s="11"/>
-      <c r="HO27" s="11"/>
-      <c r="HP27" s="11"/>
-      <c r="HQ27" s="11"/>
-      <c r="HR27" s="11"/>
-      <c r="HS27" s="11"/>
-      <c r="HT27" s="11"/>
-      <c r="HU27" s="11"/>
-      <c r="HV27" s="11"/>
-      <c r="HW27" s="11"/>
-      <c r="HX27" s="11"/>
-      <c r="HY27" s="11"/>
-      <c r="HZ27" s="11"/>
-      <c r="IA27" s="11"/>
-      <c r="IB27" s="11"/>
-      <c r="IC27" s="11"/>
-      <c r="ID27" s="11"/>
-      <c r="IE27" s="11"/>
-      <c r="IF27" s="11"/>
-      <c r="IG27" s="11"/>
-      <c r="IH27" s="11"/>
-      <c r="II27" s="11"/>
-      <c r="IJ27" s="11"/>
-      <c r="IK27" s="11"/>
-      <c r="IL27" s="11"/>
-      <c r="IM27" s="11"/>
-      <c r="IN27" s="11"/>
-      <c r="IO27" s="11"/>
-      <c r="IP27" s="11"/>
-      <c r="IQ27" s="11"/>
-      <c r="IR27" s="11"/>
-      <c r="IS27" s="11"/>
-      <c r="IT27" s="11"/>
-      <c r="IU27" s="11"/>
-      <c r="IV27" s="11"/>
-      <c r="IW27" s="11"/>
-      <c r="IX27" s="11"/>
-      <c r="IY27" s="11"/>
-      <c r="IZ27" s="11"/>
-      <c r="JA27" s="11"/>
-      <c r="JB27" s="11"/>
-      <c r="JC27" s="11"/>
-      <c r="JD27" s="11"/>
-      <c r="JE27" s="11"/>
-      <c r="JF27" s="11"/>
-      <c r="JG27" s="11"/>
-      <c r="JH27" s="11"/>
-      <c r="JI27" s="11"/>
-      <c r="JJ27" s="11"/>
-      <c r="JK27" s="11"/>
-      <c r="JL27" s="11"/>
-      <c r="JM27" s="11"/>
-      <c r="JN27" s="11"/>
-      <c r="JO27" s="11"/>
-      <c r="JP27" s="11"/>
-      <c r="JQ27" s="11"/>
-      <c r="JR27" s="11"/>
-      <c r="JS27" s="11"/>
-      <c r="JT27" s="11"/>
-      <c r="JU27" s="11"/>
-      <c r="JV27" s="11"/>
-      <c r="JW27" s="11"/>
-      <c r="JX27" s="11"/>
-      <c r="JY27" s="11"/>
-      <c r="JZ27" s="11"/>
-      <c r="KA27" s="11"/>
-      <c r="KB27" s="11"/>
-      <c r="KC27" s="11"/>
-      <c r="KD27" s="11"/>
-      <c r="KE27" s="11"/>
-      <c r="KF27" s="11"/>
-      <c r="KG27" s="11"/>
-      <c r="KH27" s="11"/>
-      <c r="KI27" s="11"/>
-      <c r="KJ27" s="11"/>
-      <c r="KK27" s="11"/>
-      <c r="KL27" s="11"/>
-      <c r="KM27" s="11"/>
-      <c r="KN27" s="11"/>
-      <c r="KO27" s="11"/>
-      <c r="KP27" s="11"/>
-      <c r="KQ27" s="11"/>
-      <c r="KR27" s="11"/>
-      <c r="KS27" s="11"/>
-      <c r="KT27" s="11"/>
-      <c r="KU27" s="11"/>
-      <c r="KV27" s="11"/>
-      <c r="KW27" s="11"/>
-      <c r="KX27" s="11"/>
-      <c r="KY27" s="11"/>
-      <c r="KZ27" s="11"/>
-      <c r="LA27" s="11"/>
-      <c r="LB27" s="11"/>
-      <c r="LC27" s="11"/>
-      <c r="LD27" s="11"/>
-      <c r="LE27" s="11"/>
-      <c r="LF27" s="11"/>
-      <c r="LG27" s="11"/>
-      <c r="LH27" s="11"/>
-      <c r="LI27" s="11"/>
-      <c r="LJ27" s="11"/>
-      <c r="LK27" s="11"/>
-      <c r="LL27" s="11"/>
-      <c r="LM27" s="11"/>
-      <c r="LN27" s="11"/>
-      <c r="LO27" s="11"/>
-      <c r="LP27" s="11"/>
-      <c r="LQ27" s="11"/>
-      <c r="LR27" s="11"/>
-      <c r="LS27" s="11"/>
-      <c r="LT27" s="11"/>
-      <c r="LU27" s="11"/>
-      <c r="LV27" s="11"/>
-      <c r="LW27" s="11"/>
-      <c r="LX27" s="11"/>
-      <c r="LY27" s="11"/>
-      <c r="LZ27" s="11"/>
-      <c r="MA27" s="11"/>
-      <c r="MB27" s="11"/>
-      <c r="MC27" s="11"/>
-      <c r="MD27" s="11"/>
-      <c r="ME27" s="11"/>
-      <c r="MF27" s="11"/>
-      <c r="MG27" s="11"/>
-      <c r="MH27" s="11"/>
-      <c r="MI27" s="11"/>
-      <c r="MJ27" s="11"/>
-      <c r="MK27" s="11"/>
-      <c r="ML27" s="11"/>
-      <c r="MM27" s="11"/>
-      <c r="MN27" s="11"/>
-      <c r="MO27" s="11"/>
-      <c r="MP27" s="11"/>
-      <c r="MQ27" s="11"/>
-      <c r="MR27" s="11"/>
-      <c r="MS27" s="11"/>
-      <c r="MT27" s="11"/>
-      <c r="MU27" s="11"/>
-      <c r="MV27" s="11"/>
-      <c r="MW27" s="11"/>
-      <c r="MX27" s="11"/>
-      <c r="MY27" s="11"/>
-      <c r="MZ27" s="11"/>
-      <c r="NA27" s="11"/>
-      <c r="NB27" s="11"/>
-      <c r="NC27" s="11"/>
-      <c r="ND27" s="11"/>
-      <c r="NE27" s="11"/>
-      <c r="NF27" s="11"/>
-      <c r="NG27" s="11"/>
-      <c r="NH27" s="11"/>
-      <c r="NI27" s="11"/>
-      <c r="NJ27" s="11"/>
-      <c r="NK27" s="11"/>
-      <c r="NL27" s="11"/>
-      <c r="NM27" s="11"/>
-      <c r="NN27" s="11"/>
-      <c r="NO27" s="11"/>
-      <c r="NP27" s="11"/>
-      <c r="NQ27" s="11"/>
-      <c r="NR27" s="11"/>
-      <c r="NS27" s="11"/>
-      <c r="NT27" s="11"/>
-      <c r="NU27" s="11"/>
-      <c r="NV27" s="11"/>
-      <c r="NW27" s="11"/>
-      <c r="NX27" s="11"/>
-      <c r="NY27" s="11"/>
-      <c r="NZ27" s="11"/>
-      <c r="OA27" s="11"/>
-      <c r="OB27" s="11"/>
-      <c r="OC27" s="11"/>
-      <c r="OD27" s="11"/>
-      <c r="OE27" s="11"/>
-      <c r="OF27" s="11"/>
-      <c r="OG27" s="11"/>
-      <c r="OH27" s="11"/>
-      <c r="OI27" s="11"/>
-      <c r="OJ27" s="11"/>
-      <c r="OK27" s="11"/>
-      <c r="OL27" s="11"/>
-      <c r="OM27" s="11"/>
-      <c r="ON27" s="11"/>
-      <c r="OO27" s="11"/>
-      <c r="OP27" s="11"/>
-      <c r="OQ27" s="11"/>
-      <c r="OR27" s="11"/>
-      <c r="OS27" s="11"/>
-      <c r="OT27" s="11"/>
-      <c r="OU27" s="11"/>
-      <c r="OV27" s="11"/>
-      <c r="OW27" s="11"/>
-      <c r="OX27" s="11"/>
-      <c r="OY27" s="11"/>
-      <c r="OZ27" s="11"/>
-      <c r="PA27" s="11"/>
-      <c r="PB27" s="11"/>
-      <c r="PC27" s="11"/>
-      <c r="PD27" s="11"/>
-      <c r="PE27" s="11"/>
-      <c r="PF27" s="11"/>
-      <c r="PG27" s="11"/>
-      <c r="PH27" s="11"/>
-      <c r="PI27" s="11"/>
-      <c r="PJ27" s="11"/>
-      <c r="PK27" s="11"/>
-      <c r="PL27" s="11"/>
-      <c r="PM27" s="11"/>
-      <c r="PN27" s="11"/>
-      <c r="PO27" s="11"/>
-      <c r="PP27" s="11"/>
-      <c r="PQ27" s="11"/>
-      <c r="PR27" s="11"/>
-      <c r="PS27" s="11"/>
-      <c r="PT27" s="11"/>
-      <c r="PU27" s="11"/>
-      <c r="PV27" s="11"/>
-      <c r="PW27" s="11"/>
-      <c r="PX27" s="11"/>
-      <c r="PY27" s="11"/>
-      <c r="PZ27" s="11"/>
-      <c r="QA27" s="11"/>
-      <c r="QB27" s="11"/>
-      <c r="QC27" s="11"/>
-      <c r="QD27" s="11"/>
-      <c r="QE27" s="11"/>
-      <c r="QF27" s="11"/>
-      <c r="QG27" s="11"/>
-      <c r="QH27" s="11"/>
-      <c r="QI27" s="11"/>
-      <c r="QJ27" s="11"/>
-      <c r="QK27" s="11"/>
-      <c r="QL27" s="11"/>
-      <c r="QM27" s="11"/>
-      <c r="QN27" s="11"/>
-      <c r="QO27" s="11"/>
-      <c r="QP27" s="11"/>
-      <c r="QQ27" s="11"/>
-      <c r="QR27" s="11"/>
-      <c r="QS27" s="11"/>
-      <c r="QT27" s="11"/>
-      <c r="QU27" s="11"/>
-      <c r="QV27" s="11"/>
-      <c r="QW27" s="11"/>
-      <c r="QX27" s="11"/>
-      <c r="QY27" s="11"/>
-      <c r="QZ27" s="11"/>
-      <c r="RA27" s="11"/>
-      <c r="RB27" s="11"/>
-      <c r="RC27" s="11"/>
-      <c r="RD27" s="11"/>
-      <c r="RE27" s="11"/>
-      <c r="RF27" s="11"/>
-      <c r="RG27" s="11"/>
-      <c r="RH27" s="11"/>
-      <c r="RI27" s="11"/>
-      <c r="RJ27" s="11"/>
-      <c r="RK27" s="11"/>
-      <c r="RL27" s="11"/>
-      <c r="RM27" s="11"/>
-      <c r="RN27" s="11"/>
-      <c r="RO27" s="11"/>
-      <c r="RP27" s="11"/>
-      <c r="RQ27" s="11"/>
-      <c r="RR27" s="11"/>
-      <c r="RS27" s="11"/>
-      <c r="RT27" s="11"/>
-      <c r="RU27" s="11"/>
-      <c r="RV27" s="11"/>
-      <c r="RW27" s="11"/>
-      <c r="RX27" s="11"/>
-      <c r="RY27" s="11"/>
-      <c r="RZ27" s="11"/>
-      <c r="SA27" s="11"/>
-      <c r="SB27" s="11"/>
-      <c r="SC27" s="11"/>
-      <c r="SD27" s="11"/>
-      <c r="SE27" s="11"/>
-      <c r="SF27" s="11"/>
-      <c r="SG27" s="11"/>
-      <c r="SH27" s="11"/>
-      <c r="SI27" s="11"/>
-      <c r="SJ27" s="11"/>
-      <c r="SK27" s="11"/>
-      <c r="SL27" s="11"/>
-      <c r="SM27" s="11"/>
-      <c r="SN27" s="11"/>
-      <c r="SO27" s="11"/>
-      <c r="SP27" s="11"/>
-      <c r="SQ27" s="11"/>
-      <c r="SR27" s="11"/>
-      <c r="SS27" s="11"/>
-      <c r="ST27" s="11"/>
-      <c r="SU27" s="11"/>
-      <c r="SV27" s="11"/>
-      <c r="SW27" s="11"/>
-      <c r="SX27" s="11"/>
-      <c r="SY27" s="11"/>
-      <c r="SZ27" s="11"/>
-      <c r="TA27" s="11"/>
-      <c r="TB27" s="11"/>
-      <c r="TC27" s="11"/>
-      <c r="TD27" s="11"/>
-      <c r="TE27" s="11"/>
-      <c r="TF27" s="11"/>
-      <c r="TG27" s="11"/>
-      <c r="TH27" s="11"/>
-      <c r="TI27" s="11"/>
-      <c r="TJ27" s="11"/>
-      <c r="TK27" s="11"/>
-      <c r="TL27" s="11"/>
-      <c r="TM27" s="11"/>
-      <c r="TN27" s="11"/>
-      <c r="TO27" s="11"/>
-      <c r="TP27" s="11"/>
-      <c r="TQ27" s="11"/>
-      <c r="TR27" s="11"/>
-      <c r="TS27" s="11"/>
-      <c r="TT27" s="11"/>
-      <c r="TU27" s="11"/>
-      <c r="TV27" s="11"/>
-      <c r="TW27" s="11"/>
-      <c r="TX27" s="11"/>
-      <c r="TY27" s="11"/>
-      <c r="TZ27" s="11"/>
-      <c r="UA27" s="11"/>
-      <c r="UB27" s="11"/>
-      <c r="UC27" s="11"/>
-      <c r="UD27" s="11"/>
-      <c r="UE27" s="11"/>
-      <c r="UF27" s="11"/>
-      <c r="UG27" s="11"/>
-      <c r="UH27" s="11"/>
-      <c r="UI27" s="11"/>
-      <c r="UJ27" s="11"/>
-      <c r="UK27" s="11"/>
-      <c r="UL27" s="11"/>
-      <c r="UM27" s="11"/>
-      <c r="UN27" s="11"/>
-      <c r="UO27" s="11"/>
-      <c r="UP27" s="11"/>
-      <c r="UQ27" s="11"/>
-      <c r="UR27" s="11"/>
-      <c r="US27" s="11"/>
-      <c r="UT27" s="11"/>
-      <c r="UU27" s="11"/>
-      <c r="UV27" s="11"/>
-      <c r="UW27" s="11"/>
-      <c r="UX27" s="11"/>
-      <c r="UY27" s="11"/>
-      <c r="UZ27" s="11"/>
-      <c r="VA27" s="11"/>
-      <c r="VB27" s="11"/>
-      <c r="VC27" s="11"/>
-      <c r="VD27" s="11"/>
-      <c r="VE27" s="11"/>
-      <c r="VF27" s="11"/>
-      <c r="VG27" s="11"/>
-      <c r="VH27" s="11"/>
-      <c r="VI27" s="11"/>
-      <c r="VJ27" s="11"/>
-      <c r="VK27" s="11"/>
-      <c r="VL27" s="11"/>
-      <c r="VM27" s="11"/>
-      <c r="VN27" s="11"/>
-      <c r="VO27" s="11"/>
-      <c r="VP27" s="11"/>
-      <c r="VQ27" s="11"/>
-      <c r="VR27" s="11"/>
-      <c r="VS27" s="11"/>
-      <c r="VT27" s="11"/>
-      <c r="VU27" s="11"/>
-      <c r="VV27" s="11"/>
-      <c r="VW27" s="11"/>
-      <c r="VX27" s="11"/>
-      <c r="VY27" s="11"/>
-      <c r="VZ27" s="11"/>
-      <c r="WA27" s="11"/>
-      <c r="WB27" s="11"/>
-      <c r="WC27" s="11"/>
-      <c r="WD27" s="11"/>
-      <c r="WE27" s="11"/>
-      <c r="WF27" s="11"/>
-      <c r="WG27" s="11"/>
-      <c r="WH27" s="11"/>
-      <c r="WI27" s="11"/>
-      <c r="WJ27" s="11"/>
-      <c r="WK27" s="11"/>
-      <c r="WL27" s="11"/>
-      <c r="WM27" s="11"/>
-      <c r="WN27" s="11"/>
-      <c r="WO27" s="11"/>
-      <c r="WP27" s="11"/>
-      <c r="WQ27" s="11"/>
-      <c r="WR27" s="11"/>
-      <c r="WS27" s="11"/>
-      <c r="WT27" s="11"/>
-      <c r="WU27" s="11"/>
-      <c r="WV27" s="11"/>
-      <c r="WW27" s="11"/>
-      <c r="WX27" s="11"/>
-      <c r="WY27" s="11"/>
-      <c r="WZ27" s="11"/>
-      <c r="XA27" s="11"/>
-      <c r="XB27" s="11"/>
-      <c r="XC27" s="11"/>
-      <c r="XD27" s="11"/>
-      <c r="XE27" s="11"/>
-      <c r="XF27" s="11"/>
-      <c r="XG27" s="11"/>
-      <c r="XH27" s="11"/>
-      <c r="XI27" s="11"/>
-      <c r="XJ27" s="11"/>
-      <c r="XK27" s="11"/>
-      <c r="XL27" s="11"/>
-      <c r="XM27" s="11"/>
-      <c r="XN27" s="11"/>
-      <c r="XO27" s="11"/>
-      <c r="XP27" s="11"/>
-      <c r="XQ27" s="11"/>
-      <c r="XR27" s="11"/>
-      <c r="XS27" s="11"/>
-      <c r="XT27" s="11"/>
-      <c r="XU27" s="11"/>
-      <c r="XV27" s="11"/>
-      <c r="XW27" s="11"/>
-      <c r="XX27" s="11"/>
-      <c r="XY27" s="11"/>
-      <c r="XZ27" s="11"/>
-      <c r="YA27" s="11"/>
-      <c r="YB27" s="11"/>
-      <c r="YC27" s="11"/>
-      <c r="YD27" s="11"/>
-      <c r="YE27" s="11"/>
-      <c r="YF27" s="11"/>
-      <c r="YG27" s="11"/>
-      <c r="YH27" s="11"/>
-      <c r="YI27" s="11"/>
-      <c r="YJ27" s="11"/>
-      <c r="YK27" s="11"/>
-      <c r="YL27" s="11"/>
-      <c r="YM27" s="11"/>
-      <c r="YN27" s="11"/>
-      <c r="YO27" s="11"/>
-      <c r="YP27" s="11"/>
-      <c r="YQ27" s="11"/>
-      <c r="YR27" s="11"/>
-      <c r="YS27" s="11"/>
-      <c r="YT27" s="11"/>
-      <c r="YU27" s="11"/>
-      <c r="YV27" s="11"/>
-      <c r="YW27" s="11"/>
-      <c r="YX27" s="11"/>
-      <c r="YY27" s="11"/>
-      <c r="YZ27" s="11"/>
-      <c r="ZA27" s="11"/>
-      <c r="ZB27" s="11"/>
-      <c r="ZC27" s="11"/>
-      <c r="ZD27" s="11"/>
-      <c r="ZE27" s="11"/>
-      <c r="ZF27" s="11"/>
-      <c r="ZG27" s="11"/>
-      <c r="ZH27" s="11"/>
-      <c r="ZI27" s="11"/>
-      <c r="ZJ27" s="11"/>
-      <c r="ZK27" s="11"/>
-      <c r="ZL27" s="11"/>
-      <c r="ZM27" s="11"/>
-      <c r="ZN27" s="11"/>
-      <c r="ZO27" s="11"/>
-      <c r="ZP27" s="11"/>
-      <c r="ZQ27" s="11"/>
-      <c r="ZR27" s="11"/>
-      <c r="ZS27" s="11"/>
-      <c r="ZT27" s="11"/>
-      <c r="ZU27" s="11"/>
-      <c r="ZV27" s="11"/>
-      <c r="ZW27" s="11"/>
-      <c r="ZX27" s="11"/>
-      <c r="ZY27" s="11"/>
-      <c r="ZZ27" s="11"/>
-      <c r="AAA27" s="11"/>
-      <c r="AAB27" s="11"/>
-      <c r="AAC27" s="11"/>
-      <c r="AAD27" s="11"/>
-      <c r="AAE27" s="11"/>
-      <c r="AAF27" s="11"/>
-      <c r="AAG27" s="11"/>
-      <c r="AAH27" s="11"/>
-      <c r="AAI27" s="11"/>
-      <c r="AAJ27" s="11"/>
-      <c r="AAK27" s="11"/>
-      <c r="AAL27" s="11"/>
-      <c r="AAM27" s="11"/>
-      <c r="AAN27" s="11"/>
-      <c r="AAO27" s="11"/>
-      <c r="AAP27" s="11"/>
-      <c r="AAQ27" s="11"/>
-      <c r="AAR27" s="11"/>
-      <c r="AAS27" s="11"/>
-      <c r="AAT27" s="11"/>
-      <c r="AAU27" s="11"/>
-      <c r="AAV27" s="11"/>
-      <c r="AAW27" s="11"/>
-      <c r="AAX27" s="11"/>
-      <c r="AAY27" s="11"/>
-      <c r="AAZ27" s="11"/>
-      <c r="ABA27" s="11"/>
-      <c r="ABB27" s="11"/>
-      <c r="ABC27" s="11"/>
-      <c r="ABD27" s="11"/>
-      <c r="ABE27" s="11"/>
-      <c r="ABF27" s="11"/>
-      <c r="ABG27" s="11"/>
-      <c r="ABH27" s="11"/>
-      <c r="ABI27" s="11"/>
-      <c r="ABJ27" s="11"/>
-      <c r="ABK27" s="11"/>
-      <c r="ABL27" s="11"/>
-      <c r="ABM27" s="11"/>
-      <c r="ABN27" s="11"/>
-      <c r="ABO27" s="11"/>
-      <c r="ABP27" s="11"/>
-      <c r="ABQ27" s="11"/>
-      <c r="ABR27" s="11"/>
-      <c r="ABS27" s="11"/>
-      <c r="ABT27" s="11"/>
-      <c r="ABU27" s="11"/>
-      <c r="ABV27" s="11"/>
-      <c r="ABW27" s="11"/>
-      <c r="ABX27" s="11"/>
-      <c r="ABY27" s="11"/>
-      <c r="ABZ27" s="11"/>
-      <c r="ACA27" s="11"/>
-      <c r="ACB27" s="11"/>
-      <c r="ACC27" s="11"/>
-      <c r="ACD27" s="11"/>
-      <c r="ACE27" s="11"/>
-      <c r="ACF27" s="11"/>
-      <c r="ACG27" s="11"/>
-      <c r="ACH27" s="11"/>
-      <c r="ACI27" s="11"/>
-      <c r="ACJ27" s="11"/>
-      <c r="ACK27" s="11"/>
-      <c r="ACL27" s="11"/>
-      <c r="ACM27" s="11"/>
-      <c r="ACN27" s="11"/>
-      <c r="ACO27" s="11"/>
-      <c r="ACP27" s="11"/>
-      <c r="ACQ27" s="11"/>
-      <c r="ACR27" s="11"/>
-      <c r="ACS27" s="11"/>
-      <c r="ACT27" s="11"/>
-      <c r="ACU27" s="11"/>
-      <c r="ACV27" s="11"/>
-      <c r="ACW27" s="11"/>
-      <c r="ACX27" s="11"/>
-      <c r="ACY27" s="11"/>
-      <c r="ACZ27" s="11"/>
-      <c r="ADA27" s="11"/>
-      <c r="ADB27" s="11"/>
-      <c r="ADC27" s="11"/>
-      <c r="ADD27" s="11"/>
-      <c r="ADE27" s="11"/>
-      <c r="ADF27" s="11"/>
-      <c r="ADG27" s="11"/>
-      <c r="ADH27" s="11"/>
-      <c r="ADI27" s="11"/>
-      <c r="ADJ27" s="11"/>
-      <c r="ADK27" s="11"/>
-      <c r="ADL27" s="11"/>
-      <c r="ADM27" s="11"/>
-      <c r="ADN27" s="11"/>
-      <c r="ADO27" s="11"/>
-      <c r="ADP27" s="11"/>
-      <c r="ADQ27" s="11"/>
-      <c r="ADR27" s="11"/>
-      <c r="ADS27" s="11"/>
-      <c r="ADT27" s="11"/>
-      <c r="ADU27" s="11"/>
-      <c r="ADV27" s="11"/>
-      <c r="ADW27" s="11"/>
-      <c r="ADX27" s="11"/>
-      <c r="ADY27" s="11"/>
-      <c r="ADZ27" s="11"/>
-      <c r="AEA27" s="11"/>
-      <c r="AEB27" s="11"/>
-      <c r="AEC27" s="11"/>
-      <c r="AED27" s="11"/>
-      <c r="AEE27" s="11"/>
-      <c r="AEF27" s="11"/>
-      <c r="AEG27" s="11"/>
-      <c r="AEH27" s="11"/>
-      <c r="AEI27" s="11"/>
-      <c r="AEJ27" s="11"/>
-      <c r="AEK27" s="11"/>
-      <c r="AEL27" s="11"/>
-      <c r="AEM27" s="11"/>
-      <c r="AEN27" s="11"/>
-      <c r="AEO27" s="11"/>
-      <c r="AEP27" s="11"/>
-      <c r="AEQ27" s="11"/>
-      <c r="AER27" s="11"/>
-      <c r="AES27" s="11"/>
-      <c r="AET27" s="11"/>
-      <c r="AEU27" s="11"/>
-      <c r="AEV27" s="11"/>
-      <c r="AEW27" s="11"/>
-      <c r="AEX27" s="11"/>
-      <c r="AEY27" s="11"/>
-      <c r="AEZ27" s="11"/>
-      <c r="AFA27" s="11"/>
-      <c r="AFB27" s="11"/>
-      <c r="AFC27" s="11"/>
-      <c r="AFD27" s="11"/>
-      <c r="AFE27" s="11"/>
-      <c r="AFF27" s="11"/>
-      <c r="AFG27" s="11"/>
-      <c r="AFH27" s="11"/>
-      <c r="AFI27" s="11"/>
-      <c r="AFJ27" s="11"/>
-      <c r="AFK27" s="11"/>
-      <c r="AFL27" s="11"/>
-      <c r="AFM27" s="11"/>
-      <c r="AFN27" s="11"/>
-      <c r="AFO27" s="11"/>
-      <c r="AFP27" s="11"/>
-      <c r="AFQ27" s="11"/>
-      <c r="AFR27" s="11"/>
-      <c r="AFS27" s="11"/>
-      <c r="AFT27" s="11"/>
-      <c r="AFU27" s="11"/>
-      <c r="AFV27" s="11"/>
-      <c r="AFW27" s="11"/>
-      <c r="AFX27" s="11"/>
-      <c r="AFY27" s="11"/>
-      <c r="AFZ27" s="11"/>
-      <c r="AGA27" s="11"/>
-      <c r="AGB27" s="11"/>
-      <c r="AGC27" s="11"/>
-      <c r="AGD27" s="11"/>
-      <c r="AGE27" s="11"/>
-      <c r="AGF27" s="11"/>
-      <c r="AGG27" s="11"/>
-      <c r="AGH27" s="11"/>
-      <c r="AGI27" s="11"/>
-      <c r="AGJ27" s="11"/>
-      <c r="AGK27" s="11"/>
-      <c r="AGL27" s="11"/>
-      <c r="AGM27" s="11"/>
-      <c r="AGN27" s="11"/>
-      <c r="AGO27" s="11"/>
-      <c r="AGP27" s="11"/>
-      <c r="AGQ27" s="11"/>
-      <c r="AGR27" s="11"/>
-      <c r="AGS27" s="11"/>
-      <c r="AGT27" s="11"/>
-      <c r="AGU27" s="11"/>
-      <c r="AGV27" s="11"/>
-      <c r="AGW27" s="11"/>
-      <c r="AGX27" s="11"/>
-      <c r="AGY27" s="11"/>
-      <c r="AGZ27" s="11"/>
-      <c r="AHA27" s="11"/>
-      <c r="AHB27" s="11"/>
-      <c r="AHC27" s="11"/>
-      <c r="AHD27" s="11"/>
-      <c r="AHE27" s="11"/>
-      <c r="AHF27" s="11"/>
-      <c r="AHG27" s="11"/>
-      <c r="AHH27" s="11"/>
-      <c r="AHI27" s="11"/>
-      <c r="AHJ27" s="11"/>
-      <c r="AHK27" s="11"/>
-      <c r="AHL27" s="11"/>
-      <c r="AHM27" s="11"/>
-      <c r="AHN27" s="11"/>
-      <c r="AHO27" s="11"/>
-      <c r="AHP27" s="11"/>
-      <c r="AHQ27" s="11"/>
-      <c r="AHR27" s="11"/>
-      <c r="AHS27" s="11"/>
-      <c r="AHT27" s="11"/>
-      <c r="AHU27" s="11"/>
-      <c r="AHV27" s="11"/>
-      <c r="AHW27" s="11"/>
-      <c r="AHX27" s="11"/>
-      <c r="AHY27" s="11"/>
-      <c r="AHZ27" s="11"/>
-      <c r="AIA27" s="11"/>
-      <c r="AIB27" s="11"/>
-      <c r="AIC27" s="11"/>
-      <c r="AID27" s="11"/>
-      <c r="AIE27" s="11"/>
-      <c r="AIF27" s="11"/>
-      <c r="AIG27" s="11"/>
-      <c r="AIH27" s="11"/>
-      <c r="AII27" s="11"/>
-      <c r="AIJ27" s="11"/>
-      <c r="AIK27" s="11"/>
-      <c r="AIL27" s="11"/>
-      <c r="AIM27" s="11"/>
-      <c r="AIN27" s="11"/>
-      <c r="AIO27" s="11"/>
-      <c r="AIP27" s="11"/>
-      <c r="AIQ27" s="11"/>
-      <c r="AIR27" s="11"/>
-      <c r="AIS27" s="11"/>
-      <c r="AIT27" s="11"/>
-      <c r="AIU27" s="11"/>
-      <c r="AIV27" s="11"/>
-      <c r="AIW27" s="11"/>
-      <c r="AIX27" s="11"/>
-      <c r="AIY27" s="11"/>
-      <c r="AIZ27" s="11"/>
-      <c r="AJA27" s="11"/>
-      <c r="AJB27" s="11"/>
-      <c r="AJC27" s="11"/>
-      <c r="AJD27" s="11"/>
-      <c r="AJE27" s="11"/>
-      <c r="AJF27" s="11"/>
-      <c r="AJG27" s="11"/>
-      <c r="AJH27" s="11"/>
-      <c r="AJI27" s="11"/>
-      <c r="AJJ27" s="11"/>
-      <c r="AJK27" s="11"/>
-      <c r="AJL27" s="11"/>
-      <c r="AJM27" s="11"/>
-      <c r="AJN27" s="11"/>
-      <c r="AJO27" s="11"/>
-      <c r="AJP27" s="11"/>
-      <c r="AJQ27" s="11"/>
-      <c r="AJR27" s="11"/>
-      <c r="AJS27" s="11"/>
-      <c r="AJT27" s="11"/>
-      <c r="AJU27" s="11"/>
-      <c r="AJV27" s="11"/>
-      <c r="AJW27" s="11"/>
-      <c r="AJX27" s="11"/>
-      <c r="AJY27" s="11"/>
-      <c r="AJZ27" s="11"/>
-      <c r="AKA27" s="11"/>
-      <c r="AKB27" s="11"/>
-      <c r="AKC27" s="11"/>
-      <c r="AKD27" s="11"/>
-      <c r="AKE27" s="11"/>
-      <c r="AKF27" s="11"/>
-      <c r="AKG27" s="11"/>
-      <c r="AKH27" s="11"/>
-      <c r="AKI27" s="11"/>
-      <c r="AKJ27" s="11"/>
-      <c r="AKK27" s="11"/>
-      <c r="AKL27" s="11"/>
-      <c r="AKM27" s="11"/>
-      <c r="AKN27" s="11"/>
-      <c r="AKO27" s="11"/>
-      <c r="AKP27" s="11"/>
-      <c r="AKQ27" s="11"/>
-      <c r="AKR27" s="11"/>
-      <c r="AKS27" s="11"/>
-      <c r="AKT27" s="11"/>
-      <c r="AKU27" s="11"/>
-      <c r="AKV27" s="11"/>
-      <c r="AKW27" s="11"/>
-      <c r="AKX27" s="11"/>
-      <c r="AKY27" s="11"/>
-      <c r="AKZ27" s="11"/>
-      <c r="ALA27" s="11"/>
-      <c r="ALB27" s="11"/>
-      <c r="ALC27" s="11"/>
-      <c r="ALD27" s="11"/>
-      <c r="ALE27" s="11"/>
-      <c r="ALF27" s="11"/>
-      <c r="ALG27" s="11"/>
-      <c r="ALH27" s="11"/>
-      <c r="ALI27" s="11"/>
-      <c r="ALJ27" s="11"/>
-      <c r="ALK27" s="11"/>
-      <c r="ALL27" s="11"/>
-      <c r="ALM27" s="11"/>
-      <c r="ALN27" s="11"/>
-      <c r="ALO27" s="11"/>
-      <c r="ALP27" s="11"/>
-      <c r="ALQ27" s="11"/>
-      <c r="ALR27" s="11"/>
-      <c r="ALS27" s="11"/>
-      <c r="ALT27" s="11"/>
-      <c r="ALU27" s="11"/>
-      <c r="ALV27" s="11"/>
-      <c r="ALW27" s="11"/>
-      <c r="ALX27" s="11"/>
-      <c r="ALY27" s="11"/>
-      <c r="ALZ27" s="11"/>
-      <c r="AMA27" s="11"/>
-      <c r="AMB27" s="11"/>
-      <c r="AMC27" s="11"/>
-      <c r="AMD27" s="11"/>
-      <c r="AME27" s="11"/>
-      <c r="AMF27" s="11"/>
-      <c r="AMG27" s="11"/>
-      <c r="AMH27" s="11"/>
-      <c r="AMI27" s="11"/>
-      <c r="AMJ27" s="11"/>
-      <c r="AMK27" s="11"/>
-      <c r="AML27" s="11"/>
-    </row>
-    <row r="28" spans="1:1026" ht="30">
-      <c r="A28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="11"/>
+      <c r="AE28" s="11"/>
+      <c r="AF28" s="11"/>
+      <c r="AG28" s="11"/>
+      <c r="AH28" s="11"/>
+      <c r="AI28" s="11"/>
+      <c r="AJ28" s="11"/>
+      <c r="AK28" s="11"/>
+      <c r="AL28" s="11"/>
+      <c r="AM28" s="11"/>
+      <c r="AN28" s="11"/>
+      <c r="AO28" s="11"/>
+      <c r="AP28" s="11"/>
+      <c r="AQ28" s="11"/>
+      <c r="AR28" s="11"/>
+      <c r="AS28" s="11"/>
+      <c r="AT28" s="11"/>
+      <c r="AU28" s="11"/>
+      <c r="AV28" s="11"/>
+      <c r="AW28" s="11"/>
+      <c r="AX28" s="11"/>
+      <c r="AY28" s="11"/>
+      <c r="AZ28" s="11"/>
+      <c r="BA28" s="11"/>
+      <c r="BB28" s="11"/>
+      <c r="BC28" s="11"/>
+      <c r="BD28" s="11"/>
+      <c r="BE28" s="11"/>
+      <c r="BF28" s="11"/>
+      <c r="BG28" s="11"/>
+      <c r="BH28" s="11"/>
+      <c r="BI28" s="11"/>
+      <c r="BJ28" s="11"/>
+      <c r="BK28" s="11"/>
+      <c r="BL28" s="11"/>
+      <c r="BM28" s="11"/>
+      <c r="BN28" s="11"/>
+      <c r="BO28" s="11"/>
+      <c r="BP28" s="11"/>
+      <c r="BQ28" s="11"/>
+      <c r="BR28" s="11"/>
+      <c r="BS28" s="11"/>
+      <c r="BT28" s="11"/>
+      <c r="BU28" s="11"/>
+      <c r="BV28" s="11"/>
+      <c r="BW28" s="11"/>
+      <c r="BX28" s="11"/>
+      <c r="BY28" s="11"/>
+      <c r="BZ28" s="11"/>
+      <c r="CA28" s="11"/>
+      <c r="CB28" s="11"/>
+      <c r="CC28" s="11"/>
+      <c r="CD28" s="11"/>
+      <c r="CE28" s="11"/>
+      <c r="CF28" s="11"/>
+      <c r="CG28" s="11"/>
+      <c r="CH28" s="11"/>
+      <c r="CI28" s="11"/>
+      <c r="CJ28" s="11"/>
+      <c r="CK28" s="11"/>
+      <c r="CL28" s="11"/>
+      <c r="CM28" s="11"/>
+      <c r="CN28" s="11"/>
+      <c r="CO28" s="11"/>
+      <c r="CP28" s="11"/>
+      <c r="CQ28" s="11"/>
+      <c r="CR28" s="11"/>
+      <c r="CS28" s="11"/>
+      <c r="CT28" s="11"/>
+      <c r="CU28" s="11"/>
+      <c r="CV28" s="11"/>
+      <c r="CW28" s="11"/>
+      <c r="CX28" s="11"/>
+      <c r="CY28" s="11"/>
+      <c r="CZ28" s="11"/>
+      <c r="DA28" s="11"/>
+      <c r="DB28" s="11"/>
+      <c r="DC28" s="11"/>
+      <c r="DD28" s="11"/>
+      <c r="DE28" s="11"/>
+      <c r="DF28" s="11"/>
+      <c r="DG28" s="11"/>
+      <c r="DH28" s="11"/>
+      <c r="DI28" s="11"/>
+      <c r="DJ28" s="11"/>
+      <c r="DK28" s="11"/>
+      <c r="DL28" s="11"/>
+      <c r="DM28" s="11"/>
+      <c r="DN28" s="11"/>
+      <c r="DO28" s="11"/>
+      <c r="DP28" s="11"/>
+      <c r="DQ28" s="11"/>
+      <c r="DR28" s="11"/>
+      <c r="DS28" s="11"/>
+      <c r="DT28" s="11"/>
+      <c r="DU28" s="11"/>
+      <c r="DV28" s="11"/>
+      <c r="DW28" s="11"/>
+      <c r="DX28" s="11"/>
+      <c r="DY28" s="11"/>
+      <c r="DZ28" s="11"/>
+      <c r="EA28" s="11"/>
+      <c r="EB28" s="11"/>
+      <c r="EC28" s="11"/>
+      <c r="ED28" s="11"/>
+      <c r="EE28" s="11"/>
+      <c r="EF28" s="11"/>
+      <c r="EG28" s="11"/>
+      <c r="EH28" s="11"/>
+      <c r="EI28" s="11"/>
+      <c r="EJ28" s="11"/>
+      <c r="EK28" s="11"/>
+      <c r="EL28" s="11"/>
+      <c r="EM28" s="11"/>
+      <c r="EN28" s="11"/>
+      <c r="EO28" s="11"/>
+      <c r="EP28" s="11"/>
+      <c r="EQ28" s="11"/>
+      <c r="ER28" s="11"/>
+      <c r="ES28" s="11"/>
+      <c r="ET28" s="11"/>
+      <c r="EU28" s="11"/>
+      <c r="EV28" s="11"/>
+      <c r="EW28" s="11"/>
+      <c r="EX28" s="11"/>
+      <c r="EY28" s="11"/>
+      <c r="EZ28" s="11"/>
+      <c r="FA28" s="11"/>
+      <c r="FB28" s="11"/>
+      <c r="FC28" s="11"/>
+      <c r="FD28" s="11"/>
+      <c r="FE28" s="11"/>
+      <c r="FF28" s="11"/>
+      <c r="FG28" s="11"/>
+      <c r="FH28" s="11"/>
+      <c r="FI28" s="11"/>
+      <c r="FJ28" s="11"/>
+      <c r="FK28" s="11"/>
+      <c r="FL28" s="11"/>
+      <c r="FM28" s="11"/>
+      <c r="FN28" s="11"/>
+      <c r="FO28" s="11"/>
+      <c r="FP28" s="11"/>
+      <c r="FQ28" s="11"/>
+      <c r="FR28" s="11"/>
+      <c r="FS28" s="11"/>
+      <c r="FT28" s="11"/>
+      <c r="FU28" s="11"/>
+      <c r="FV28" s="11"/>
+      <c r="FW28" s="11"/>
+      <c r="FX28" s="11"/>
+      <c r="FY28" s="11"/>
+      <c r="FZ28" s="11"/>
+      <c r="GA28" s="11"/>
+      <c r="GB28" s="11"/>
+      <c r="GC28" s="11"/>
+      <c r="GD28" s="11"/>
+      <c r="GE28" s="11"/>
+      <c r="GF28" s="11"/>
+      <c r="GG28" s="11"/>
+      <c r="GH28" s="11"/>
+      <c r="GI28" s="11"/>
+      <c r="GJ28" s="11"/>
+      <c r="GK28" s="11"/>
+      <c r="GL28" s="11"/>
+      <c r="GM28" s="11"/>
+      <c r="GN28" s="11"/>
+      <c r="GO28" s="11"/>
+      <c r="GP28" s="11"/>
+      <c r="GQ28" s="11"/>
+      <c r="GR28" s="11"/>
+      <c r="GS28" s="11"/>
+      <c r="GT28" s="11"/>
+      <c r="GU28" s="11"/>
+      <c r="GV28" s="11"/>
+      <c r="GW28" s="11"/>
+      <c r="GX28" s="11"/>
+      <c r="GY28" s="11"/>
+      <c r="GZ28" s="11"/>
+      <c r="HA28" s="11"/>
+      <c r="HB28" s="11"/>
+      <c r="HC28" s="11"/>
+      <c r="HD28" s="11"/>
+      <c r="HE28" s="11"/>
+      <c r="HF28" s="11"/>
+      <c r="HG28" s="11"/>
+      <c r="HH28" s="11"/>
+      <c r="HI28" s="11"/>
+      <c r="HJ28" s="11"/>
+      <c r="HK28" s="11"/>
+      <c r="HL28" s="11"/>
+      <c r="HM28" s="11"/>
+      <c r="HN28" s="11"/>
+      <c r="HO28" s="11"/>
+      <c r="HP28" s="11"/>
+      <c r="HQ28" s="11"/>
+      <c r="HR28" s="11"/>
+      <c r="HS28" s="11"/>
+      <c r="HT28" s="11"/>
+      <c r="HU28" s="11"/>
+      <c r="HV28" s="11"/>
+      <c r="HW28" s="11"/>
+      <c r="HX28" s="11"/>
+      <c r="HY28" s="11"/>
+      <c r="HZ28" s="11"/>
+      <c r="IA28" s="11"/>
+      <c r="IB28" s="11"/>
+      <c r="IC28" s="11"/>
+      <c r="ID28" s="11"/>
+      <c r="IE28" s="11"/>
+      <c r="IF28" s="11"/>
+      <c r="IG28" s="11"/>
+      <c r="IH28" s="11"/>
+      <c r="II28" s="11"/>
+      <c r="IJ28" s="11"/>
+      <c r="IK28" s="11"/>
+      <c r="IL28" s="11"/>
+      <c r="IM28" s="11"/>
+      <c r="IN28" s="11"/>
+      <c r="IO28" s="11"/>
+      <c r="IP28" s="11"/>
+      <c r="IQ28" s="11"/>
+      <c r="IR28" s="11"/>
+      <c r="IS28" s="11"/>
+      <c r="IT28" s="11"/>
+      <c r="IU28" s="11"/>
+      <c r="IV28" s="11"/>
+      <c r="IW28" s="11"/>
+      <c r="IX28" s="11"/>
+      <c r="IY28" s="11"/>
+      <c r="IZ28" s="11"/>
+      <c r="JA28" s="11"/>
+      <c r="JB28" s="11"/>
+      <c r="JC28" s="11"/>
+      <c r="JD28" s="11"/>
+      <c r="JE28" s="11"/>
+      <c r="JF28" s="11"/>
+      <c r="JG28" s="11"/>
+      <c r="JH28" s="11"/>
+      <c r="JI28" s="11"/>
+      <c r="JJ28" s="11"/>
+      <c r="JK28" s="11"/>
+      <c r="JL28" s="11"/>
+      <c r="JM28" s="11"/>
+      <c r="JN28" s="11"/>
+      <c r="JO28" s="11"/>
+      <c r="JP28" s="11"/>
+      <c r="JQ28" s="11"/>
+      <c r="JR28" s="11"/>
+      <c r="JS28" s="11"/>
+      <c r="JT28" s="11"/>
+      <c r="JU28" s="11"/>
+      <c r="JV28" s="11"/>
+      <c r="JW28" s="11"/>
+      <c r="JX28" s="11"/>
+      <c r="JY28" s="11"/>
+      <c r="JZ28" s="11"/>
+      <c r="KA28" s="11"/>
+      <c r="KB28" s="11"/>
+      <c r="KC28" s="11"/>
+      <c r="KD28" s="11"/>
+      <c r="KE28" s="11"/>
+      <c r="KF28" s="11"/>
+      <c r="KG28" s="11"/>
+      <c r="KH28" s="11"/>
+      <c r="KI28" s="11"/>
+      <c r="KJ28" s="11"/>
+      <c r="KK28" s="11"/>
+      <c r="KL28" s="11"/>
+      <c r="KM28" s="11"/>
+      <c r="KN28" s="11"/>
+      <c r="KO28" s="11"/>
+      <c r="KP28" s="11"/>
+      <c r="KQ28" s="11"/>
+      <c r="KR28" s="11"/>
+      <c r="KS28" s="11"/>
+      <c r="KT28" s="11"/>
+      <c r="KU28" s="11"/>
+      <c r="KV28" s="11"/>
+      <c r="KW28" s="11"/>
+      <c r="KX28" s="11"/>
+      <c r="KY28" s="11"/>
+      <c r="KZ28" s="11"/>
+      <c r="LA28" s="11"/>
+      <c r="LB28" s="11"/>
+      <c r="LC28" s="11"/>
+      <c r="LD28" s="11"/>
+      <c r="LE28" s="11"/>
+      <c r="LF28" s="11"/>
+      <c r="LG28" s="11"/>
+      <c r="LH28" s="11"/>
+      <c r="LI28" s="11"/>
+      <c r="LJ28" s="11"/>
+      <c r="LK28" s="11"/>
+      <c r="LL28" s="11"/>
+      <c r="LM28" s="11"/>
+      <c r="LN28" s="11"/>
+      <c r="LO28" s="11"/>
+      <c r="LP28" s="11"/>
+      <c r="LQ28" s="11"/>
+      <c r="LR28" s="11"/>
+      <c r="LS28" s="11"/>
+      <c r="LT28" s="11"/>
+      <c r="LU28" s="11"/>
+      <c r="LV28" s="11"/>
+      <c r="LW28" s="11"/>
+      <c r="LX28" s="11"/>
+      <c r="LY28" s="11"/>
+      <c r="LZ28" s="11"/>
+      <c r="MA28" s="11"/>
+      <c r="MB28" s="11"/>
+      <c r="MC28" s="11"/>
+      <c r="MD28" s="11"/>
+      <c r="ME28" s="11"/>
+      <c r="MF28" s="11"/>
+      <c r="MG28" s="11"/>
+      <c r="MH28" s="11"/>
+      <c r="MI28" s="11"/>
+      <c r="MJ28" s="11"/>
+      <c r="MK28" s="11"/>
+      <c r="ML28" s="11"/>
+      <c r="MM28" s="11"/>
+      <c r="MN28" s="11"/>
+      <c r="MO28" s="11"/>
+      <c r="MP28" s="11"/>
+      <c r="MQ28" s="11"/>
+      <c r="MR28" s="11"/>
+      <c r="MS28" s="11"/>
+      <c r="MT28" s="11"/>
+      <c r="MU28" s="11"/>
+      <c r="MV28" s="11"/>
+      <c r="MW28" s="11"/>
+      <c r="MX28" s="11"/>
+      <c r="MY28" s="11"/>
+      <c r="MZ28" s="11"/>
+      <c r="NA28" s="11"/>
+      <c r="NB28" s="11"/>
+      <c r="NC28" s="11"/>
+      <c r="ND28" s="11"/>
+      <c r="NE28" s="11"/>
+      <c r="NF28" s="11"/>
+      <c r="NG28" s="11"/>
+      <c r="NH28" s="11"/>
+      <c r="NI28" s="11"/>
+      <c r="NJ28" s="11"/>
+      <c r="NK28" s="11"/>
+      <c r="NL28" s="11"/>
+      <c r="NM28" s="11"/>
+      <c r="NN28" s="11"/>
+      <c r="NO28" s="11"/>
+      <c r="NP28" s="11"/>
+      <c r="NQ28" s="11"/>
+      <c r="NR28" s="11"/>
+      <c r="NS28" s="11"/>
+      <c r="NT28" s="11"/>
+      <c r="NU28" s="11"/>
+      <c r="NV28" s="11"/>
+      <c r="NW28" s="11"/>
+      <c r="NX28" s="11"/>
+      <c r="NY28" s="11"/>
+      <c r="NZ28" s="11"/>
+      <c r="OA28" s="11"/>
+      <c r="OB28" s="11"/>
+      <c r="OC28" s="11"/>
+      <c r="OD28" s="11"/>
+      <c r="OE28" s="11"/>
+      <c r="OF28" s="11"/>
+      <c r="OG28" s="11"/>
+      <c r="OH28" s="11"/>
+      <c r="OI28" s="11"/>
+      <c r="OJ28" s="11"/>
+      <c r="OK28" s="11"/>
+      <c r="OL28" s="11"/>
+      <c r="OM28" s="11"/>
+      <c r="ON28" s="11"/>
+      <c r="OO28" s="11"/>
+      <c r="OP28" s="11"/>
+      <c r="OQ28" s="11"/>
+      <c r="OR28" s="11"/>
+      <c r="OS28" s="11"/>
+      <c r="OT28" s="11"/>
+      <c r="OU28" s="11"/>
+      <c r="OV28" s="11"/>
+      <c r="OW28" s="11"/>
+      <c r="OX28" s="11"/>
+      <c r="OY28" s="11"/>
+      <c r="OZ28" s="11"/>
+      <c r="PA28" s="11"/>
+      <c r="PB28" s="11"/>
+      <c r="PC28" s="11"/>
+      <c r="PD28" s="11"/>
+      <c r="PE28" s="11"/>
+      <c r="PF28" s="11"/>
+      <c r="PG28" s="11"/>
+      <c r="PH28" s="11"/>
+      <c r="PI28" s="11"/>
+      <c r="PJ28" s="11"/>
+      <c r="PK28" s="11"/>
+      <c r="PL28" s="11"/>
+      <c r="PM28" s="11"/>
+      <c r="PN28" s="11"/>
+      <c r="PO28" s="11"/>
+      <c r="PP28" s="11"/>
+      <c r="PQ28" s="11"/>
+      <c r="PR28" s="11"/>
+      <c r="PS28" s="11"/>
+      <c r="PT28" s="11"/>
+      <c r="PU28" s="11"/>
+      <c r="PV28" s="11"/>
+      <c r="PW28" s="11"/>
+      <c r="PX28" s="11"/>
+      <c r="PY28" s="11"/>
+      <c r="PZ28" s="11"/>
+      <c r="QA28" s="11"/>
+      <c r="QB28" s="11"/>
+      <c r="QC28" s="11"/>
+      <c r="QD28" s="11"/>
+      <c r="QE28" s="11"/>
+      <c r="QF28" s="11"/>
+      <c r="QG28" s="11"/>
+      <c r="QH28" s="11"/>
+      <c r="QI28" s="11"/>
+      <c r="QJ28" s="11"/>
+      <c r="QK28" s="11"/>
+      <c r="QL28" s="11"/>
+      <c r="QM28" s="11"/>
+      <c r="QN28" s="11"/>
+      <c r="QO28" s="11"/>
+      <c r="QP28" s="11"/>
+      <c r="QQ28" s="11"/>
+      <c r="QR28" s="11"/>
+      <c r="QS28" s="11"/>
+      <c r="QT28" s="11"/>
+      <c r="QU28" s="11"/>
+      <c r="QV28" s="11"/>
+      <c r="QW28" s="11"/>
+      <c r="QX28" s="11"/>
+      <c r="QY28" s="11"/>
+      <c r="QZ28" s="11"/>
+      <c r="RA28" s="11"/>
+      <c r="RB28" s="11"/>
+      <c r="RC28" s="11"/>
+      <c r="RD28" s="11"/>
+      <c r="RE28" s="11"/>
+      <c r="RF28" s="11"/>
+      <c r="RG28" s="11"/>
+      <c r="RH28" s="11"/>
+      <c r="RI28" s="11"/>
+      <c r="RJ28" s="11"/>
+      <c r="RK28" s="11"/>
+      <c r="RL28" s="11"/>
+      <c r="RM28" s="11"/>
+      <c r="RN28" s="11"/>
+      <c r="RO28" s="11"/>
+      <c r="RP28" s="11"/>
+      <c r="RQ28" s="11"/>
+      <c r="RR28" s="11"/>
+      <c r="RS28" s="11"/>
+      <c r="RT28" s="11"/>
+      <c r="RU28" s="11"/>
+      <c r="RV28" s="11"/>
+      <c r="RW28" s="11"/>
+      <c r="RX28" s="11"/>
+      <c r="RY28" s="11"/>
+      <c r="RZ28" s="11"/>
+      <c r="SA28" s="11"/>
+      <c r="SB28" s="11"/>
+      <c r="SC28" s="11"/>
+      <c r="SD28" s="11"/>
+      <c r="SE28" s="11"/>
+      <c r="SF28" s="11"/>
+      <c r="SG28" s="11"/>
+      <c r="SH28" s="11"/>
+      <c r="SI28" s="11"/>
+      <c r="SJ28" s="11"/>
+      <c r="SK28" s="11"/>
+      <c r="SL28" s="11"/>
+      <c r="SM28" s="11"/>
+      <c r="SN28" s="11"/>
+      <c r="SO28" s="11"/>
+      <c r="SP28" s="11"/>
+      <c r="SQ28" s="11"/>
+      <c r="SR28" s="11"/>
+      <c r="SS28" s="11"/>
+      <c r="ST28" s="11"/>
+      <c r="SU28" s="11"/>
+      <c r="SV28" s="11"/>
+      <c r="SW28" s="11"/>
+      <c r="SX28" s="11"/>
+      <c r="SY28" s="11"/>
+      <c r="SZ28" s="11"/>
+      <c r="TA28" s="11"/>
+      <c r="TB28" s="11"/>
+      <c r="TC28" s="11"/>
+      <c r="TD28" s="11"/>
+      <c r="TE28" s="11"/>
+      <c r="TF28" s="11"/>
+      <c r="TG28" s="11"/>
+      <c r="TH28" s="11"/>
+      <c r="TI28" s="11"/>
+      <c r="TJ28" s="11"/>
+      <c r="TK28" s="11"/>
+      <c r="TL28" s="11"/>
+      <c r="TM28" s="11"/>
+      <c r="TN28" s="11"/>
+      <c r="TO28" s="11"/>
+      <c r="TP28" s="11"/>
+      <c r="TQ28" s="11"/>
+      <c r="TR28" s="11"/>
+      <c r="TS28" s="11"/>
+      <c r="TT28" s="11"/>
+      <c r="TU28" s="11"/>
+      <c r="TV28" s="11"/>
+      <c r="TW28" s="11"/>
+      <c r="TX28" s="11"/>
+      <c r="TY28" s="11"/>
+      <c r="TZ28" s="11"/>
+      <c r="UA28" s="11"/>
+      <c r="UB28" s="11"/>
+      <c r="UC28" s="11"/>
+      <c r="UD28" s="11"/>
+      <c r="UE28" s="11"/>
+      <c r="UF28" s="11"/>
+      <c r="UG28" s="11"/>
+      <c r="UH28" s="11"/>
+      <c r="UI28" s="11"/>
+      <c r="UJ28" s="11"/>
+      <c r="UK28" s="11"/>
+      <c r="UL28" s="11"/>
+      <c r="UM28" s="11"/>
+      <c r="UN28" s="11"/>
+      <c r="UO28" s="11"/>
+      <c r="UP28" s="11"/>
+      <c r="UQ28" s="11"/>
+      <c r="UR28" s="11"/>
+      <c r="US28" s="11"/>
+      <c r="UT28" s="11"/>
+      <c r="UU28" s="11"/>
+      <c r="UV28" s="11"/>
+      <c r="UW28" s="11"/>
+      <c r="UX28" s="11"/>
+      <c r="UY28" s="11"/>
+      <c r="UZ28" s="11"/>
+      <c r="VA28" s="11"/>
+      <c r="VB28" s="11"/>
+      <c r="VC28" s="11"/>
+      <c r="VD28" s="11"/>
+      <c r="VE28" s="11"/>
+      <c r="VF28" s="11"/>
+      <c r="VG28" s="11"/>
+      <c r="VH28" s="11"/>
+      <c r="VI28" s="11"/>
+      <c r="VJ28" s="11"/>
+      <c r="VK28" s="11"/>
+      <c r="VL28" s="11"/>
+      <c r="VM28" s="11"/>
+      <c r="VN28" s="11"/>
+      <c r="VO28" s="11"/>
+      <c r="VP28" s="11"/>
+      <c r="VQ28" s="11"/>
+      <c r="VR28" s="11"/>
+      <c r="VS28" s="11"/>
+      <c r="VT28" s="11"/>
+      <c r="VU28" s="11"/>
+      <c r="VV28" s="11"/>
+      <c r="VW28" s="11"/>
+      <c r="VX28" s="11"/>
+      <c r="VY28" s="11"/>
+      <c r="VZ28" s="11"/>
+      <c r="WA28" s="11"/>
+      <c r="WB28" s="11"/>
+      <c r="WC28" s="11"/>
+      <c r="WD28" s="11"/>
+      <c r="WE28" s="11"/>
+      <c r="WF28" s="11"/>
+      <c r="WG28" s="11"/>
+      <c r="WH28" s="11"/>
+      <c r="WI28" s="11"/>
+      <c r="WJ28" s="11"/>
+      <c r="WK28" s="11"/>
+      <c r="WL28" s="11"/>
+      <c r="WM28" s="11"/>
+      <c r="WN28" s="11"/>
+      <c r="WO28" s="11"/>
+      <c r="WP28" s="11"/>
+      <c r="WQ28" s="11"/>
+      <c r="WR28" s="11"/>
+      <c r="WS28" s="11"/>
+      <c r="WT28" s="11"/>
+      <c r="WU28" s="11"/>
+      <c r="WV28" s="11"/>
+      <c r="WW28" s="11"/>
+      <c r="WX28" s="11"/>
+      <c r="WY28" s="11"/>
+      <c r="WZ28" s="11"/>
+      <c r="XA28" s="11"/>
+      <c r="XB28" s="11"/>
+      <c r="XC28" s="11"/>
+      <c r="XD28" s="11"/>
+      <c r="XE28" s="11"/>
+      <c r="XF28" s="11"/>
+      <c r="XG28" s="11"/>
+      <c r="XH28" s="11"/>
+      <c r="XI28" s="11"/>
+      <c r="XJ28" s="11"/>
+      <c r="XK28" s="11"/>
+      <c r="XL28" s="11"/>
+      <c r="XM28" s="11"/>
+      <c r="XN28" s="11"/>
+      <c r="XO28" s="11"/>
+      <c r="XP28" s="11"/>
+      <c r="XQ28" s="11"/>
+      <c r="XR28" s="11"/>
+      <c r="XS28" s="11"/>
+      <c r="XT28" s="11"/>
+      <c r="XU28" s="11"/>
+      <c r="XV28" s="11"/>
+      <c r="XW28" s="11"/>
+      <c r="XX28" s="11"/>
+      <c r="XY28" s="11"/>
+      <c r="XZ28" s="11"/>
+      <c r="YA28" s="11"/>
+      <c r="YB28" s="11"/>
+      <c r="YC28" s="11"/>
+      <c r="YD28" s="11"/>
+      <c r="YE28" s="11"/>
+      <c r="YF28" s="11"/>
+      <c r="YG28" s="11"/>
+      <c r="YH28" s="11"/>
+      <c r="YI28" s="11"/>
+      <c r="YJ28" s="11"/>
+      <c r="YK28" s="11"/>
+      <c r="YL28" s="11"/>
+      <c r="YM28" s="11"/>
+      <c r="YN28" s="11"/>
+      <c r="YO28" s="11"/>
+      <c r="YP28" s="11"/>
+      <c r="YQ28" s="11"/>
+      <c r="YR28" s="11"/>
+      <c r="YS28" s="11"/>
+      <c r="YT28" s="11"/>
+      <c r="YU28" s="11"/>
+      <c r="YV28" s="11"/>
+      <c r="YW28" s="11"/>
+      <c r="YX28" s="11"/>
+      <c r="YY28" s="11"/>
+      <c r="YZ28" s="11"/>
+      <c r="ZA28" s="11"/>
+      <c r="ZB28" s="11"/>
+      <c r="ZC28" s="11"/>
+      <c r="ZD28" s="11"/>
+      <c r="ZE28" s="11"/>
+      <c r="ZF28" s="11"/>
+      <c r="ZG28" s="11"/>
+      <c r="ZH28" s="11"/>
+      <c r="ZI28" s="11"/>
+      <c r="ZJ28" s="11"/>
+      <c r="ZK28" s="11"/>
+      <c r="ZL28" s="11"/>
+      <c r="ZM28" s="11"/>
+      <c r="ZN28" s="11"/>
+      <c r="ZO28" s="11"/>
+      <c r="ZP28" s="11"/>
+      <c r="ZQ28" s="11"/>
+      <c r="ZR28" s="11"/>
+      <c r="ZS28" s="11"/>
+      <c r="ZT28" s="11"/>
+      <c r="ZU28" s="11"/>
+      <c r="ZV28" s="11"/>
+      <c r="ZW28" s="11"/>
+      <c r="ZX28" s="11"/>
+      <c r="ZY28" s="11"/>
+      <c r="ZZ28" s="11"/>
+      <c r="AAA28" s="11"/>
+      <c r="AAB28" s="11"/>
+      <c r="AAC28" s="11"/>
+      <c r="AAD28" s="11"/>
+      <c r="AAE28" s="11"/>
+      <c r="AAF28" s="11"/>
+      <c r="AAG28" s="11"/>
+      <c r="AAH28" s="11"/>
+      <c r="AAI28" s="11"/>
+      <c r="AAJ28" s="11"/>
+      <c r="AAK28" s="11"/>
+      <c r="AAL28" s="11"/>
+      <c r="AAM28" s="11"/>
+      <c r="AAN28" s="11"/>
+      <c r="AAO28" s="11"/>
+      <c r="AAP28" s="11"/>
+      <c r="AAQ28" s="11"/>
+      <c r="AAR28" s="11"/>
+      <c r="AAS28" s="11"/>
+      <c r="AAT28" s="11"/>
+      <c r="AAU28" s="11"/>
+      <c r="AAV28" s="11"/>
+      <c r="AAW28" s="11"/>
+      <c r="AAX28" s="11"/>
+      <c r="AAY28" s="11"/>
+      <c r="AAZ28" s="11"/>
+      <c r="ABA28" s="11"/>
+      <c r="ABB28" s="11"/>
+      <c r="ABC28" s="11"/>
+      <c r="ABD28" s="11"/>
+      <c r="ABE28" s="11"/>
+      <c r="ABF28" s="11"/>
+      <c r="ABG28" s="11"/>
+      <c r="ABH28" s="11"/>
+      <c r="ABI28" s="11"/>
+      <c r="ABJ28" s="11"/>
+      <c r="ABK28" s="11"/>
+      <c r="ABL28" s="11"/>
+      <c r="ABM28" s="11"/>
+      <c r="ABN28" s="11"/>
+      <c r="ABO28" s="11"/>
+      <c r="ABP28" s="11"/>
+      <c r="ABQ28" s="11"/>
+      <c r="ABR28" s="11"/>
+      <c r="ABS28" s="11"/>
+      <c r="ABT28" s="11"/>
+      <c r="ABU28" s="11"/>
+      <c r="ABV28" s="11"/>
+      <c r="ABW28" s="11"/>
+      <c r="ABX28" s="11"/>
+      <c r="ABY28" s="11"/>
+      <c r="ABZ28" s="11"/>
+      <c r="ACA28" s="11"/>
+      <c r="ACB28" s="11"/>
+      <c r="ACC28" s="11"/>
+      <c r="ACD28" s="11"/>
+      <c r="ACE28" s="11"/>
+      <c r="ACF28" s="11"/>
+      <c r="ACG28" s="11"/>
+      <c r="ACH28" s="11"/>
+      <c r="ACI28" s="11"/>
+      <c r="ACJ28" s="11"/>
+      <c r="ACK28" s="11"/>
+      <c r="ACL28" s="11"/>
+      <c r="ACM28" s="11"/>
+      <c r="ACN28" s="11"/>
+      <c r="ACO28" s="11"/>
+      <c r="ACP28" s="11"/>
+      <c r="ACQ28" s="11"/>
+      <c r="ACR28" s="11"/>
+      <c r="ACS28" s="11"/>
+      <c r="ACT28" s="11"/>
+      <c r="ACU28" s="11"/>
+      <c r="ACV28" s="11"/>
+      <c r="ACW28" s="11"/>
+      <c r="ACX28" s="11"/>
+      <c r="ACY28" s="11"/>
+      <c r="ACZ28" s="11"/>
+      <c r="ADA28" s="11"/>
+      <c r="ADB28" s="11"/>
+      <c r="ADC28" s="11"/>
+      <c r="ADD28" s="11"/>
+      <c r="ADE28" s="11"/>
+      <c r="ADF28" s="11"/>
+      <c r="ADG28" s="11"/>
+      <c r="ADH28" s="11"/>
+      <c r="ADI28" s="11"/>
+      <c r="ADJ28" s="11"/>
+      <c r="ADK28" s="11"/>
+      <c r="ADL28" s="11"/>
+      <c r="ADM28" s="11"/>
+      <c r="ADN28" s="11"/>
+      <c r="ADO28" s="11"/>
+      <c r="ADP28" s="11"/>
+      <c r="ADQ28" s="11"/>
+      <c r="ADR28" s="11"/>
+      <c r="ADS28" s="11"/>
+      <c r="ADT28" s="11"/>
+      <c r="ADU28" s="11"/>
+      <c r="ADV28" s="11"/>
+      <c r="ADW28" s="11"/>
+      <c r="ADX28" s="11"/>
+      <c r="ADY28" s="11"/>
+      <c r="ADZ28" s="11"/>
+      <c r="AEA28" s="11"/>
+      <c r="AEB28" s="11"/>
+      <c r="AEC28" s="11"/>
+      <c r="AED28" s="11"/>
+      <c r="AEE28" s="11"/>
+      <c r="AEF28" s="11"/>
+      <c r="AEG28" s="11"/>
+      <c r="AEH28" s="11"/>
+      <c r="AEI28" s="11"/>
+      <c r="AEJ28" s="11"/>
+      <c r="AEK28" s="11"/>
+      <c r="AEL28" s="11"/>
+      <c r="AEM28" s="11"/>
+      <c r="AEN28" s="11"/>
+      <c r="AEO28" s="11"/>
+      <c r="AEP28" s="11"/>
+      <c r="AEQ28" s="11"/>
+      <c r="AER28" s="11"/>
+      <c r="AES28" s="11"/>
+      <c r="AET28" s="11"/>
+      <c r="AEU28" s="11"/>
+      <c r="AEV28" s="11"/>
+      <c r="AEW28" s="11"/>
+      <c r="AEX28" s="11"/>
+      <c r="AEY28" s="11"/>
+      <c r="AEZ28" s="11"/>
+      <c r="AFA28" s="11"/>
+      <c r="AFB28" s="11"/>
+      <c r="AFC28" s="11"/>
+      <c r="AFD28" s="11"/>
+      <c r="AFE28" s="11"/>
+      <c r="AFF28" s="11"/>
+      <c r="AFG28" s="11"/>
+      <c r="AFH28" s="11"/>
+      <c r="AFI28" s="11"/>
+      <c r="AFJ28" s="11"/>
+      <c r="AFK28" s="11"/>
+      <c r="AFL28" s="11"/>
+      <c r="AFM28" s="11"/>
+      <c r="AFN28" s="11"/>
+      <c r="AFO28" s="11"/>
+      <c r="AFP28" s="11"/>
+      <c r="AFQ28" s="11"/>
+      <c r="AFR28" s="11"/>
+      <c r="AFS28" s="11"/>
+      <c r="AFT28" s="11"/>
+      <c r="AFU28" s="11"/>
+      <c r="AFV28" s="11"/>
+      <c r="AFW28" s="11"/>
+      <c r="AFX28" s="11"/>
+      <c r="AFY28" s="11"/>
+      <c r="AFZ28" s="11"/>
+      <c r="AGA28" s="11"/>
+      <c r="AGB28" s="11"/>
+      <c r="AGC28" s="11"/>
+      <c r="AGD28" s="11"/>
+      <c r="AGE28" s="11"/>
+      <c r="AGF28" s="11"/>
+      <c r="AGG28" s="11"/>
+      <c r="AGH28" s="11"/>
+      <c r="AGI28" s="11"/>
+      <c r="AGJ28" s="11"/>
+      <c r="AGK28" s="11"/>
+      <c r="AGL28" s="11"/>
+      <c r="AGM28" s="11"/>
+      <c r="AGN28" s="11"/>
+      <c r="AGO28" s="11"/>
+      <c r="AGP28" s="11"/>
+      <c r="AGQ28" s="11"/>
+      <c r="AGR28" s="11"/>
+      <c r="AGS28" s="11"/>
+      <c r="AGT28" s="11"/>
+      <c r="AGU28" s="11"/>
+      <c r="AGV28" s="11"/>
+      <c r="AGW28" s="11"/>
+      <c r="AGX28" s="11"/>
+      <c r="AGY28" s="11"/>
+      <c r="AGZ28" s="11"/>
+      <c r="AHA28" s="11"/>
+      <c r="AHB28" s="11"/>
+      <c r="AHC28" s="11"/>
+      <c r="AHD28" s="11"/>
+      <c r="AHE28" s="11"/>
+      <c r="AHF28" s="11"/>
+      <c r="AHG28" s="11"/>
+      <c r="AHH28" s="11"/>
+      <c r="AHI28" s="11"/>
+      <c r="AHJ28" s="11"/>
+      <c r="AHK28" s="11"/>
+      <c r="AHL28" s="11"/>
+      <c r="AHM28" s="11"/>
+      <c r="AHN28" s="11"/>
+      <c r="AHO28" s="11"/>
+      <c r="AHP28" s="11"/>
+      <c r="AHQ28" s="11"/>
+      <c r="AHR28" s="11"/>
+      <c r="AHS28" s="11"/>
+      <c r="AHT28" s="11"/>
+      <c r="AHU28" s="11"/>
+      <c r="AHV28" s="11"/>
+      <c r="AHW28" s="11"/>
+      <c r="AHX28" s="11"/>
+      <c r="AHY28" s="11"/>
+      <c r="AHZ28" s="11"/>
+      <c r="AIA28" s="11"/>
+      <c r="AIB28" s="11"/>
+      <c r="AIC28" s="11"/>
+      <c r="AID28" s="11"/>
+      <c r="AIE28" s="11"/>
+      <c r="AIF28" s="11"/>
+      <c r="AIG28" s="11"/>
+      <c r="AIH28" s="11"/>
+      <c r="AII28" s="11"/>
+      <c r="AIJ28" s="11"/>
+      <c r="AIK28" s="11"/>
+      <c r="AIL28" s="11"/>
+      <c r="AIM28" s="11"/>
+      <c r="AIN28" s="11"/>
+      <c r="AIO28" s="11"/>
+      <c r="AIP28" s="11"/>
+      <c r="AIQ28" s="11"/>
+      <c r="AIR28" s="11"/>
+      <c r="AIS28" s="11"/>
+      <c r="AIT28" s="11"/>
+      <c r="AIU28" s="11"/>
+      <c r="AIV28" s="11"/>
+      <c r="AIW28" s="11"/>
+      <c r="AIX28" s="11"/>
+      <c r="AIY28" s="11"/>
+      <c r="AIZ28" s="11"/>
+      <c r="AJA28" s="11"/>
+      <c r="AJB28" s="11"/>
+      <c r="AJC28" s="11"/>
+      <c r="AJD28" s="11"/>
+      <c r="AJE28" s="11"/>
+      <c r="AJF28" s="11"/>
+      <c r="AJG28" s="11"/>
+      <c r="AJH28" s="11"/>
+      <c r="AJI28" s="11"/>
+      <c r="AJJ28" s="11"/>
+      <c r="AJK28" s="11"/>
+      <c r="AJL28" s="11"/>
+      <c r="AJM28" s="11"/>
+      <c r="AJN28" s="11"/>
+      <c r="AJO28" s="11"/>
+      <c r="AJP28" s="11"/>
+      <c r="AJQ28" s="11"/>
+      <c r="AJR28" s="11"/>
+      <c r="AJS28" s="11"/>
+      <c r="AJT28" s="11"/>
+      <c r="AJU28" s="11"/>
+      <c r="AJV28" s="11"/>
+      <c r="AJW28" s="11"/>
+      <c r="AJX28" s="11"/>
+      <c r="AJY28" s="11"/>
+      <c r="AJZ28" s="11"/>
+      <c r="AKA28" s="11"/>
+      <c r="AKB28" s="11"/>
+      <c r="AKC28" s="11"/>
+      <c r="AKD28" s="11"/>
+      <c r="AKE28" s="11"/>
+      <c r="AKF28" s="11"/>
+      <c r="AKG28" s="11"/>
+      <c r="AKH28" s="11"/>
+      <c r="AKI28" s="11"/>
+      <c r="AKJ28" s="11"/>
+      <c r="AKK28" s="11"/>
+      <c r="AKL28" s="11"/>
+      <c r="AKM28" s="11"/>
+      <c r="AKN28" s="11"/>
+      <c r="AKO28" s="11"/>
+      <c r="AKP28" s="11"/>
+      <c r="AKQ28" s="11"/>
+      <c r="AKR28" s="11"/>
+      <c r="AKS28" s="11"/>
+      <c r="AKT28" s="11"/>
+      <c r="AKU28" s="11"/>
+      <c r="AKV28" s="11"/>
+      <c r="AKW28" s="11"/>
+      <c r="AKX28" s="11"/>
+      <c r="AKY28" s="11"/>
+      <c r="AKZ28" s="11"/>
+      <c r="ALA28" s="11"/>
+      <c r="ALB28" s="11"/>
+      <c r="ALC28" s="11"/>
+      <c r="ALD28" s="11"/>
+      <c r="ALE28" s="11"/>
+      <c r="ALF28" s="11"/>
+      <c r="ALG28" s="11"/>
+      <c r="ALH28" s="11"/>
+      <c r="ALI28" s="11"/>
+      <c r="ALJ28" s="11"/>
+      <c r="ALK28" s="11"/>
+      <c r="ALL28" s="11"/>
+      <c r="ALM28" s="11"/>
+      <c r="ALN28" s="11"/>
+      <c r="ALO28" s="11"/>
+      <c r="ALP28" s="11"/>
+      <c r="ALQ28" s="11"/>
+      <c r="ALR28" s="11"/>
+      <c r="ALS28" s="11"/>
+      <c r="ALT28" s="11"/>
+      <c r="ALU28" s="11"/>
+      <c r="ALV28" s="11"/>
+      <c r="ALW28" s="11"/>
+      <c r="ALX28" s="11"/>
+      <c r="ALY28" s="11"/>
+      <c r="ALZ28" s="11"/>
+      <c r="AMA28" s="11"/>
+      <c r="AMB28" s="11"/>
+      <c r="AMC28" s="11"/>
+      <c r="AMD28" s="11"/>
+      <c r="AME28" s="11"/>
+      <c r="AMF28" s="11"/>
+      <c r="AMG28" s="11"/>
+      <c r="AMH28" s="11"/>
+      <c r="AMI28" s="11"/>
+      <c r="AMJ28" s="11"/>
+      <c r="AMK28" s="11"/>
+      <c r="AML28" s="11"/>
     </row>
     <row r="29" spans="1:1026" ht="30">
       <c r="A29" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>16</v>
@@ -9091,24 +9126,24 @@
         <v>0</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:1026">
+    <row r="30" spans="1:1026" ht="30">
       <c r="A30" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>16</v>
@@ -9123,16 +9158,19 @@
     </row>
     <row r="31" spans="1:1026">
       <c r="A31" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>16</v>
@@ -9142,24 +9180,21 @@
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:1026" ht="75">
+    <row r="32" spans="1:1026">
       <c r="A32" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>16</v>
@@ -9169,27 +9204,24 @@
         <v>0</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>361</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30">
+    <row r="33" spans="1:13" ht="75">
       <c r="A33" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>16</v>
@@ -9198,125 +9230,134 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="K33" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="30">
       <c r="A34" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>348</v>
+        <v>150</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G34" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="30">
+      <c r="A35" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K35" s="1">
         <v>990399123</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:13">
+      <c r="A36" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G36" s="2">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="30">
-      <c r="A36" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E36"/>
-      <c r="F36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30">
       <c r="A37" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>165</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="E37"/>
       <c r="F37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="2">
-        <f>0</f>
-        <v>0</v>
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30">
       <c r="A38" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>168</v>
+        <v>38</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>16</v>
@@ -9325,24 +9366,20 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="39" spans="1:13" ht="30">
       <c r="A39" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>168</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E39"/>
+        <v>169</v>
+      </c>
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
@@ -9350,43 +9387,44 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="K39" s="1" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="40" spans="1:13" ht="30">
       <c r="A40" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>168</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>177</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="E40"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G40" s="2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>179</v>
+        <f>0</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" ht="30">
       <c r="A41" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>117</v>
+        <v>168</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>119</v>
+        <v>177</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>16</v>
@@ -9396,77 +9434,74 @@
         <v>1</v>
       </c>
       <c r="H41" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="45">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:13" ht="45">
+      <c r="A43" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="G42" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E43"/>
-      <c r="F43" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="G43" s="2">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>190</v>
-      </c>
     </row>
-    <row r="44" spans="1:13" ht="30">
+    <row r="44" spans="1:13">
       <c r="A44" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>178</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="E44"/>
       <c r="F44" s="1" t="s">
         <v>179</v>
       </c>
@@ -9474,68 +9509,73 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="I44" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="45" spans="1:13" ht="30">
       <c r="A45" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G45" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="30">
+      <c r="A46" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G45" s="2" t="b">
+      <c r="G46" s="2" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>430</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E46"/>
-      <c r="F46" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G46" s="2">
-        <f>0</f>
-        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E47"/>
       <c r="F47" s="1" t="s">
@@ -9548,16 +9588,16 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E48"/>
       <c r="F48" s="1" t="s">
@@ -9570,16 +9610,16 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E49"/>
       <c r="F49" s="1" t="s">
@@ -9592,16 +9632,16 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>213</v>
+        <v>106</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E50"/>
       <c r="F50" s="1" t="s">
@@ -9614,16 +9654,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E51"/>
       <c r="F51" s="1" t="s">
@@ -9636,17 +9676,18 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="E52"/>
       <c r="F52" s="1" t="s">
         <v>153</v>
       </c>
@@ -9657,18 +9698,17 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="8" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E53"/>
+        <v>222</v>
+      </c>
       <c r="F53" s="1" t="s">
         <v>153</v>
       </c>
@@ -9679,16 +9719,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="8" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E54"/>
       <c r="F54" s="1" t="s">
@@ -9701,16 +9741,16 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="8" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>95</v>
+        <v>229</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E55"/>
       <c r="F55" s="1" t="s">
@@ -9722,17 +9762,17 @@
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="9" t="s">
-        <v>234</v>
+      <c r="A56" s="8" t="s">
+        <v>231</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>236</v>
+        <v>95</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E56"/>
       <c r="F56" s="1" t="s">
@@ -9745,16 +9785,16 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="9" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E57"/>
       <c r="F57" s="1" t="s">
@@ -9767,16 +9807,16 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E58"/>
       <c r="F58" s="1" t="s">
@@ -9789,16 +9829,16 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E59"/>
       <c r="F59" s="1" t="s">
@@ -9811,16 +9851,16 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="9" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E60"/>
       <c r="F60" s="1" t="s">
@@ -9833,16 +9873,16 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="9" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>122</v>
+        <v>252</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E61"/>
       <c r="F61" s="1" t="s">
@@ -9855,16 +9895,16 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>259</v>
+        <v>122</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E62"/>
       <c r="F62" s="1" t="s">
@@ -9877,16 +9917,16 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E63"/>
       <c r="F63" s="1" t="s">
@@ -9899,16 +9939,16 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E64"/>
       <c r="F64" s="1" t="s">
@@ -9921,16 +9961,16 @@
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E65"/>
       <c r="F65" s="1" t="s">
@@ -9941,18 +9981,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="30">
+    <row r="66" spans="1:13">
       <c r="A66" s="9" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E66"/>
       <c r="F66" s="1" t="s">
@@ -9963,18 +10003,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" ht="30">
       <c r="A67" s="9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E67"/>
       <c r="F67" s="1" t="s">
@@ -9987,16 +10027,16 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="9" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>58</v>
+        <v>279</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="1" t="s">
@@ -10009,16 +10049,16 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>286</v>
+        <v>58</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E69"/>
       <c r="F69" s="1" t="s">
@@ -10031,16 +10071,16 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E70"/>
       <c r="F70" s="1" t="s">
@@ -10053,16 +10093,16 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="9" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E71"/>
       <c r="F71" s="1" t="s">
@@ -10075,16 +10115,16 @@
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E72"/>
       <c r="F72" s="1" t="s">
@@ -10097,16 +10137,16 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E73"/>
       <c r="F73" s="1" t="s">
@@ -10119,16 +10159,16 @@
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="9" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E74"/>
       <c r="F74" s="1" t="s">
@@ -10141,17 +10181,18 @@
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="9" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>311</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="E75"/>
       <c r="F75" s="1" t="s">
         <v>153</v>
       </c>
@@ -10162,18 +10203,17 @@
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="9" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E76"/>
+        <v>311</v>
+      </c>
       <c r="F76" s="1" t="s">
         <v>153</v>
       </c>
@@ -10182,18 +10222,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="30">
+    <row r="77" spans="1:13">
       <c r="A77" s="9" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E77"/>
       <c r="F77" s="1" t="s">
@@ -10204,93 +10244,91 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
-      <c r="A78" s="1" t="s">
-        <v>320</v>
+    <row r="78" spans="1:13" ht="30">
+      <c r="A78" s="9" t="s">
+        <v>316</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>58</v>
+        <v>318</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>322</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="E78"/>
       <c r="F78" s="1" t="s">
-        <v>323</v>
+        <v>153</v>
       </c>
       <c r="G78" s="2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M78" s="1" t="s">
-        <v>324</v>
+        <f>0</f>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G79" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="A80" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="G79" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="30">
-      <c r="A80" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="G80" s="2">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I80" s="3" t="s">
-        <v>333</v>
-      </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" ht="30">
       <c r="A81" s="1" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>87</v>
@@ -10299,33 +10337,60 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="I81" s="3" t="s">
+        <v>333</v>
+      </c>
     </row>
-    <row r="82" spans="1:13" ht="30">
+    <row r="82" spans="1:13">
       <c r="A82" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>229</v>
+        <v>13</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G82" s="2">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="M82" s="1" t="s">
+    </row>
+    <row r="83" spans="1:13" ht="30">
+      <c r="A83" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G83" s="2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="M83" s="1" t="s">
         <v>340</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M82">
+  <autoFilter ref="A1:M83">
     <filterColumn colId="11"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Using consistent deprecated column value
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
@@ -1637,7 +1637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1668,9 +1668,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1976,28 +1973,28 @@
   <dimension ref="A1:AML83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.73046875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="67.85546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="34.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="54.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" style="1" customWidth="1"/>
-    <col min="14" max="1026" width="14.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.1328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.3984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.3984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="67.86328125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="34.1328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="23.73046875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="54.265625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="29.1328125" style="1" customWidth="1"/>
+    <col min="14" max="1026" width="14.1328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1026" s="4" customFormat="1">
@@ -2041,7 +2038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1026" ht="105">
+    <row r="2" spans="1:1026" ht="85.5">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -2060,8 +2057,8 @@
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2">
-        <f>0</f>
+      <c r="G2" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -2080,7 +2077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1026" ht="45">
+    <row r="3" spans="1:1026" ht="42.75">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -2099,8 +2096,8 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2">
-        <f>0</f>
+      <c r="G3" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -2116,7 +2113,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:1026" ht="30">
+    <row r="4" spans="1:1026" ht="28.5">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -2135,8 +2132,8 @@
       <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="2">
-        <f>0</f>
+      <c r="G4" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -2152,7 +2149,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:1026" ht="135">
+    <row r="5" spans="1:1026" ht="99.75">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -2171,8 +2168,8 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="2">
-        <f>0</f>
+      <c r="G5" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I5" s="7" t="s">
@@ -2191,7 +2188,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:1026" ht="90">
+    <row r="6" spans="1:1026" ht="71.25">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -2210,8 +2207,8 @@
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="2">
-        <f>0</f>
+      <c r="G6" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -2230,7 +2227,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="7" spans="1:1026" ht="30">
+    <row r="7" spans="1:1026" ht="28.5">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -2249,8 +2246,8 @@
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="2">
-        <f>0</f>
+      <c r="G7" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -2269,7 +2266,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="8" spans="1:1026" ht="180">
+    <row r="8" spans="1:1026" ht="142.5">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2288,8 +2285,8 @@
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="2">
-        <f>0</f>
+      <c r="G8" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -2302,7 +2299,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="1:1026" ht="180">
+    <row r="9" spans="1:1026" ht="171">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -2321,8 +2318,8 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="2">
-        <f>0</f>
+      <c r="G9" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -2338,7 +2335,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:1026" ht="195">
+    <row r="10" spans="1:1026" ht="156.75">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -2357,8 +2354,8 @@
       <c r="F10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="2">
-        <f>0</f>
+      <c r="G10" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -2374,7 +2371,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="11" spans="1:1026" s="14" customFormat="1" ht="45">
+    <row r="11" spans="1:1026" s="13" customFormat="1" ht="28.5">
       <c r="A11" s="11" t="s">
         <v>62</v>
       </c>
@@ -2393,19 +2390,19 @@
       <c r="F11" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="12">
-        <f>0</f>
+      <c r="G11" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H11" s="11"/>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K11" s="11"/>
-      <c r="L11" s="13"/>
+      <c r="L11" s="12"/>
       <c r="M11" s="11" t="s">
         <v>391</v>
       </c>
@@ -3423,7 +3420,7 @@
       <c r="AMK11" s="11"/>
       <c r="AML11" s="11"/>
     </row>
-    <row r="12" spans="1:1026" s="14" customFormat="1" ht="30">
+    <row r="12" spans="1:1026" s="13" customFormat="1" ht="28.5">
       <c r="A12" s="11" t="s">
         <v>68</v>
       </c>
@@ -3442,19 +3439,19 @@
       <c r="F12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="12">
-        <f>0</f>
+      <c r="G12" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H12" s="11"/>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K12" s="11"/>
-      <c r="L12" s="13"/>
+      <c r="L12" s="12"/>
       <c r="M12" s="11" t="s">
         <v>393</v>
       </c>
@@ -4472,7 +4469,7 @@
       <c r="AMK12" s="11"/>
       <c r="AML12" s="11"/>
     </row>
-    <row r="13" spans="1:1026" s="14" customFormat="1">
+    <row r="13" spans="1:1026" s="13" customFormat="1">
       <c r="A13" s="11" t="s">
         <v>72</v>
       </c>
@@ -4491,19 +4488,19 @@
       <c r="F13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="12">
-        <f>0</f>
+      <c r="G13" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H13" s="11"/>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K13" s="11"/>
-      <c r="L13" s="13"/>
+      <c r="L13" s="12"/>
       <c r="M13" s="11" t="s">
         <v>393</v>
       </c>
@@ -5521,7 +5518,7 @@
       <c r="AMK13" s="11"/>
       <c r="AML13" s="11"/>
     </row>
-    <row r="14" spans="1:1026" ht="165">
+    <row r="14" spans="1:1026" ht="156.75">
       <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
@@ -5540,8 +5537,8 @@
       <c r="F14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="2">
-        <f>0</f>
+      <c r="G14" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -5560,7 +5557,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="15" spans="1:1026" ht="150">
+    <row r="15" spans="1:1026" ht="142.5">
       <c r="A15" s="1" t="s">
         <v>345</v>
       </c>
@@ -5596,7 +5593,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="16" spans="1:1026" s="14" customFormat="1">
+    <row r="16" spans="1:1026" s="13" customFormat="1">
       <c r="A16" s="11" t="s">
         <v>84</v>
       </c>
@@ -5615,19 +5612,19 @@
       <c r="F16" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="12">
-        <f>0</f>
+      <c r="G16" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H16" s="11"/>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="12" t="s">
         <v>400</v>
       </c>
       <c r="K16" s="11"/>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="12" t="s">
         <v>404</v>
       </c>
       <c r="M16" s="11"/>
@@ -6645,7 +6642,7 @@
       <c r="AMK16" s="11"/>
       <c r="AML16" s="11"/>
     </row>
-    <row r="17" spans="1:1026" ht="135">
+    <row r="17" spans="1:1026" ht="114">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -6664,8 +6661,8 @@
       <c r="F17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="2">
-        <f>0</f>
+      <c r="G17" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I17" s="3" t="s">
@@ -6684,7 +6681,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="18" spans="1:1026" ht="165">
+    <row r="18" spans="1:1026" ht="156.75">
       <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
@@ -6703,8 +6700,8 @@
       <c r="F18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="2">
-        <f>0</f>
+      <c r="G18" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I18" s="3" t="s">
@@ -6716,14 +6713,14 @@
       <c r="K18" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="14" t="s">
         <v>410</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="19" spans="1:1026" ht="60">
+    <row r="19" spans="1:1026" ht="57">
       <c r="A19" s="1" t="s">
         <v>98</v>
       </c>
@@ -6742,8 +6739,8 @@
       <c r="F19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="2">
-        <f>0</f>
+      <c r="G19" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I19" s="3" t="s">
@@ -6759,7 +6756,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="20" spans="1:1026" s="14" customFormat="1" ht="45">
+    <row r="20" spans="1:1026" s="13" customFormat="1" ht="42.75">
       <c r="A20" s="11" t="s">
         <v>104</v>
       </c>
@@ -6778,19 +6775,19 @@
       <c r="F20" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="12">
-        <f>0</f>
+      <c r="G20" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H20" s="11"/>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K20" s="11"/>
-      <c r="L20" s="13" t="s">
+      <c r="L20" s="12" t="s">
         <v>413</v>
       </c>
       <c r="M20" s="11"/>
@@ -7808,7 +7805,7 @@
       <c r="AMK20" s="11"/>
       <c r="AML20" s="11"/>
     </row>
-    <row r="21" spans="1:1026" ht="75">
+    <row r="21" spans="1:1026" ht="71.25">
       <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
@@ -7827,8 +7824,8 @@
       <c r="F21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="2">
-        <f>0</f>
+      <c r="G21" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I21" s="3" t="s">
@@ -7844,7 +7841,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="22" spans="1:1026" ht="90">
+    <row r="22" spans="1:1026" ht="85.5">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -7863,8 +7860,8 @@
       <c r="F22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="2">
-        <f>0</f>
+      <c r="G22" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I22" s="3" t="s">
@@ -7877,7 +7874,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="1:1026" ht="30">
+    <row r="23" spans="1:1026" ht="28.5">
       <c r="A23" s="1" t="s">
         <v>351</v>
       </c>
@@ -7943,7 +7940,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:1026" ht="75">
+    <row r="25" spans="1:1026" ht="71.25">
       <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
@@ -7979,7 +7976,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="26" spans="1:1026" ht="30">
+    <row r="26" spans="1:1026" ht="28.5">
       <c r="A26" s="1" t="s">
         <v>433</v>
       </c>
@@ -8016,7 +8013,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="27" spans="1:1026" ht="45">
+    <row r="27" spans="1:1026" ht="42.75">
       <c r="A27" s="1" t="s">
         <v>435</v>
       </c>
@@ -8053,7 +8050,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="28" spans="1:1026" s="14" customFormat="1" ht="30">
+    <row r="28" spans="1:1026" s="13" customFormat="1">
       <c r="A28" s="11" t="s">
         <v>126</v>
       </c>
@@ -8072,19 +8069,19 @@
       <c r="F28" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="12">
-        <f>0</f>
+      <c r="G28" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H28" s="11"/>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K28" s="11"/>
-      <c r="L28" s="13"/>
+      <c r="L28" s="12"/>
       <c r="M28" s="11" t="s">
         <v>426</v>
       </c>
@@ -9102,7 +9099,7 @@
       <c r="AMK28" s="11"/>
       <c r="AML28" s="11"/>
     </row>
-    <row r="29" spans="1:1026" ht="30">
+    <row r="29" spans="1:1026" ht="28.5">
       <c r="A29" s="1" t="s">
         <v>130</v>
       </c>
@@ -9121,15 +9118,15 @@
       <c r="F29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="2">
-        <f>0</f>
+      <c r="G29" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:1026" ht="30">
+    <row r="30" spans="1:1026" ht="28.5">
       <c r="A30" s="1" t="s">
         <v>134</v>
       </c>
@@ -9148,8 +9145,8 @@
       <c r="F30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="2">
-        <f>0</f>
+      <c r="G30" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K30" s="1" t="s">
@@ -9175,8 +9172,8 @@
       <c r="F31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="2">
-        <f>0</f>
+      <c r="G31" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
@@ -9199,15 +9196,15 @@
       <c r="F32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="2">
-        <f>0</f>
+      <c r="G32" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="75">
+    <row r="33" spans="1:13" ht="71.25">
       <c r="A33" s="1" t="s">
         <v>145</v>
       </c>
@@ -9226,8 +9223,8 @@
       <c r="F33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="2">
-        <f>0</f>
+      <c r="G33" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K33" s="1" t="s">
@@ -9237,7 +9234,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="30">
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
         <v>148</v>
       </c>
@@ -9256,12 +9253,12 @@
       <c r="F34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="2">
-        <f>0</f>
+      <c r="G34" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="30">
+    <row r="35" spans="1:13" ht="28.5">
       <c r="A35" s="1" t="s">
         <v>151</v>
       </c>
@@ -9280,8 +9277,8 @@
       <c r="F35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="2">
-        <f>1</f>
+      <c r="G35" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -9307,15 +9304,15 @@
       <c r="F36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="2">
-        <f>0</f>
+      <c r="G36" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="30">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>159</v>
       </c>
@@ -9332,8 +9329,8 @@
       <c r="F37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="2">
-        <f>1</f>
+      <c r="G37" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -9343,7 +9340,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="30">
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
         <v>163</v>
       </c>
@@ -9362,12 +9359,12 @@
       <c r="F38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="2">
-        <f>0</f>
+      <c r="G38" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="30">
+    <row r="39" spans="1:13" ht="28.5">
       <c r="A39" s="1" t="s">
         <v>166</v>
       </c>
@@ -9383,15 +9380,15 @@
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="2">
-        <f>0</f>
+      <c r="G39" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="30">
+    <row r="40" spans="1:13" ht="28.5">
       <c r="A40" s="1" t="s">
         <v>172</v>
       </c>
@@ -9408,12 +9405,12 @@
       <c r="F40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="2">
-        <f>0</f>
+      <c r="G40" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="30">
+    <row r="41" spans="1:13" ht="28.5">
       <c r="A41" s="1" t="s">
         <v>175</v>
       </c>
@@ -9429,8 +9426,8 @@
       <c r="F41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="2">
-        <f>1</f>
+      <c r="G41" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -9453,8 +9450,8 @@
       <c r="F42" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="2">
-        <f>1</f>
+      <c r="G42" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -9464,7 +9461,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="45">
+    <row r="43" spans="1:13" ht="42.75">
       <c r="A43" s="1" t="s">
         <v>184</v>
       </c>
@@ -9483,8 +9480,8 @@
       <c r="F43" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G43" s="2">
-        <f>0</f>
+      <c r="G43" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9505,15 +9502,15 @@
       <c r="F44" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G44" s="2">
-        <f>0</f>
+      <c r="G44" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="30">
+    <row r="45" spans="1:13" ht="28.5">
       <c r="A45" s="1" t="s">
         <v>191</v>
       </c>
@@ -9532,12 +9529,12 @@
       <c r="F45" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G45" s="2">
-        <f>0</f>
+      <c r="G45" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="30">
+    <row r="46" spans="1:13">
       <c r="A46" s="1" t="s">
         <v>194</v>
       </c>
@@ -9581,8 +9578,8 @@
       <c r="F47" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G47" s="2">
-        <f>0</f>
+      <c r="G47" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9603,8 +9600,8 @@
       <c r="F48" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G48" s="2">
-        <f>0</f>
+      <c r="G48" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9625,8 +9622,8 @@
       <c r="F49" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G49" s="2">
-        <f>0</f>
+      <c r="G49" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9647,8 +9644,8 @@
       <c r="F50" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G50" s="2">
-        <f>0</f>
+      <c r="G50" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9669,8 +9666,8 @@
       <c r="F51" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G51" s="2">
-        <f>0</f>
+      <c r="G51" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9691,8 +9688,8 @@
       <c r="F52" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G52" s="2">
-        <f>0</f>
+      <c r="G52" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9712,8 +9709,8 @@
       <c r="F53" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G53" s="2">
-        <f>0</f>
+      <c r="G53" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9734,8 +9731,8 @@
       <c r="F54" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G54" s="2">
-        <f>0</f>
+      <c r="G54" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9756,8 +9753,8 @@
       <c r="F55" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G55" s="2">
-        <f>0</f>
+      <c r="G55" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9778,8 +9775,8 @@
       <c r="F56" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G56" s="2">
-        <f>0</f>
+      <c r="G56" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9800,8 +9797,8 @@
       <c r="F57" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G57" s="2">
-        <f>0</f>
+      <c r="G57" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9822,8 +9819,8 @@
       <c r="F58" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G58" s="2">
-        <f>0</f>
+      <c r="G58" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9844,8 +9841,8 @@
       <c r="F59" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G59" s="2">
-        <f>0</f>
+      <c r="G59" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9866,8 +9863,8 @@
       <c r="F60" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G60" s="2">
-        <f>0</f>
+      <c r="G60" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9888,8 +9885,8 @@
       <c r="F61" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G61" s="2">
-        <f>0</f>
+      <c r="G61" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9910,8 +9907,8 @@
       <c r="F62" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G62" s="2">
-        <f>0</f>
+      <c r="G62" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9932,8 +9929,8 @@
       <c r="F63" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G63" s="2">
-        <f>0</f>
+      <c r="G63" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9954,8 +9951,8 @@
       <c r="F64" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G64" s="2">
-        <f>0</f>
+      <c r="G64" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9976,8 +9973,8 @@
       <c r="F65" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G65" s="2">
-        <f>0</f>
+      <c r="G65" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -9998,12 +9995,12 @@
       <c r="F66" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G66" s="2">
-        <f>0</f>
+      <c r="G66" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="30">
+    <row r="67" spans="1:13" ht="28.5">
       <c r="A67" s="9" t="s">
         <v>273</v>
       </c>
@@ -10020,8 +10017,8 @@
       <c r="F67" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G67" s="2">
-        <f>0</f>
+      <c r="G67" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10042,8 +10039,8 @@
       <c r="F68" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G68" s="2">
-        <f>0</f>
+      <c r="G68" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10064,8 +10061,8 @@
       <c r="F69" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G69" s="2">
-        <f>0</f>
+      <c r="G69" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10086,8 +10083,8 @@
       <c r="F70" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G70" s="2">
-        <f>0</f>
+      <c r="G70" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10108,8 +10105,8 @@
       <c r="F71" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G71" s="2">
-        <f>0</f>
+      <c r="G71" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10130,8 +10127,8 @@
       <c r="F72" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G72" s="2">
-        <f>0</f>
+      <c r="G72" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10152,8 +10149,8 @@
       <c r="F73" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G73" s="2">
-        <f>0</f>
+      <c r="G73" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10174,8 +10171,8 @@
       <c r="F74" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G74" s="2">
-        <f>0</f>
+      <c r="G74" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10196,8 +10193,8 @@
       <c r="F75" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G75" s="2">
-        <f>0</f>
+      <c r="G75" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10217,8 +10214,8 @@
       <c r="F76" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G76" s="2">
-        <f>0</f>
+      <c r="G76" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10239,12 +10236,12 @@
       <c r="F77" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G77" s="2">
-        <f>0</f>
+      <c r="G77" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="30">
+    <row r="78" spans="1:13">
       <c r="A78" s="9" t="s">
         <v>316</v>
       </c>
@@ -10261,8 +10258,8 @@
       <c r="F78" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G78" s="2">
-        <f>0</f>
+      <c r="G78" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
@@ -10282,8 +10279,8 @@
       <c r="F79" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="G79" s="2">
-        <f>1</f>
+      <c r="G79" s="2" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H79" s="1" t="s">
@@ -10309,12 +10306,12 @@
       <c r="F80" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="G80" s="2">
-        <f>0</f>
+      <c r="G80" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="30">
+    <row r="81" spans="1:13">
       <c r="A81" s="1" t="s">
         <v>329</v>
       </c>
@@ -10333,8 +10330,8 @@
       <c r="F81" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G81" s="2">
-        <f>0</f>
+      <c r="G81" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I81" s="3" t="s">
@@ -10357,12 +10354,12 @@
       <c r="F82" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G82" s="2">
-        <f>0</f>
+      <c r="G82" s="2" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="30">
+    <row r="83" spans="1:13" ht="28.5">
       <c r="A83" s="1" t="s">
         <v>337</v>
       </c>
@@ -10395,6 +10392,10 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <ignoredErrors>
+    <ignoredError sqref="G79" formula="1"/>
+    <ignoredError sqref="F79" twoDigitTextYear="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deprecated country specific VAT codes - TICC-104
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v6 draft.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="465">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1601,9 +1601,6 @@
     <t>RegEx: [A-Z]{2}[A-Z0-9]{,20}</t>
   </si>
   <si>
-    <t>Proposed to undeprecate; longest known is 18 chars (incl. country code)</t>
-  </si>
-  <si>
     <t>Proposed to deprecate</t>
   </si>
   <si>
@@ -1637,6 +1634,10 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>Proposed to undeprecate; longest known is 18 chars (incl. country code)
+Deprecated in 1.1.0; undeprecated in v6</t>
   </si>
 </sst>
 </file>
@@ -2070,10 +2071,10 @@
   <dimension ref="A1:AML83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -2431,7 +2432,7 @@
         <v>384</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
@@ -11335,8 +11336,11 @@
         <v>16</v>
       </c>
       <c r="G32" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>427</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>143</v>
@@ -12479,36 +12483,37 @@
         <v>16</v>
       </c>
       <c r="G36" s="2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1026" s="13" customFormat="1" ht="72.5">
+      <c r="A37" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="16" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="L36" s="3" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1026" s="13" customFormat="1" ht="43.5">
-      <c r="A37" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="16" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>152</v>
-      </c>
+      <c r="H37" s="11"/>
       <c r="I37" s="12" t="s">
         <v>161</v>
       </c>
@@ -12518,7 +12523,7 @@
         <v>453</v>
       </c>
       <c r="M37" s="11" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="N37" s="11"/>
       <c r="O37" s="11"/>
@@ -13563,7 +13568,7 @@
       <c r="K38" s="11"/>
       <c r="L38" s="12"/>
       <c r="M38" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="N38" s="11"/>
       <c r="O38" s="11"/>
@@ -14596,8 +14601,11 @@
         <v>16</v>
       </c>
       <c r="G39" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>427</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>170</v>
@@ -14625,13 +14633,13 @@
         <v>0</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="L40" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="M40" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="41" spans="1:1026" s="13" customFormat="1" ht="29">
@@ -16752,7 +16760,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="44" spans="1:1026" s="13" customFormat="1">
@@ -16783,7 +16791,7 @@
       <c r="K44" s="11"/>
       <c r="L44" s="12"/>
       <c r="M44" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="N44" s="11"/>
       <c r="O44" s="11"/>
@@ -17819,8 +17827,11 @@
         <v>178</v>
       </c>
       <c r="G45" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="46" spans="1:1026" s="13" customFormat="1" ht="29">
@@ -18888,8 +18899,11 @@
         <v>152</v>
       </c>
       <c r="G47" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="48" spans="1:1026">
@@ -18910,11 +18924,14 @@
         <v>152</v>
       </c>
       <c r="G48" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" s="8" t="s">
         <v>203</v>
       </c>
@@ -18932,11 +18949,14 @@
         <v>152</v>
       </c>
       <c r="G49" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" s="8" t="s">
         <v>207</v>
       </c>
@@ -18954,11 +18974,14 @@
         <v>152</v>
       </c>
       <c r="G50" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" s="8" t="s">
         <v>210</v>
       </c>
@@ -18976,11 +18999,14 @@
         <v>152</v>
       </c>
       <c r="G51" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52" s="8" t="s">
         <v>214</v>
       </c>
@@ -18998,11 +19024,14 @@
         <v>152</v>
       </c>
       <c r="G52" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53" s="8" t="s">
         <v>218</v>
       </c>
@@ -19019,11 +19048,14 @@
         <v>152</v>
       </c>
       <c r="G53" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54" s="8" t="s">
         <v>222</v>
       </c>
@@ -19041,11 +19073,14 @@
         <v>152</v>
       </c>
       <c r="G54" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" s="8" t="s">
         <v>226</v>
       </c>
@@ -19063,11 +19098,14 @@
         <v>152</v>
       </c>
       <c r="G55" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56" s="8" t="s">
         <v>230</v>
       </c>
@@ -19085,11 +19123,14 @@
         <v>152</v>
       </c>
       <c r="G56" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:8">
       <c r="A57" s="9" t="s">
         <v>233</v>
       </c>
@@ -19107,11 +19148,14 @@
         <v>152</v>
       </c>
       <c r="G57" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:8">
       <c r="A58" s="9" t="s">
         <v>237</v>
       </c>
@@ -19129,11 +19173,14 @@
         <v>152</v>
       </c>
       <c r="G58" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:8">
       <c r="A59" s="9" t="s">
         <v>241</v>
       </c>
@@ -19151,11 +19198,14 @@
         <v>152</v>
       </c>
       <c r="G59" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8">
       <c r="A60" s="9" t="s">
         <v>245</v>
       </c>
@@ -19173,11 +19223,14 @@
         <v>152</v>
       </c>
       <c r="G60" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61" s="9" t="s">
         <v>249</v>
       </c>
@@ -19195,11 +19248,14 @@
         <v>152</v>
       </c>
       <c r="G61" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8">
       <c r="A62" s="9" t="s">
         <v>253</v>
       </c>
@@ -19217,11 +19273,14 @@
         <v>152</v>
       </c>
       <c r="G62" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8">
       <c r="A63" s="9" t="s">
         <v>256</v>
       </c>
@@ -19239,11 +19298,14 @@
         <v>152</v>
       </c>
       <c r="G63" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:8">
       <c r="A64" s="9" t="s">
         <v>260</v>
       </c>
@@ -19261,8 +19323,11 @@
         <v>152</v>
       </c>
       <c r="G64" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="65" spans="1:1026">
@@ -19283,8 +19348,11 @@
         <v>152</v>
       </c>
       <c r="G65" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="66" spans="1:1026">
@@ -19305,8 +19373,11 @@
         <v>152</v>
       </c>
       <c r="G66" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="67" spans="1:1026" ht="29">
@@ -19327,8 +19398,11 @@
         <v>152</v>
       </c>
       <c r="G67" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="68" spans="1:1026">
@@ -19349,8 +19423,11 @@
         <v>152</v>
       </c>
       <c r="G68" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="69" spans="1:1026">
@@ -19371,8 +19448,11 @@
         <v>152</v>
       </c>
       <c r="G69" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="70" spans="1:1026">
@@ -19393,8 +19473,11 @@
         <v>152</v>
       </c>
       <c r="G70" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="71" spans="1:1026">
@@ -19415,8 +19498,11 @@
         <v>152</v>
       </c>
       <c r="G71" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="72" spans="1:1026">
@@ -19437,8 +19523,11 @@
         <v>152</v>
       </c>
       <c r="G72" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="73" spans="1:1026">
@@ -19459,8 +19548,11 @@
         <v>152</v>
       </c>
       <c r="G73" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="74" spans="1:1026">
@@ -19481,8 +19573,11 @@
         <v>152</v>
       </c>
       <c r="G74" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="75" spans="1:1026">
@@ -19503,8 +19598,11 @@
         <v>152</v>
       </c>
       <c r="G75" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="76" spans="1:1026">
@@ -19524,8 +19622,11 @@
         <v>152</v>
       </c>
       <c r="G76" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="77" spans="1:1026">
@@ -19546,8 +19647,11 @@
         <v>152</v>
       </c>
       <c r="G77" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="78" spans="1:1026">
@@ -19568,8 +19672,11 @@
         <v>152</v>
       </c>
       <c r="G78" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="79" spans="1:1026" s="13" customFormat="1">
@@ -20634,8 +20741,11 @@
         <v>327</v>
       </c>
       <c r="G80" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="81" spans="1:1026" ht="58">
@@ -20665,10 +20775,10 @@
         <v>332</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="82" spans="1:1026">
@@ -20688,8 +20798,11 @@
         <v>87</v>
       </c>
       <c r="G82" s="2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="83" spans="1:1026" s="13" customFormat="1">
@@ -20721,7 +20834,7 @@
       <c r="K83" s="11"/>
       <c r="L83" s="12"/>
       <c r="M83" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="N83" s="11"/>
       <c r="O83" s="11"/>

</xml_diff>